<commit_message>
clean songs for celestin's artist)
</commit_message>
<xml_diff>
--- a/data/02_intermediate/cleaned_Mister_You_songs.xlsx
+++ b/data/02_intermediate/cleaned_Mister_You_songs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C268"/>
+  <dimension ref="A1:C269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>11.43</t>
+          <t>La Rue Puis La Prison</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>J'suis dans mon quartier, j'galère, j'regarde en l'air J'suis en train d'cogiter, j'suis défoncé sa mère J'arrive chargé, comme une porteuse à Tanger Après mon passage, ou t'es refait ou bien il te reste plus grand chose à manger J'roule un sdeh pour me percher, rejoindre l'étoile du Berger C'est plus des couilles que j'ai, eh non, c'est des gros ufs de Fabergé J'suis overbooké, ok zoogataga J'ai appris une chose chez Ruquier, c'est le mot rutabaga J'rêve que d'pouvoir, et comme vous avez pu le voir Bah le rap français c'est pas vraiment l'truc tah Audrey Pulvar Mon point commun avec Natacha c'est mes chicos d'devant Que moi-même sans mes 32 dents, j'leur faisais du rentre-dedans Ouais, bien sûr que l'avenir est inquiétant Pour des barrettes, ils nous mettent 8 ans, wesh, monsieur le président Dites leur bien que j'représente les 3arbis et les niggas Moi, j'suis plus riche qu'eux, donc pourquoi j'irai fouiller leurs caisses Eux, ils sont en pleine crise, moi j'suis en plein dans les 30 glorieuses Mais j'sais que ma liberté bah, vaut pas grand chose à leur yeuz Demande à Lacrim quand j'étais à l'école, c'était pour gratter les remises de peine Du dispatching au disque d'platine, de la fiche de recherche à la fiche de paye J'ai pété tous les barrages, mais j'n'ai jamais été odieux Comment idolâtrer la vache, quand l'univers est à Dieu Dites leur bien que, m'en bats les couilles de leur baratin Que là j'suis en promenade, 3ème tour, khapta dans un bar à tinp' Nique l'État, ces chmatas, ils rêvent que de nous mettre dans la de-mer J'vais m'branler et même cracher sur leur putain de système de merde Woogata ekh tfou, rap tah les fous Qui préfèrent s'acheter une Rafleuse que d'faire du kung-fu La Mecque, j'suis d'ceux qui se baissent et qui toussent, mec, Allah yaafo J't'ai déjà dis, nous on cotise tous pour la retraite à Clairvaux Ils nous mettent des peines de pédophile pour des histoires de barrettes Autant vendre de la cocaïne, butez-nous pour qu'on s'arrête Les 3ineurs montrent pas l'il, dites-leur de niquer leur mère les chouettes Moi, m'occupe de la vodka, woogataga gardez la Schweppes Hey, d'après mon entourage, moi, j'reste un brave J'reste un vrai, c'est pour ça qu'il m'encourage Après la pluie, y a pas le beau temps, y a l'orage C'est vrai que les petits sont hardcore, on était pareil à leur âge À deux sur un scooter on vivait que de vol à l'arrach' Puis on a connu la crave-bi et on a vite tourné la page On s'est mis à couper des barrettes, ensuite à vendre des plaquettes Puis d'la coke et des galettes, jusqu'à ce que les keufs nous arrêtent Un jour j'étais dans le 19, l'lendemain un hessess fermait ma porte Un soir j'étais avec une meuf, l'lendemain elle était avec mon pote La vie c'est dur, pas de peine nous tout ce qu'on porte c'est des flingues Et y a pas de vice de procédure gros c'est la loi de la jungle C'est pas d'ma faute, darwa, j'crois bien que j'suis taré d'naissance J'me reconnais pas moi-même des fois j'suis ravi de faire ma connaissance Et quand je pars au shtar, bah t'inquiète pas que j'reçois des mandats Et j'ai toujours la frappe, tah Hollanda et tah Belhanda J'suis khapta, zoogataga sous ma véranda J'glisse mes doigts dans les cheveux tah Esméralda J'emmerde l'État, j'emmerde les stups, j'emmerde les gendarmes Trafiquant de rimes, trafiquant d'stups ou trafiquant d'armes Je suis, comment vous dites ? Paranoïaque ! Ouais J'm'en bat les yeuks, madame la juge, baraneyek ! Ytiyyeh sa3dek ! J'te l'avais dit que j'avais des projets Là, j'graille des brochettes, j'insulte ta mère et j'touche des gros chèques M'achète des trucs qui valent cher, rien qu'avant hier J'me suis acheté 3-4 t-shirt, j'ai dépensé ton salaire J'me suis roulé un gros sdeh, puis j'ai repensé à la misère À cet été, à cet hiver, Alicante ou au Val-d'Isère Au mitard tah la Santé, les promenades en camembert Au mitard tah Fleury, j'revois les toilettes, j'me dis beurk ! Ah les bâtards, comment ils ont pu me faire ça ? Ils me l'ont mise, j'leur ai remise woogata vice et versa Ya zzeh, obligé de se faire remarquer Obligé de se faire embarquer, déféré au parquet Direction les grillages, bon, trêve d'enfantillage Yeah, I speak a little English, motherfucking biatch ! Weld lqahba, what you gonna do? Ok, j'continue tout doux, j're-big up le rott' Mamadou Yoogata yoogata gangz to gangz Ouais, tu connais la musique, celui qui veut me test, j'le baise You might also like Ban-ban-bandit j'fait que du propre, j'effectue les sales tâches Ça sert à quoi de jouer le pirate, si pas à l'abordage Ils dopent en dopant, co on t'laisse le dos en deux On est nous-mêmes en paix exorcistes avec un joint d'beuh Tous les soirs j'dégrise, nos combines se développent Mais des fois les quis' débarquent et dans les comptes ça fait des flops Du crime ouais y'a la crème, Sta-ive c'est du vécu Mon gros, chez moi le sang s'est vidé à cause du manque d'écus Pas de ces collabos, que t'achètes avec alcool et abus De plus, j'baise ces nabots qui croient contrôler la rue Les yeux cernés au poste, menotté à des barreaux de chaise J'rêve d'Îles Vierges m'en fumer avec des barreaux de chaises La nuit j'dors mal, éternellement tourmenté En pensant que j'vais prendre cher si les keufs arrivent à tout remonter Ceux qui sèment le vent, récolte du ons dans le ventre A-L, futur ex-braqueur reconverti dans la vente J'aimerais partir tranquille, les pieds d'vant Un monde de fils de pute, j'suis obligé de vendre Ah bon ? Ça suffit pas alors on braque sa mère M'en voulais pas dans le rap y'a trop de zamels 3 quart, belle coupe, chico cassé La vie c'est speed même mon ombre veut me dépasser Oh, le sky est classé, j'suis chaud Menacer ne sert à rien, j't'envoie 2-3 balles l'affaire est classé Ramassé du biff, voilà dans quoi j'me suis perdu J'sais c'que c'est d'avoir la dalle, j'en connais ces vertus Hyper dur, fréquentation malsaine Chiale pas sur mon sort, tu sais qu'ici personne nous accepte On connait le respect, les valeurs et les principes T'es le plus grand des hommes si tu te lèves pour bosser à Rungis Malheureusement pas mon cas, au fond de moi je les envie Nos vies, c'est faire du biff, mais resté en vie Donc faut marcher armé, puis avoir la trique Aujourd'hui t'allumes demain t'es complètement matrixé C'est la vie du western, la vie d'moi j'suis réel La tranquillité frérot est bloquée dans mes rêves Impossible de l'avoir, je ne prends jamais de Mais Belek au feu le couz si tu mets trop de bois Beaucoup de salopes font les voyous, wallah que c'est pas une fierté Dis-moi qui sera là le jour ou t'auras vraiment merdé J'ai l'orgueil d'un bébé, je m'énerve et je pète tout J'assume les conséquences khey dans mes bras je prend le mektoub Oui j'aime pas les poulets et je f'rais recette sans eux Une impression même jaloux de ma paire à 700E Ils m'inventent des vies, le mythe ils veulent casser Hum j'en ai assez, les traquer, les chlasser Quand j'allais tu revenais, dans ta tête ça ne rentre pas Je le ferai tout les jours, je compte l'oseille me dérange pas Bien sur qu'on s'est fait tout seul, je sais très bien que tu sais J'ai braqué des bijouteries quand les autres allaient sucer Sans t'manquer de respect, dans l'rap dis-moi ce qui est facile Frérot on viens de la rue c'est des filles faciles J'ai roulé ma bosse, j'en ai marre d'bouffer d'la merde Coup d'crosse, la vie t'assomme pire qu'un joint d'herbe Tout c'qu'on a, on finit par l'perdre Étoile de mer, dix mille kilomètres, perdu sur la lune verte J'suis tellement loin des je veux être Berrad d'atay, j'allume un jaabouq à la fenêtre T'es dans l'paraître, moi j'veux disparaître Les kheys passent au dispatching, une mère qui pleure c'est la faute d'un traître Y'a plus qu'des bras cassés dis-moi à qui serrer les coudes ? Six pieds sous terre, quand j'me ferai bouffer par l'doud Noyé dans l'doute, j'suis toujours dans l'hood Les yeux rouges, Wydad Casanegra j'suis pas un Blood Passe-moi des feuilles, c'soir j'fume mes dernières illusions Sers-moi un verre que j'tourne cette tragédie en dérision 11.43, mortuaire sera la saison Maintenant j'marche avec des rétros, dis-moi qui va m'sauter l'caisson Y'a, y'a, y'a plus d'rage que d'la fashionnerie J'enterre l'espoir dans un parloir à Fleury Ghetto youth langage, du whisky, les chicots pourries Bonbon sauvage, 0.4 khoya souris Heh-hep-pep, Dieu seul est maitre de ma destinée Moi j'me verrais bien à La Mecque avec mes rents-pa et ma dulcinée La vie c'est pas un clip ni du ciné ou une bande dessinée On va peut-être finir à Clairvaux, on va peut-être s'faire assassiner C'est clair gros qu'on peut tout perdre sur un coup d'ker-po J'te parle d'une boite où pour rentrer y'a même pas besoin d'se faire beau Le cercle est vicieux bienvenue dans le cerceau Quand j'ai fêté mes 16 ans c'est pas du plomb que j'avais dans le cerveau J'ai 28 ans, j'habite dans l'zoo, je m'appelle Hédi Chabar J'veux réussir, j'veux m'en sortir depuis que j'suis tout petit je chabarde J'ai bicrave, j'ai fais plein d'conneries dont j'suis pas du tout fier Comme les aller-retours à Fleury pour battre le fer faut du fer Pour faire du flouze faut du flouze, des couilles et d'la gamberge Surtout quand t'es seul contre tous y'a personne pour te tendre la perche Moi, hamdullah, j'suis pas comme ça, j'préfère aider mon prochain Car j'sais que Dieu me l'rendra ici bas ou dans un monde prochain Howa yaalem b kolchi, hata tkoun labes Gucci Lmout tjik w teddik, tedderbek kima lfuchi J'arrive dans l'game avec You pour écraser tous ces chiens Même s'ils sont plein, on les baise tous kalachnikov à la main Ça va péter dans l'quartier, dans tous les ghettos d'France Ayet lkursi, 11.43 pour me souhaiter bonne chance M'en bats les couilles de c'que tu penses, depuis ma tendre enfance J'laisse la concurrence en transe, lourde sera la sentence Brulux on the flux toujours dans les bacs Hier, ils m'boycottaient, maintenant, ils veulent faire mes backs Prochain clip, j'appelle Fredo, il m'prépare le Maybach Cette fois-ci, j'ferai pas l'gamin, promis, j'cacherai tes plaques Ils m'ont pris pour une blague, des mesures, il m'en reste quatre Pour ma mère, j'veux du 2.4, pour moi qamis, un RS4 Dédicace l'Algérie, le Maroc, la Tunisie Faudra bientôt retourner chez nous car y a trop d'crapules ici Parce que tu manges du lion l'matin devant moi tu veux rugir Approche j'te mets une claque de roumain, tu vas rougir Plus tu vas monter, plus les rumeurs vont surgir Personne n'est au-dessus d'personne, écoute bien tout c'que j'vais te dire Tout ce qui est autour de moi, j'vais te l'exposer La j'pète les plombs j'ai retiré la goupille, j'vais exploser À ma droite, les frères muz débarquent pour nous faire des rappels Par la gauche, y en a qui vesqui s'hab quelqu'un les appelle En primaire j'te frappais ouai j'me prenais pour l'king À 10 ans au comico voiture péta dans un parking Le quartier c'est une plaque tournante, ça défouraille de partout Dans mon escalier j'tombe sur un sac remplis d'billets j'garde tout Assis sur un banc toute la journée ça bibi Dans les bois ça fait bep-bep ou cric-cric bim bim ! Au collège, lycée v'là les bagarres, boy, j'casse des dents Avec Oxmo ou pas leurs uppercuts te rentre dedans On sait que la police nous surveille mais elle ne sait pas tout Les malins savent très bien que l'argent ne fait pas tout On a des avocats mais ils n'arrangent pas tout Les médecins sont la mais il ne soignent pas tout Pas de chance cette nuit la juge s'est fait mal baiser Donc forcément des chance d'être acquitté on baissées T'es pressé, t'accélères risquer sont les raccourcis Kazou dis leur que cette est pute mais plus de soucis que d'sursis Posé à la tess j'ai rien vu, rien entendu J'ves-qui les histoires tendu, des fois c'est tes potes qui t'enculent Avec du recul, tu finis par devenir solitaire Pour l'Etat on a pas les critères, donc on a fini sur le ter J'vois des pères, des mères qui travaillent dur pour ceux qu'ils aiment Wallah ça m'fait de la peine d'les rentrer pour rien dans nos problèmes 11.43 c'est le thème, là c'est Tirgo sur l'antenne Poto dès l'début de l'enquête c'est possible que tu perds la tête Envoie la frappe de Ketama dédicace à Khadama J'suis obligé d'faire du sale y'a toute la cité derrière moi Y'en a qui braquait des tabacs nous on bicravait du taga Ouais continuer à taguer nous on à pas l'temps on tabasse On va t'laisser aux aguets dé-ter comme l'armée du Hamas J'savais pas que sur ce banc ouais j'allais fumer des kamas Toute l'année tu fais des phases poto, c'est pas comme a-ç Dans l'arène j'ai toujours la faille, flow qui tire comme un Fa-mas Nous on est comme des hommes, on va toujours à la chasse Y'a du biff' et des liasses obligé on s'déplace Ça bicrave au fond de l'impasse, désolé si ça dépasse Dans ton bigo y'a les vrais et les boloss que t'effaces We-wesh la racaille, les raclures la police en a ras-le-cul Ma vie c'est un texte de rap remplit d'ratures Nerveux l'sourire aux lèvres doté d'pouvoir céleste J'ai perdu l'nord ma direction à moi c'est l'est J'écris des textes de fou, beaucoup métaphorique L'histoire d'un braqueur qui finit par taffer au Ritz Rosny-sous-Bois, la Sambuy, les braquos, les sous-salles Les sous-sols, les mouses, ceux qui moussent et qui s'débat ainsi qu'les douzes J'rappe, je pense comme un mec de la ur J'aime la pure qui branche les clients sur mon terrain tout les jours J'ai pas d'bonnes habitudes j'descends et j'traine J'truande j'ves-qui la justice dédicace à Fresnes Les sirènes retentissent, les criminels se repentissent La pisse du sheïtan, mes repentises, ma hantise C'est vraiment pas la mort mais c'qui s'en suit J'aime quand ça va que dans un sens Oui !, quand c'est classé sans suite Moi j'ai ramé, ramené la merde à mes rents-pa Et j'donne tout à mes frères marlich s'ils me le rendent pas La justice on s'la fait nous même, I'm so Hood ! Un dialogue de sourd entre moi et ma bouteille d'Absolut Me parle pas d'la gloire n'y même du sommet Nan, nan, nan Pour l'instant j'me bats pour finir la semaine Mais guette moi j'suis la j'rappe sale vas-y acquiesce De nos jours tu peux rater l'grand amour si t'as pas d'caisse - Sta-ive c'est du vécu On comprend que chez moi le sang c'est vidé à cause du manque d'écus - Oui c'est l'cercle est vicieux bienvenue dans le cerceau - Ça va péter dans l'quartier, dans tout les ghettos d'France - J'sais c'que c'est d'avoir la dalle, j'en connais les vertus - 11.43 mortuaire sera la saison13</t>
+          <t>Be be be be Belleville Ougataga ! C'est Mister You ! Ha'tention ! La rue puis la prison gros, écoute ça Dire à un bâtard d'm'écrire autant dire à Fat Joe d'maigrir Demain ils vont pleurer donc aujourd'hui j'laisse les mecs rire Nos vaches si on n'peut les prendre on va les traire c'est mieux qu'rien Ma bite ouais ils ont pris nos terres donc faut qu'ils crèvent ces mécréants Ils m'ont grillé en train d'mettre ma bite dans leur cul puis Ils n'ont fait que m'pister car pour me sauter fallait du r'cul 75 mon matricule ça défouraille au crépuscule Celui qui veut test il coule vu qu'nous on s'en bas les testicules Astiquez ma cellule j'ai tout dans l'cul plastifié On ne peut pas l'identifier mais c'est du seum certifié Petit frère leurs paroles, c'est d'la merde faut pas t'y fier T'as beau être fort à l'école eux ils t'conseilleront pâtissier Tout dans l'excès on sait pas tiser, on regrette Tony et petit Zé D'une balle on peut t'viser après avoir sympathisé Petit c'est, tranchant si, si comme un coup d'couteau C'est bouillant comme un toto poto, c'est clair comme une goutte d'eau Qu'les p'tits oiseaux dans l'ghetto, ils bé-tom avant d'savoir voler Parce qu'ils s'achètent un pistolet pour plus vite se rafistoler Pédé si tu sais sucer ben personne pourra t'pistonner Jadis c'était sur 6 maintenant sur 24, piste on est Sous haute tension, Ah'ttention mesdames et messieurs Dans un instant, ça devrait vous crever les yeux Nos avocats souillent nos sous, nous avons cassé le zoo On sait pas c'qui s'passe mais bon en tout cas c'est le souk On sait pas danser le zouk par contre on sait frotter les cavus On sait chiner une pute sans lui payer ce qu'elle veut On fait un vu que d'vant un oint-j à quatre feuilles On aide les p'tites vieilles que pour chlaker leurs portefeuilles On va au charbon quand y'a foye, dans l'système on ne voit qu'la faille Yougataga pour du shit on pète la vitre de l'hygiaphone Fuck la stup au microphone, au 36 ils raffolent Voir les siste-gro s'faire soulever, pister via leurs phone Moi j'suis pas l'genre à baver en g.a.v J'criais d'jà Belleville j'savais même pas quel âge j'avais Chez moi on ne confond pas le cool-al et la javel Rentre ma bite dans ton cul va en vacances et nage avec Le me-seu c'est ma navette, la ille-feu c'est ma manette J'cogite, il m'faut du shit pour qu'mon esprit s'évade avec Belleville, ça m'manque le pacifique et ses mangues J'suis bloqué par l'ciment j'prie Dieu, j'remercie m'man Car j'suis né en ce-Fran mais je ne suis pas un autochtone Putain d'poissard aux arrivants un mois d'octobre J'mérite le brassard tel Ronaldinho au Barça Golden Crew aux platines une grosse dédicace à bersa J'roule un perso, je hula hoop avec un vicieux cerceau Étant p'tit j'rêvais d'limer les barreaux de mon berceau A Belleville zoo c'est l'ptit risou qui tue le rat Comme on dit un tiens vaut mieux que deux tu l'auras Promesse tenue rime toujours avec prouesse Vengeance avec finesse, Marvin avec Younes Le coup droit d'la coupe, barrage en couille dès ma jeunesse C'que j'ai fait et c'que j'vais faire était écrit avant qu'je naisse L'homme descend du singe, le singe descend de l'arbre C'est pour ça qu'j'kiffe l'herbe chaque jour j'fume 200 dollars L'été ma liberté fut acheminée vers le cachot Où j'fumais plus qu'une cheminée tout en tisant du Coca chaud Hey mutchatcho, Shriki once quarenta y tres Big up Chérif Triki Frederico Fernandez Pour mon frère Yacine j'pourrais comparaitre pour assassinat Un braquage lyrical j'dédicace à Nos mère pleurent, les lits sont vides dans nos chambres On compte sur l'Seigneur, nos deux bras, nos trois jambes La rue la son-pri ses rasoirs à double tranchant J'pourrais t'saigner comme Diz l'araignée et Tandian Y'a tant d'gens qu'aimeraient savoir ce que nous savons On n'dit jamais jamais à part quand faut ramasser l'savon Les gavons aimeraient avoir ce que nous avons On va d'l'avant l'arme pour l'suicide on t'la vend c'est navrant Ougataga mais nique sa mère c'est comme ça La vie c'est une pute faut la maquer cette lope-sa J'suis cette debza sous faya qu'a dérapé Et quiconque voudra m'tester sera VIP au Quai d'l'a Rapée J'suis avec mes khels mes 3arbis j'suis lancé on ne m'arrête plus J'ai mon sky ma redbi j'dédicace à Omar Hedbi J'cogite, j'gamelle mon co-détenu c'est Djamel L'un s'embrouille l'autre s'amène dites bien au juge qu'il nique sa mère Avant hier j'étais au D5 bientôt j'me barre en Thaï L'ancien garde tes conseils sérieux t'es pas rentable Autrefois c'était pour les alloc' familiales Maintenant ça t'met en cloque pour une condi' parentale Si si on braque ni les banques ni les pharmacies Par contre on crosse les grossistes on les fait fort mincir La vie c'est une pute faut qu'tu la maques moi aussi Mon niveau d'étude, j'crois qu'j'ai un bac -6 Fuck les ton-ma qui jouent les cro-ma et s'prennent pour Percie J'roule un gare-ci si l'préau s'rait Bercy j'aurais d'jà percé Quand on m'a ouvert la porte c'était un surveillant comment lui dire merci Aux arrivants, déboussolant totale inertie Tout à prouver roofer j'débarque en R6 ou en ZX Et vers neuf heures j'pète le Mercier Face au passé ça sent la merde à présent La rue puis la prison, Belleville zoo ça tombe à treize ans Dès qu'ça sent la patate hata nous maîtrisons Gamberge de triso pour un 10E ça peux t'ghissou À quiconque voudrait parier ben ça d'vrait lui couter ses sous Pour Lassana Diarra ben on pourrait ligoter Zizou J'mérite pas d'bisou, j'm'en fous j'sors du zoo J'éclate les ondes, j'éclaire les ombres j'rappe quatre saisons J'vend du crack des tazoo, j'suis d'la bande à Bazoo On a rencard avec les shlag donc la pure nous la basons Dehors ça vend la maxou au parloir ça cale des maxons Les matonnes mouillent à la vue de ce qu'on a dans le caleçon Dehors ça vend la maxou au parloir ça cale des maxons Les mecs sont farouches depuis qu'tous les chemins mènent à Zou J'grille les rouges passe au feu vert m'a dit Philippe J'lui ai dit j'arrive avec Mahmoud, Karter et Madi Filis Avec ma bande d'enfoirés j'fous la merde dans vos soirées J'vais ramener tout l'quartier, Kirchon Dadjé et Salim Souaré N'est-il pas vrai frelon que l'on s'regarde au grand quartier ? Moral en béton quand on bé-tom y'a pas d'brancardier Ça sert à rien de vouloir jouer les G.I.Joe imbécile Droite gauche dans tes cils comme dit Wadjon Ramenez toutes vos putes elles vous diront c'est qui le mac Nadjib, Bilel c'est la famille c'est Kill O Mic Rap trop violent à chaque mesure j'cause l'hématome J'en ai vu des surveillants jouer les cro-ma d'vant les matonnes Stop, regarde la gueule de l'ingé' qui m'enregistre Et qui fait l'écoute du flow sorti tout droit de Fleury Mérogis J'vend d'la came donc j'porte trois fois l'numéro six gros Quand j'monte à Dam c'est pour crosser la mère au sisste-gro Le micro j'le rend paro il attrape le chikungunya C'lui qui veut m'test ben j'lui pète ses chicots d'une bounia Pour Zied et Bouna à qui ils ont remis la chaise électrique Rechargeons nos puhska et allons tous chasser les flics Pour Zied et Bouna à qui ils ont remis la chaise électrique Rechargeons nos puchska et allons tous chasser les flics Pou-pou-pour Zied et Bouna à qui ils ont remis la chaise électrique Rechargeons nos puhska et allons tous chasser les flics You might also like Be-bebebe-bebebe-bebebe-Belleville ! Attention, c'est Mister You, gros Ah, Woogataga La rue puis la prison, gros Belleville, 11ème, 19ème4</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>La Rue Puis La Prison</t>
+          <t>11.43</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Be be be be Belleville Ougataga ! C'est Mister You ! Ha'tention ! La rue puis la prison gros, écoute ça Dire à un bâtard d'm'écrire autant dire à Fat Joe d'maigrir Demain ils vont pleurer donc aujourd'hui j'laisse les mecs rire Nos vaches si on n'peut les prendre on va les traire c'est mieux qu'rien Ma bite ouais ils ont pris nos terres donc faut qu'ils crèvent ces mécréants Ils m'ont grillé en train d'mettre ma bite dans leur cul puis Ils n'ont fait que m'pister car pour me sauter fallait du r'cul 75 mon matricule ça défouraille au crépuscule Celui qui veut test il coule vu qu'nous on s'en bas les testicules Astiquez ma cellule j'ai tout dans l'cul plastifié On ne peut pas l'identifier mais c'est du seum certifié Petit frère leurs paroles, c'est d'la merde faut pas t'y fier T'as beau être fort à l'école eux ils t'conseilleront pâtissier Tout dans l'excès on sait pas tiser, on regrette Tony et petit Zé D'une balle on peut t'viser après avoir sympathisé Petit c'est, tranchant si, si comme un coup d'couteau C'est bouillant comme un toto poto, c'est clair comme une goutte d'eau Qu'les p'tits oiseaux dans l'ghetto, ils bé-tom avant d'savoir voler Parce qu'ils s'achètent un pistolet pour plus vite se rafistoler Pédé si tu sais sucer ben personne pourra t'pistonner Jadis c'était sur 6 maintenant sur 24, piste on est Sous haute tension, Ah'ttention mesdames et messieurs Dans un instant, ça devrait vous crever les yeux Nos avocats souillent nos sous, nous avons cassé le zoo On sait pas c'qui s'passe mais bon en tout cas c'est le souk On sait pas danser le zouk par contre on sait frotter les cavus On sait chiner une pute sans lui payer ce qu'elle veut On fait un vu que d'vant un oint-j à quatre feuilles On aide les p'tites vieilles que pour chlaker leurs portefeuilles On va au charbon quand y'a foye, dans l'système on ne voit qu'la faille Yougataga pour du shit on pète la vitre de l'hygiaphone Fuck la stup au microphone, au 36 ils raffolent Voir les siste-gro s'faire soulever, pister via leurs phone Moi j'suis pas l'genre à baver en g.a.v J'criais d'jà Belleville j'savais même pas quel âge j'avais Chez moi on ne confond pas le cool-al et la javel Rentre ma bite dans ton cul va en vacances et nage avec Le me-seu c'est ma navette, la ille-feu c'est ma manette J'cogite, il m'faut du shit pour qu'mon esprit s'évade avec Belleville, ça m'manque le pacifique et ses mangues J'suis bloqué par l'ciment j'prie Dieu, j'remercie m'man Car j'suis né en ce-Fran mais je ne suis pas un autochtone Putain d'poissard aux arrivants un mois d'octobre J'mérite le brassard tel Ronaldinho au Barça Golden Crew aux platines une grosse dédicace à bersa J'roule un perso, je hula hoop avec un vicieux cerceau Étant p'tit j'rêvais d'limer les barreaux de mon berceau A Belleville zoo c'est l'ptit risou qui tue le rat Comme on dit un tiens vaut mieux que deux tu l'auras Promesse tenue rime toujours avec prouesse Vengeance avec finesse, Marvin avec Younes Le coup droit d'la coupe, barrage en couille dès ma jeunesse C'que j'ai fait et c'que j'vais faire était écrit avant qu'je naisse L'homme descend du singe, le singe descend de l'arbre C'est pour ça qu'j'kiffe l'herbe chaque jour j'fume 200 dollars L'été ma liberté fut acheminée vers le cachot Où j'fumais plus qu'une cheminée tout en tisant du Coca chaud Hey mutchatcho, Shriki once quarenta y tres Big up Chérif Triki Frederico Fernandez Pour mon frère Yacine j'pourrais comparaitre pour assassinat Un braquage lyrical j'dédicace à Nos mère pleurent, les lits sont vides dans nos chambres On compte sur l'Seigneur, nos deux bras, nos trois jambes La rue la son-pri ses rasoirs à double tranchant J'pourrais t'saigner comme Diz l'araignée et Tandian Y'a tant d'gens qu'aimeraient savoir ce que nous savons On n'dit jamais jamais à part quand faut ramasser l'savon Les gavons aimeraient avoir ce que nous avons On va d'l'avant l'arme pour l'suicide on t'la vend c'est navrant Ougataga mais nique sa mère c'est comme ça La vie c'est une pute faut la maquer cette lope-sa J'suis cette debza sous faya qu'a dérapé Et quiconque voudra m'tester sera VIP au Quai d'l'a Rapée J'suis avec mes khels mes 3arbis j'suis lancé on ne m'arrête plus J'ai mon sky ma redbi j'dédicace à Omar Hedbi J'cogite, j'gamelle mon co-détenu c'est Djamel L'un s'embrouille l'autre s'amène dites bien au juge qu'il nique sa mère Avant hier j'étais au D5 bientôt j'me barre en Thaï L'ancien garde tes conseils sérieux t'es pas rentable Autrefois c'était pour les alloc' familiales Maintenant ça t'met en cloque pour une condi' parentale Si si on braque ni les banques ni les pharmacies Par contre on crosse les grossistes on les fait fort mincir La vie c'est une pute faut qu'tu la maques moi aussi Mon niveau d'étude, j'crois qu'j'ai un bac -6 Fuck les ton-ma qui jouent les cro-ma et s'prennent pour Percie J'roule un gare-ci si l'préau s'rait Bercy j'aurais d'jà percé Quand on m'a ouvert la porte c'était un surveillant comment lui dire merci Aux arrivants, déboussolant totale inertie Tout à prouver roofer j'débarque en R6 ou en ZX Et vers neuf heures j'pète le Mercier Face au passé ça sent la merde à présent La rue puis la prison, Belleville zoo ça tombe à treize ans Dès qu'ça sent la patate hata nous maîtrisons Gamberge de triso pour un 10E ça peux t'ghissou À quiconque voudrait parier ben ça d'vrait lui couter ses sous Pour Lassana Diarra ben on pourrait ligoter Zizou J'mérite pas d'bisou, j'm'en fous j'sors du zoo J'éclate les ondes, j'éclaire les ombres j'rappe quatre saisons J'vend du crack des tazoo, j'suis d'la bande à Bazoo On a rencard avec les shlag donc la pure nous la basons Dehors ça vend la maxou au parloir ça cale des maxons Les matonnes mouillent à la vue de ce qu'on a dans le caleçon Dehors ça vend la maxou au parloir ça cale des maxons Les mecs sont farouches depuis qu'tous les chemins mènent à Zou J'grille les rouges passe au feu vert m'a dit Philippe J'lui ai dit j'arrive avec Mahmoud, Karter et Madi Filis Avec ma bande d'enfoirés j'fous la merde dans vos soirées J'vais ramener tout l'quartier, Kirchon Dadjé et Salim Souaré N'est-il pas vrai frelon que l'on s'regarde au grand quartier ? Moral en béton quand on bé-tom y'a pas d'brancardier Ça sert à rien de vouloir jouer les G.I.Joe imbécile Droite gauche dans tes cils comme dit Wadjon Ramenez toutes vos putes elles vous diront c'est qui le mac Nadjib, Bilel c'est la famille c'est Kill O Mic Rap trop violent à chaque mesure j'cause l'hématome J'en ai vu des surveillants jouer les cro-ma d'vant les matonnes Stop, regarde la gueule de l'ingé' qui m'enregistre Et qui fait l'écoute du flow sorti tout droit de Fleury Mérogis J'vend d'la came donc j'porte trois fois l'numéro six gros Quand j'monte à Dam c'est pour crosser la mère au sisste-gro Le micro j'le rend paro il attrape le chikungunya C'lui qui veut m'test ben j'lui pète ses chicots d'une bounia Pour Zied et Bouna à qui ils ont remis la chaise électrique Rechargeons nos puhska et allons tous chasser les flics Pour Zied et Bouna à qui ils ont remis la chaise électrique Rechargeons nos puchska et allons tous chasser les flics Pou-pou-pour Zied et Bouna à qui ils ont remis la chaise électrique Rechargeons nos puhska et allons tous chasser les flics You might also like Be-bebebe-bebebe-bebebe-Belleville ! Attention, c'est Mister You, gros Ah, Woogataga La rue puis la prison, gros Belleville, 11ème, 19ème4</t>
+          <t>J'suis dans mon quartier, j'galère, j'regarde en l'air J'suis en train d'cogiter, j'suis défoncé sa mère J'arrive chargé, comme une porteuse à Tanger Après mon passage, ou t'es refait ou bien il te reste plus grand chose à manger J'roule un sdeh pour me percher, rejoindre l'étoile du Berger C'est plus des couilles que j'ai, eh non, c'est des gros ufs de Fabergé J'suis overbooké, ok zoogataga J'ai appris une chose chez Ruquier, c'est le mot rutabaga J'rêve que d'pouvoir, et comme vous avez pu le voir Bah le rap français c'est pas vraiment l'truc tah Audrey Pulvar Mon point commun avec Natacha c'est mes chicos d'devant Que moi-même sans mes 32 dents, j'leur faisais du rentre-dedans Ouais, bien sûr que l'avenir est inquiétant Pour des barrettes, ils nous mettent 8 ans, wesh, monsieur le président Dites leur bien que j'représente les 3arbis et les niggas Moi, j'suis plus riche qu'eux, donc pourquoi j'irai fouiller leurs caisses Eux, ils sont en pleine crise, moi j'suis en plein dans les 30 glorieuses Mais j'sais que ma liberté bah, vaut pas grand chose à leur yeuz Demande à Lacrim quand j'étais à l'école, c'était pour gratter les remises de peine Du dispatching au disque d'platine, de la fiche de recherche à la fiche de paye J'ai pété tous les barrages, mais j'n'ai jamais été odieux Comment idolâtrer la vache, quand l'univers est à Dieu Dites leur bien que, m'en bats les couilles de leur baratin Que là j'suis en promenade, 3ème tour, khapta dans un bar à tinp' Nique l'État, ces chmatas, ils rêvent que de nous mettre dans la de-mer J'vais m'branler et même cracher sur leur putain de système de merde Woogata ekh tfou, rap tah les fous Qui préfèrent s'acheter une Rafleuse que d'faire du kung-fu La Mecque, j'suis d'ceux qui se baissent et qui toussent, mec, Allah yaafo J't'ai déjà dis, nous on cotise tous pour la retraite à Clairvaux Ils nous mettent des peines de pédophile pour des histoires de barrettes Autant vendre de la cocaïne, butez-nous pour qu'on s'arrête Les 3ineurs montrent pas l'il, dites-leur de niquer leur mère les chouettes Moi, m'occupe de la vodka, woogataga gardez la Schweppes Hey, d'après mon entourage, moi, j'reste un brave J'reste un vrai, c'est pour ça qu'il m'encourage Après la pluie, y a pas le beau temps, y a l'orage C'est vrai que les petits sont hardcore, on était pareil à leur âge À deux sur un scooter on vivait que de vol à l'arrach' Puis on a connu la crave-bi et on a vite tourné la page On s'est mis à couper des barrettes, ensuite à vendre des plaquettes Puis d'la coke et des galettes, jusqu'à ce que les keufs nous arrêtent Un jour j'étais dans le 19, l'lendemain un hessess fermait ma porte Un soir j'étais avec une meuf, l'lendemain elle était avec mon pote La vie c'est dur, pas de peine nous tout ce qu'on porte c'est des flingues Et y a pas de vice de procédure gros c'est la loi de la jungle C'est pas d'ma faute, darwa, j'crois bien que j'suis taré d'naissance J'me reconnais pas moi-même des fois j'suis ravi de faire ma connaissance Et quand je pars au shtar, bah t'inquiète pas que j'reçois des mandats Et j'ai toujours la frappe, tah Hollanda et tah Belhanda J'suis khapta, zoogataga sous ma véranda J'glisse mes doigts dans les cheveux tah Esméralda J'emmerde l'État, j'emmerde les stups, j'emmerde les gendarmes Trafiquant de rimes, trafiquant d'stups ou trafiquant d'armes Je suis, comment vous dites ? Paranoïaque ! Ouais J'm'en bat les yeuks, madame la juge, baraneyek ! Ytiyyeh sa3dek ! J'te l'avais dit que j'avais des projets Là, j'graille des brochettes, j'insulte ta mère et j'touche des gros chèques M'achète des trucs qui valent cher, rien qu'avant hier J'me suis acheté 3-4 t-shirt, j'ai dépensé ton salaire J'me suis roulé un gros sdeh, puis j'ai repensé à la misère À cet été, à cet hiver, Alicante ou au Val-d'Isère Au mitard tah la Santé, les promenades en camembert Au mitard tah Fleury, j'revois les toilettes, j'me dis beurk ! Ah les bâtards, comment ils ont pu me faire ça ? Ils me l'ont mise, j'leur ai remise woogata vice et versa Ya zzeh, obligé de se faire remarquer Obligé de se faire embarquer, déféré au parquet Direction les grillages, bon, trêve d'enfantillage Yeah, I speak a little English, motherfucking biatch ! Weld lqahba, what you gonna do? Ok, j'continue tout doux, j're-big up le rott' Mamadou Yoogata yoogata gangz to gangz Ouais, tu connais la musique, celui qui veut me test, j'le baise You might also like Ban-ban-bandit j'fait que du propre, j'effectue les sales tâches Ça sert à quoi de jouer le pirate, si pas à l'abordage Ils dopent en dopant, co on t'laisse le dos en deux On est nous-mêmes en paix exorcistes avec un joint d'beuh Tous les soirs j'dégrise, nos combines se développent Mais des fois les quis' débarquent et dans les comptes ça fait des flops Du crime ouais y'a la crème, Sta-ive c'est du vécu Mon gros, chez moi le sang s'est vidé à cause du manque d'écus Pas de ces collabos, que t'achètes avec alcool et abus De plus, j'baise ces nabots qui croient contrôler la rue Les yeux cernés au poste, menotté à des barreaux de chaise J'rêve d'Îles Vierges m'en fumer avec des barreaux de chaises La nuit j'dors mal, éternellement tourmenté En pensant que j'vais prendre cher si les keufs arrivent à tout remonter Ceux qui sèment le vent, récolte du ons dans le ventre A-L, futur ex-braqueur reconverti dans la vente J'aimerais partir tranquille, les pieds d'vant Un monde de fils de pute, j'suis obligé de vendre Ah bon ? Ça suffit pas alors on braque sa mère M'en voulais pas dans le rap y'a trop de zamels 3 quart, belle coupe, chico cassé La vie c'est speed même mon ombre veut me dépasser Oh, le sky est classé, j'suis chaud Menacer ne sert à rien, j't'envoie 2-3 balles l'affaire est classé Ramassé du biff, voilà dans quoi j'me suis perdu J'sais c'que c'est d'avoir la dalle, j'en connais ces vertus Hyper dur, fréquentation malsaine Chiale pas sur mon sort, tu sais qu'ici personne nous accepte On connait le respect, les valeurs et les principes T'es le plus grand des hommes si tu te lèves pour bosser à Rungis Malheureusement pas mon cas, au fond de moi je les envie Nos vies, c'est faire du biff, mais resté en vie Donc faut marcher armé, puis avoir la trique Aujourd'hui t'allumes demain t'es complètement matrixé C'est la vie du western, la vie d'moi j'suis réel La tranquillité frérot est bloquée dans mes rêves Impossible de l'avoir, je ne prends jamais de Mais Belek au feu le couz si tu mets trop de bois Beaucoup de salopes font les voyous, wallah que c'est pas une fierté Dis-moi qui sera là le jour ou t'auras vraiment merdé J'ai l'orgueil d'un bébé, je m'énerve et je pète tout J'assume les conséquences khey dans mes bras je prend le mektoub Oui j'aime pas les poulets et je f'rais recette sans eux Une impression même jaloux de ma paire à 700E Ils m'inventent des vies, le mythe ils veulent casser Hum j'en ai assez, les traquer, les chlasser Quand j'allais tu revenais, dans ta tête ça ne rentre pas Je le ferai tout les jours, je compte l'oseille me dérange pas Bien sur qu'on s'est fait tout seul, je sais très bien que tu sais J'ai braqué des bijouteries quand les autres allaient sucer Sans t'manquer de respect, dans l'rap dis-moi ce qui est facile Frérot on viens de la rue c'est des filles faciles J'ai roulé ma bosse, j'en ai marre d'bouffer d'la merde Coup d'crosse, la vie t'assomme pire qu'un joint d'herbe Tout c'qu'on a, on finit par l'perdre Étoile de mer, dix mille kilomètres, perdu sur la lune verte J'suis tellement loin des je veux être Berrad d'atay, j'allume un jaabouq à la fenêtre T'es dans l'paraître, moi j'veux disparaître Les kheys passent au dispatching, une mère qui pleure c'est la faute d'un traître Y'a plus qu'des bras cassés dis-moi à qui serrer les coudes ? Six pieds sous terre, quand j'me ferai bouffer par l'doud Noyé dans l'doute, j'suis toujours dans l'hood Les yeux rouges, Wydad Casanegra j'suis pas un Blood Passe-moi des feuilles, c'soir j'fume mes dernières illusions Sers-moi un verre que j'tourne cette tragédie en dérision 11.43, mortuaire sera la saison Maintenant j'marche avec des rétros, dis-moi qui va m'sauter l'caisson Y'a, y'a, y'a plus d'rage que d'la fashionnerie J'enterre l'espoir dans un parloir à Fleury Ghetto youth langage, du whisky, les chicots pourries Bonbon sauvage, 0.4 khoya souris Heh-hep-pep, Dieu seul est maitre de ma destinée Moi j'me verrais bien à La Mecque avec mes rents-pa et ma dulcinée La vie c'est pas un clip ni du ciné ou une bande dessinée On va peut-être finir à Clairvaux, on va peut-être s'faire assassiner C'est clair gros qu'on peut tout perdre sur un coup d'ker-po J'te parle d'une boite où pour rentrer y'a même pas besoin d'se faire beau Le cercle est vicieux bienvenue dans le cerceau Quand j'ai fêté mes 16 ans c'est pas du plomb que j'avais dans le cerveau J'ai 28 ans, j'habite dans l'zoo, je m'appelle Hédi Chabar J'veux réussir, j'veux m'en sortir depuis que j'suis tout petit je chabarde J'ai bicrave, j'ai fais plein d'conneries dont j'suis pas du tout fier Comme les aller-retours à Fleury pour battre le fer faut du fer Pour faire du flouze faut du flouze, des couilles et d'la gamberge Surtout quand t'es seul contre tous y'a personne pour te tendre la perche Moi, hamdullah, j'suis pas comme ça, j'préfère aider mon prochain Car j'sais que Dieu me l'rendra ici bas ou dans un monde prochain Howa yaalem b kolchi, hata tkoun labes Gucci Lmout tjik w teddik, tedderbek kima lfuchi J'arrive dans l'game avec You pour écraser tous ces chiens Même s'ils sont plein, on les baise tous kalachnikov à la main Ça va péter dans l'quartier, dans tous les ghettos d'France Ayet lkursi, 11.43 pour me souhaiter bonne chance M'en bats les couilles de c'que tu penses, depuis ma tendre enfance J'laisse la concurrence en transe, lourde sera la sentence Brulux on the flux toujours dans les bacs Hier, ils m'boycottaient, maintenant, ils veulent faire mes backs Prochain clip, j'appelle Fredo, il m'prépare le Maybach Cette fois-ci, j'ferai pas l'gamin, promis, j'cacherai tes plaques Ils m'ont pris pour une blague, des mesures, il m'en reste quatre Pour ma mère, j'veux du 2.4, pour moi qamis, un RS4 Dédicace l'Algérie, le Maroc, la Tunisie Faudra bientôt retourner chez nous car y a trop d'crapules ici Parce que tu manges du lion l'matin devant moi tu veux rugir Approche j'te mets une claque de roumain, tu vas rougir Plus tu vas monter, plus les rumeurs vont surgir Personne n'est au-dessus d'personne, écoute bien tout c'que j'vais te dire Tout ce qui est autour de moi, j'vais te l'exposer La j'pète les plombs j'ai retiré la goupille, j'vais exploser À ma droite, les frères muz débarquent pour nous faire des rappels Par la gauche, y en a qui vesqui s'hab quelqu'un les appelle En primaire j'te frappais ouai j'me prenais pour l'king À 10 ans au comico voiture péta dans un parking Le quartier c'est une plaque tournante, ça défouraille de partout Dans mon escalier j'tombe sur un sac remplis d'billets j'garde tout Assis sur un banc toute la journée ça bibi Dans les bois ça fait bep-bep ou cric-cric bim bim ! Au collège, lycée v'là les bagarres, boy, j'casse des dents Avec Oxmo ou pas leurs uppercuts te rentre dedans On sait que la police nous surveille mais elle ne sait pas tout Les malins savent très bien que l'argent ne fait pas tout On a des avocats mais ils n'arrangent pas tout Les médecins sont la mais il ne soignent pas tout Pas de chance cette nuit la juge s'est fait mal baiser Donc forcément des chance d'être acquitté on baissées T'es pressé, t'accélères risquer sont les raccourcis Kazou dis leur que cette est pute mais plus de soucis que d'sursis Posé à la tess j'ai rien vu, rien entendu J'ves-qui les histoires tendu, des fois c'est tes potes qui t'enculent Avec du recul, tu finis par devenir solitaire Pour l'Etat on a pas les critères, donc on a fini sur le ter J'vois des pères, des mères qui travaillent dur pour ceux qu'ils aiment Wallah ça m'fait de la peine d'les rentrer pour rien dans nos problèmes 11.43 c'est le thème, là c'est Tirgo sur l'antenne Poto dès l'début de l'enquête c'est possible que tu perds la tête Envoie la frappe de Ketama dédicace à Khadama J'suis obligé d'faire du sale y'a toute la cité derrière moi Y'en a qui braquait des tabacs nous on bicravait du taga Ouais continuer à taguer nous on à pas l'temps on tabasse On va t'laisser aux aguets dé-ter comme l'armée du Hamas J'savais pas que sur ce banc ouais j'allais fumer des kamas Toute l'année tu fais des phases poto, c'est pas comme a-ç Dans l'arène j'ai toujours la faille, flow qui tire comme un Fa-mas Nous on est comme des hommes, on va toujours à la chasse Y'a du biff' et des liasses obligé on s'déplace Ça bicrave au fond de l'impasse, désolé si ça dépasse Dans ton bigo y'a les vrais et les boloss que t'effaces We-wesh la racaille, les raclures la police en a ras-le-cul Ma vie c'est un texte de rap remplit d'ratures Nerveux l'sourire aux lèvres doté d'pouvoir céleste J'ai perdu l'nord ma direction à moi c'est l'est J'écris des textes de fou, beaucoup métaphorique L'histoire d'un braqueur qui finit par taffer au Ritz Rosny-sous-Bois, la Sambuy, les braquos, les sous-salles Les sous-sols, les mouses, ceux qui moussent et qui s'débat ainsi qu'les douzes J'rappe, je pense comme un mec de la ur J'aime la pure qui branche les clients sur mon terrain tout les jours J'ai pas d'bonnes habitudes j'descends et j'traine J'truande j'ves-qui la justice dédicace à Fresnes Les sirènes retentissent, les criminels se repentissent La pisse du sheïtan, mes repentises, ma hantise C'est vraiment pas la mort mais c'qui s'en suit J'aime quand ça va que dans un sens Oui !, quand c'est classé sans suite Moi j'ai ramé, ramené la merde à mes rents-pa Et j'donne tout à mes frères marlich s'ils me le rendent pas La justice on s'la fait nous même, I'm so Hood ! Un dialogue de sourd entre moi et ma bouteille d'Absolut Me parle pas d'la gloire n'y même du sommet Nan, nan, nan Pour l'instant j'me bats pour finir la semaine Mais guette moi j'suis la j'rappe sale vas-y acquiesce De nos jours tu peux rater l'grand amour si t'as pas d'caisse - Sta-ive c'est du vécu On comprend que chez moi le sang c'est vidé à cause du manque d'écus - Oui c'est l'cercle est vicieux bienvenue dans le cerceau - Ça va péter dans l'quartier, dans tout les ghettos d'France - J'sais c'que c'est d'avoir la dalle, j'en connais les vertus - 11.43 mortuaire sera la saison13</t>
         </is>
       </c>
     </row>
@@ -1818,12 +1818,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Mister Mister</t>
+          <t>GOGETA</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>J'tourne au Mali, en Algérie, au Maroc, en Tunisie J'roule sans permis décapoter j'graisse la patte aux policiers Moi, mon rap c'est d'la pure donc vos oreilles s'anesthésient Y'a plus de schmet' dans c'game que d'muslims en Indonésie Si t'es un brave j'suis ton ami, si tu veux jouer j'suis Konami J'ai fait connaître Belleville de Marrakech à Miami Traces ta route, ne t'arrêtes pas j'te conseilles d'aller tout droit Un mec avertit il en vaux deux, un mec affranchis il en vaux trois Ah ! Ah ! Woogataga, y'a qu'la maille qui m'aille J'suis déréglé comme le calendrier Maya Quand tu dors moi j'suis réveillé Mon cerveau il aime trop travailler J'suis miclo, j'suis pas popeye-yé j'mésquive pas quand faut payer Mister-Mister Yougataga Toujours frais ! Mister-Mister Yougataga Ouais tu connais ! Mister-Mister Yougataga Rap the best of the best tah le best des best ! Aiiiee ! Mister-Mister Yougataga Pour les res-frè Mister-Mister Yougataga Ouai, ouai, ouai ! Mister-Mister Yougataga I'm the best of the best tah le best des best You might also like J'arrive l'sourire en coin avec un regard de vénère J'attire toutes les femelles donc tout les mâles ont les nerfs Moi mes souvenirs au château c'est des promenades en plein air J'suis devenu l'prince de machiavel, de ma ville pas de Bel-Air V'là la jet-set avenue des Peupliers Ouuaaaii ! J'suis venu foutre le feu donc appeler les pompiers Dans l'rap j'ai pris un bon billet Bénef les plus éparpillés La SACEM je l'ai plié Ca à fini par payer J'suis en règle j'ai mes papiers et mon pochka dans la saccoche J'ai deux bras droit j'ai pas d'bras gauche Et j'sais bien que l'droit chemin y vire à che-gau Eux se qui ont éco darwa j'ai dans la che-fo Mister-Mister Yougataga Toujours frais ! Mister-Mister Yougataga Ouais tu connais ! Mister-Mister Yougataga Rap the best of the best tah le best des best ! Aiiiee ! Mister-Mister Yougataga Pour les res-frè Mister-Mister Yougataga Ouai, ouai, ouai ! Mister-Mister Yougataga I'm the best of the best tah le best des best Du nord au sud, à l'est, à l'ouest Y'a qu'un Younès que j'connaisse I am the best of the best tah le best des best T'as pas senti la patate ça vient direct de Paris Passe moi les clés d'la baraque j'te laisse celle du Ferrari La patience est une vertu récompensant l'escargot Ils s'la racontent avec leur barque fallait que j'leur laisse un cargo Vas dire aux 3ineurs d'aller faire un tour chez l'ophtalmo Gros j'suis parano j'regarde même plus les panneaux Moi je n'étais rien, mais voila qu'aujourd'hui J'suis devenu l'prince du gardien du sommeil de ses nuits J'ai l'train vie d'Usain Bolt impossible que je m'ennuie J'suis en train d'danser la samba va voir le roi et demande lui qui est le best Mister-Mister Yougataga Toujours frais ! Mister-Mister Yougataga Ouais tu connais ! Mister-Mister Yougataga Rap the best of the best tah le best des best ! Aiiiee ! Mister-Mister Yougataga Pour les res-frè Mister-Mister Yougataga Ouai, ouai, ouai ! Mister-Mister Yougataga I'm the best of the best tah le best des best Toujours frais ! Ouai, ouai, ouai ! I'm the best of the best tah le best des best2</t>
+          <t>Eh T'as changé l'fusil d'épaule, dis-moi c'est quoi cette phrase Gros, t'as toujours le fusil, bref j'ai dû cracher ma haine De l'amour dans les draps, j'défends ma cause, celle de la Cosa Nostra La finalité pour moi c'est pas d'rouler en caisse Il faut des rentes et tous les mois j'encaisse Faire du gros papier sans crier sur tous les toits J'mettrai jamais de l'or dans mes lettes-toi J'suis sur la route avec elle, on écoute la Bohème Même Lacrim bâtard, il sait faire des poèmes J'ai le .45 dans la veste, les oiseaux sont dans le nid Tu rêvais de grimper l'Everest, on l'a fait dans le lit Les fantômes du passé m'attendent dans mon avenir Aussi vrai que Jésus va revenir J'connais ma vie, y'a 2000 choses qui t'attirent Tu m'aimes tellement que tu veux être là quand ça tire J'suis sur Paname avec Omar On écoute Pop Smoke Envie de faire couler le sang, très calibrés sont mes Apaches Dans le garage y'a la Kalash, aux épaules j'ai poussé 200 Depuis petit, j'ai vu des choses c'est digne d'un cinéma Que Dieu m'en soit témoin, j'ai pas besoin de mentir J'suis pas Teddy Riner mais j'ai toujours été un tigre Dans la prison pour mineurs, j'étais pas du côté victime You might also like Il fallait manger à la baraque sur qui avait pas de thune En fait, se venger car l'état fait preuve d'ingratitude Jamais se ranger, être marginal c'est dans nos habitudes On rêve de nager dans le bonheur et dans la solitude Des fils de pute, viens pas froisser nos relations On parle en crypté sur des applications On a toujours des solutions mais encore plus de problèmes On se monte dessus c'est nos résolutions Faut des diamants sur la couronne qu'est sur la tête de ma daronne Ouais nous quand on prend la parole, bah on demande pas la permission Ouvre la session, j'pars en mission, sors le whisky, sors la potion Toi plus moi la solution, hormis devant Dieu pas de soumission Suffit d'un regard pour les refroidir, on va s'les faire avant d'partir Crois mon veau-cer écrit des trucs que mes vres-lè ne peuvent pas dire C'est un empire qu'on a bâti, c'est tous les faux qu'on a battus Plus l'temps pour la sympathie, le regard noir quand y a pas d'shit Mon colonel c'est pas Fabian, mon capitaine c'est pas Magic Certains me disent C'est pas logique, moi j'leur réponds C'est d'la magie Décapoté j'suis dans la Jeep, j'écoute le son, j'suis avec Ça m'fait plaisir d'aller aux Maldives, ça m'fait kiffer d'croiser ma team C'est le 9-4 et Rebeval, tu nous connais on fait les gros titres On préfère canner d'une rafale que de crever d'une hépatite Bats les couilles de ton réseau, nous c'est la fibre optique Nous ne sommes pas de ces rappeurs qui montrent leurs chibres aux p'tites Les poulets sont déjà rôtis, on braque l'oseille à Rothschild Le show il est garanti, t'arrives en caisse, tu repars en jeans Disque d'or et l'platine, putain quelle bête de routine J'ai la rime qui touche tout le monde, le micro c'est d'la chevrotine On t'nique ta mère pour des broutilles, pour un regard on peut t' Faut une guitare pour s'dire au revoir et des bougies pour le jour J On a grandi dans l'banditisme, on n'en fait pas l'apologie Ils veulent fumer nos racines, c'est pas bon pour l'écologie</t>
         </is>
       </c>
     </row>
@@ -1835,12 +1835,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>GOGETA</t>
+          <t>Mister Mister</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Eh T'as changé l'fusil d'épaule, dis-moi c'est quoi cette phrase Gros, t'as toujours le fusil, bref j'ai dû cracher ma haine De l'amour dans les draps, j'défends ma cause, celle de la Cosa Nostra La finalité pour moi c'est pas d'rouler en caisse Il faut des rentes et tous les mois j'encaisse Faire du gros papier sans crier sur tous les toits J'mettrai jamais de l'or dans mes lettes-toi J'suis sur la route avec elle, on écoute la Bohème Même Lacrim bâtard, il sait faire des poèmes J'ai le .45 dans la veste, les oiseaux sont dans le nid Tu rêvais de grimper l'Everest, on l'a fait dans le lit Les fantômes du passé m'attendent dans mon avenir Aussi vrai que Jésus va revenir J'connais ma vie, y'a 2000 choses qui t'attirent Tu m'aimes tellement que tu veux être là quand ça tire J'suis sur Paname avec Omar On écoute Pop Smoke Envie de faire couler le sang, très calibrés sont mes Apaches Dans le garage y'a la Kalash, aux épaules j'ai poussé 200 Depuis petit, j'ai vu des choses c'est digne d'un cinéma Que Dieu m'en soit témoin, j'ai pas besoin de mentir J'suis pas Teddy Riner mais j'ai toujours été un tigre Dans la prison pour mineurs, j'étais pas du côté victime You might also like Il fallait manger à la baraque sur qui avait pas de thune En fait, se venger car l'état fait preuve d'ingratitude Jamais se ranger, être marginal c'est dans nos habitudes On rêve de nager dans le bonheur et dans la solitude Des fils de pute, viens pas froisser nos relations On parle en crypté sur des applications On a toujours des solutions mais encore plus de problèmes On se monte dessus c'est nos résolutions Faut des diamants sur la couronne qu'est sur la tête de ma daronne Ouais nous quand on prend la parole, bah on demande pas la permission Ouvre la session, j'pars en mission, sors le whisky, sors la potion Toi plus moi la solution, hormis devant Dieu pas de soumission Suffit d'un regard pour les refroidir, on va s'les faire avant d'partir Crois mon veau-cer écrit des trucs que mes vres-lè ne peuvent pas dire C'est un empire qu'on a bâti, c'est tous les faux qu'on a battus Plus l'temps pour la sympathie, le regard noir quand y a pas d'shit Mon colonel c'est pas Fabian, mon capitaine c'est pas Magic Certains me disent C'est pas logique, moi j'leur réponds C'est d'la magie Décapoté j'suis dans la Jeep, j'écoute le son, j'suis avec Ça m'fait plaisir d'aller aux Maldives, ça m'fait kiffer d'croiser ma team C'est le 9-4 et Rebeval, tu nous connais on fait les gros titres On préfère canner d'une rafale que de crever d'une hépatite Bats les couilles de ton réseau, nous c'est la fibre optique Nous ne sommes pas de ces rappeurs qui montrent leurs chibres aux p'tites Les poulets sont déjà rôtis, on braque l'oseille à Rothschild Le show il est garanti, t'arrives en caisse, tu repars en jeans Disque d'or et l'platine, putain quelle bête de routine J'ai la rime qui touche tout le monde, le micro c'est d'la chevrotine On t'nique ta mère pour des broutilles, pour un regard on peut t' Faut une guitare pour s'dire au revoir et des bougies pour le jour J On a grandi dans l'banditisme, on n'en fait pas l'apologie Ils veulent fumer nos racines, c'est pas bon pour l'écologie</t>
+          <t>J'tourne au Mali, en Algérie, au Maroc, en Tunisie J'roule sans permis décapoter j'graisse la patte aux policiers Moi, mon rap c'est d'la pure donc vos oreilles s'anesthésient Y'a plus de schmet' dans c'game que d'muslims en Indonésie Si t'es un brave j'suis ton ami, si tu veux jouer j'suis Konami J'ai fait connaître Belleville de Marrakech à Miami Traces ta route, ne t'arrêtes pas j'te conseilles d'aller tout droit Un mec avertit il en vaux deux, un mec affranchis il en vaux trois Ah ! Ah ! Woogataga, y'a qu'la maille qui m'aille J'suis déréglé comme le calendrier Maya Quand tu dors moi j'suis réveillé Mon cerveau il aime trop travailler J'suis miclo, j'suis pas popeye-yé j'mésquive pas quand faut payer Mister-Mister Yougataga Toujours frais ! Mister-Mister Yougataga Ouais tu connais ! Mister-Mister Yougataga Rap the best of the best tah le best des best ! Aiiiee ! Mister-Mister Yougataga Pour les res-frè Mister-Mister Yougataga Ouai, ouai, ouai ! Mister-Mister Yougataga I'm the best of the best tah le best des best You might also like J'arrive l'sourire en coin avec un regard de vénère J'attire toutes les femelles donc tout les mâles ont les nerfs Moi mes souvenirs au château c'est des promenades en plein air J'suis devenu l'prince de machiavel, de ma ville pas de Bel-Air V'là la jet-set avenue des Peupliers Ouuaaaii ! J'suis venu foutre le feu donc appeler les pompiers Dans l'rap j'ai pris un bon billet Bénef les plus éparpillés La SACEM je l'ai plié Ca à fini par payer J'suis en règle j'ai mes papiers et mon pochka dans la saccoche J'ai deux bras droit j'ai pas d'bras gauche Et j'sais bien que l'droit chemin y vire à che-gau Eux se qui ont éco darwa j'ai dans la che-fo Mister-Mister Yougataga Toujours frais ! Mister-Mister Yougataga Ouais tu connais ! Mister-Mister Yougataga Rap the best of the best tah le best des best ! Aiiiee ! Mister-Mister Yougataga Pour les res-frè Mister-Mister Yougataga Ouai, ouai, ouai ! Mister-Mister Yougataga I'm the best of the best tah le best des best Du nord au sud, à l'est, à l'ouest Y'a qu'un Younès que j'connaisse I am the best of the best tah le best des best T'as pas senti la patate ça vient direct de Paris Passe moi les clés d'la baraque j'te laisse celle du Ferrari La patience est une vertu récompensant l'escargot Ils s'la racontent avec leur barque fallait que j'leur laisse un cargo Vas dire aux 3ineurs d'aller faire un tour chez l'ophtalmo Gros j'suis parano j'regarde même plus les panneaux Moi je n'étais rien, mais voila qu'aujourd'hui J'suis devenu l'prince du gardien du sommeil de ses nuits J'ai l'train vie d'Usain Bolt impossible que je m'ennuie J'suis en train d'danser la samba va voir le roi et demande lui qui est le best Mister-Mister Yougataga Toujours frais ! Mister-Mister Yougataga Ouais tu connais ! Mister-Mister Yougataga Rap the best of the best tah le best des best ! Aiiiee ! Mister-Mister Yougataga Pour les res-frè Mister-Mister Yougataga Ouai, ouai, ouai ! Mister-Mister Yougataga I'm the best of the best tah le best des best Toujours frais ! Ouai, ouai, ouai ! I'm the best of the best tah le best des best2</t>
         </is>
       </c>
     </row>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Street lourd, Street lourd, Street lourd, Street lourd Street lourd, Street lourd, Street lourd, Street lourd Street lourd, Street lourd, Street lourd, Street lourd Tu veux m'décendre quoi ? Tu peux pas m'décendre nan Tu veux m'décendre quoi ? Tu peux pas m'décendre nan Tu veux m'décendre quoi ? Tu peux pas m'décendre nan Tu veux m'décendre quoi ? Tu peux pas m'décendre nan Oui on ose, oui on prouve On prend ce qu'on trouve, oui on ouvre, oui on trompe Cette jungle a fait de nous des bêtes fauves Soit on progresse, soit on retombe dans les mêmes fautes La tête dans l'oseille et les mains dans la misère Dans nos yeux y'a plus de larmes on a déjà pleurer des rivières Il nous détestent on les détestent On a la culture de la gagne, la haine de la défaite Là pour la famille, Là pour les frères Préfèrent faire les choses pour les choses Que faire les choses pour les faire On a tous un peu la même vie, les mêmes vices Partir et refuser de revenir les mains vides Le quartier c'est notre chambre On voudrais pété les portes Pour que les notre prenne une autre chance La bas le monde est a nous c'est que du flanc Soit t'es in, soit t'es out, soit t'allonge, soit tu flanche Les règles suivent, retenir les reines Ce qui t'aime c'est ce qui compte le reste On s'en bat les reins, tout n'est pas donner, tout n'est pas simple Tout n'est pas vrai, tout n'est pas faux, tout n'est pas mauvais Tout n'est pas sain, dur d'aller bien, dur de faire le point Le temps demeure et les ondes passe Et on passe le temps a refaire le coin Trop y'a la peine trop y'a mort d'hommes On voudrais revenir en arrière au temps des 11 You might also like C'est du Lourd Comme un bolide a grand d'vitesse Vitesse, hesses, on t'la met en finesse C'est du Lourd 1-3,9-3,7-5 te foudroie Tu veux test le mic t'es fou toi C'est du Lourd Pour tous les tiers-quar de Paname à seille-Mar C'est You , Luciano et Sen-Lar C'est du Lourd Comme à Street Lourd, comme nos parcours Comme tous les mecs de tés-c' en bas des tours On arrive tranquillement finte crochées passement de jambes Tu connais la musique dahwa On se mélanges pas trop avec les gens On s'en bas les couilles, il nous faut dl'argent On reve d'etre dans un palais Mais pas en étant guidé par un darme-gen Sa sent la p'tata Zoogataga Ouais wahad , jouj , tlata J'suis venu pointé du doigt l'Etat C'est enculé qui vivent dans un vrai confort 9 métres carrés sans télé y'a que le shit qui nous réconforte Pour s'évadé rejoindre les airs on s'roule de gros bulldozer Qui démolisse nos veau-cer les hésess nikez vos soeurs Vu que le me-seu c'est consistant laisse la be-her pour l'désert On a la dalle on graille nos ongles on sait ce que c'est que la misère Représente Paname hein, en ce qui m'concerne Eh ouais même en cavale, j'ai eu les couilles de faire des concerts Mais où sont passé les milliards tah la lutte contre le cancer Dans les poches de Chirac donc Balladur monte sur ses grands airs La cerise sur les frégates a comme un bon coup de peinture Sarkozy trafic les scrutins et arrache sa candidature C't'enfant de putain empoche le butin et troc sa toutes p'tites voitures Contre un bête de yacht et c'est parti pour la dictature Mais il croit la mettre à qui ces bâtards de républicains Pour nourrir une seule bouche il privent des millions d'africains Dahwa sort du taga et roule un gros z'déh pour Street Lourd Zoo-zoogataga Misla, Teddy, Mosko t'pètent la bouche C'est du Lourd Comme un bolide a grand d'vitesse Vitesse, hesses, on t'la met en finesse C'est du Lourd 1-3,9-3,7-5 te foudroie Tu veux test le mic t'es fou toi C'est du Lourd Pour tous les tiers-quar de Paname à seille-Mar C'est You , Luciano et Sen-Lar C'est du Lourd Comme à Street Lourd, comme nos parcours Comme tous les mecs de tés-c' en bas des tours Au parloir cesse de peiner, mes res-f' ton enchaînés Nos surs jouent les trainés, le Sheitan vient engrainé La course aux milliards rend notre cur noir, l'a gangrèné Sur l'autoroute du suicide inutile de freiner Imprégné pelo pelo on l'a fait melo melo Mano à mano pelo dans ta face du bédo dans l'traîneau J'donne plus mon amour pour toujours À la manu chao perquise en guise de Ciao Gadjo,Gadji, nos destins sont gâchés Enragé le navire de nos rêves a déjà naufragée Embrassé ma tess par les flammes du mal C'est fait embrassé Sur le bitume nos silhouette sont tracé Nous laissé déclassé des classes Et déplacé des basses Térassé par la pouasses Nos destins entrasse au passé khey On bataille on veut tous faire de la maille Qu'on bicrave qu'on travail on sera traité de racaille Alors nique leurs meres à c'est Gros Fils de Putes Y'a pas ma téte a l'affiche j'suis fiché chez les stups 93.13 presse dans les yeuz on pense qu'a craché comme mon gun Crache la fumée mes poumons sont encrassé Grassié Gracias muchachos muchachas, comme Fallait bien que j'me refasse Atrophié assomer par l'enclume du procureur Sur street lourd j'garde mon profil de tueur C'est du Lourd Comme un bolide a grand d'vitesse Vitesse, hesses, on t'la met en finesse C'est du Lourd 1-3,9-3,7-5 te foudroie Tu veux test le mic t'es fou toi C'est du Lourd Pour tous les tiers-quar de Paname à seille-Mar C'est You , Luciano et Sen-Lar C'est du Lourd Comme à Street Lourd, comme nos parcours Comme tous les mecs de tés-c' en bas des tours C'est du lourd</t>
+          <t>Street lourd, Street lourd, Street lourd, Street lourd Street lourd, Street lourd, Street lourd, Street lourd Street lourd, Street lourd, Street lourd, Street lourd Tu veux nous descendre quoi ? Tu peux pas nous descendre nan Tu veux nous descendre quoi ? Tu peux pas nous descendre nan Tu veux nous descendre quoi ? Tu peux pas nous descendre nan Tu veux nous descendre quoi ? Tu peux pas nous descendre nan Oui on ose, oui on prouve On prend ce qu'on trouve, oui on ouvre, oui on trompe Cette jungle a fait de nous des bêtes fauves Soit on progresse, soit on retombe dans les mêmes fautes La tête dans l'oseille et les mains dans la misère Dans nos yeux y'a plus de larmes on a déjà pleuré des rivières Il nous détestent, on les déteste On a la culture de la gagne, la haine de la défaite Là pour la famille, là pour les frères Préfère faire les choses pour les choses que faire les choses pour les faire On a tous un peu la même vie, les mêmes vices Partir et refuser de revenir les mains vides Le quartier c'est notre chambre On voudrait péter les portes pour que les nôtres aient une autre chance Là-bas le monde est à nous c'est que du flan Soit t'es in, soit t'es out, soit t'as l'manche, soit tu flanches Les règles suivent, retenir les rênes Ceux qui t'aiment, tout ce qui compte, le reste on s'en bat les reins Tout n'est pas donné, tout n'est pas simple Tout n'est pas vrai, tout n'est pas faux, tout n'est pas mauvais, tout n'est pas sain Dur d'aller bien, dur de faire le point Le temps demeure et les ondes passe Et on passe le temps à refaire le coin Trop y'a la peine, trop y'a mort d'hommes On voudrais revenir en arrière au temps des 11 You might also like C'est du Lourd Comme un bolide à grande vitesse Vie d'tess, hesses, on t'la met en finesse C'est du Lourd 1-3, 9-3, 7-5 te foudroient Tu veux test le mic t'es fou toi C'est du Lourd Pour tous les tiers-quar de Paname à seille-Mar C'est You, Luciano et Sen-Lar C'est du Lourd Comme à Street Lourd, comme notre parcours Comme tous les mecs de tés-c' en bas des tours On arrive tranquillement, feinte crochets passement de jambes Tu connais la musique, dahwa on se mélange pas trop avec les gens On s'en bas les couilles, il nous faut d'l'argent On rêve d'être dans un palais mais pas en étant guidé par un darme-gen Sa sent la p'tata, zoogataga Ouais wahad , jouj , tlata J'suis venu pointer du doigt l'État Ces enculés qui vivent dans un vrai confort Neuf mètres carrés sans télé y'a que le shit qui nous réconforte Pour s'évader, rejoindre les airs, on roule de gros bulldozers Qui démolisse nos veaux-cer, les hésess niquez vos surs Vu que le me-seu c'est consistant, laisse la be-her pour l'désert On a la dalle, on graille nos ongles, on sait ce que c'est que la misère Représente Paname hein, en ce qui m'concerne Eh ouais même en cavale, j'ai eu les couilles de faire des concerts Mais où sont passé les milliards tah la lutte contre le cancer Dans les poches de Chirac donc Balladur monte sur ses grands airs La cerise sur les frégates a comme un bon coup de peinture Sarkozy trafique les scrutins et arrache sa candidature C't'enfant de putain empoche le butin et troque sa tout p'tite voiture Contre un bête de yacht et c'est parti pour la dictature Mais ils croient la mettre à qui ces bâtards de républicains Pour nourrir une seule bouche il privent des millions d'Africains Dahwa, sors du taga et roule un gros z'déh pour Street Lourd Zoo-zoogataga, Mista, Teddy, Mosko t'pètent la bouche C'est du Lourd Comme un bolide a grand d'vitesse Vitesse, hesses, on t'la met en finesse C'est du Lourd 1-3, 9-3, 7-5 te foudroient Tu veux test le mic, t'es fou toi C'est du Lourd Pour tous les tiers-quar de Paname à seille-Mar C'est You, Luciano et Sen-Lar C'est du Lourd Comme à Street Lourd, comme notre parcours Comme tous les mecs de tés-c' en bas des tours Au parloir cesse de peiner, mes res-f' ton enchaînés Nos surs jouent les trainées, le Sheitan vient engrainer La course aux milliards rend notre cur noir, l'a gangréné Sur l'autoroute du suicide, inutile de freiner Imprégné pelo pelo on l'a fait melo melo Mano à mano pelo dans ta face, du bédo dans l'traîneau J'taime plus mon amour pour toujours À la Manu Chao, perquise en guise de Ciao Gadjo, Gadji, nos destins sont gâchés Enragé, le navire de nos rêves a déjà naufragé Embrasée, ma tess par les flammes du mal s'est faite embrasser Sur le bitume, nos silhouettes sont tracées Délaissés, déclassés, déclassés, déplacés Dépassés, terrassés par la poisse Nos destins on trace au passé, khey On bataille, on veut tous faire de la maille Qu'on bicrave, qu'on travaille, on sera traité de racaille Alors nique leurs mères à ces gros fils de putes Y'a pas ma tête a l'affiche, j'suis fiché chez les stups 93, 13 braise dans les yeuz, on pense qu'à brasser Comme mon gun, j'crache la fumée, mes poumons sont encrassés Grazie, gracias muchachos muchachas Comme Pachanga, fallait bien que j'me refasse Atrophié, assommé par l'enclume du procureur Sur Street Lourd j'garde mon profil de tueur C'est du Lourd Comme un bolide à grande vitesse Vie d'tess, hesses, on t'la met en finesse C'est du Lourd 1-3, 9-3, 7-5 te foudroient Tu veux test le mic t'es fou toi C'est du Lourd Pour tous les tiers-quar de Paname à seille-Mar C'est You, Luciano et Sen-Lar C'est du Lourd Comme à Street Lourd, comme notre parcours Comme tous les mecs de tés-c' en bas des tours C'est du lourd</t>
         </is>
       </c>
     </row>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Lets go, Lets go Grrt Lets go, Lets go Ok j'ai déjà mis les bandes, rebeu, jm'échauffe pas Tête-à-tête avec toute ta bande, bitch me chauffe pas J'attends les échos du ghetto pour mettre les salopes à lamende Y a que la 'dre qui m'alimente khawf te sauve pas La Caille c'est pas TikTok tic-tac p'tite frappe J'ai des tactiques d'attaque j'suis pas dans les cheat-codes Jtire pas sur ls ambulances et jtape pas ls p'tites fiottes Jsuis toujours fidèle à mon opinel et à ma p'tite fiole J'ai les tibias durs, j'fais tomber les bambous Trapu jte take down, j'fais tomber les montagnes J'vais refaire la peinture, le corps suit le mental Sur le champ d'bataille au premier son des tambours J'te laisse par-terre fuck le procès Dans tous les cas y aura Fateh pour te crosser J'peux revenir d'un jour à l'autre comme Ragnar J'suis un rageux comme Ivar le désossé J'marche avec ceinture noire que personne sépare Sur le bitume que ça part en JJB sous JB Nos ruelles sont cruelles ici personne t'épargne On restera des ados remplis de haine, CJD T'auras pas l'temps d'dire Ajdimé Tu manges une rafale dans l'gilet Agité, Algérien d'bâtard obligé d'te giffler D'vant ton gang j'te localise j'y vais You might also like Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods On les tabasse les tartine les marave La dalle d'un seul homme peut exploser des barrages Par principe on t'arrange ou on t'arrache Mais wAllah qu'ça m'arrange quand j'laisse parler ma rage Suce à l'arrivée critique au démarrage L'oseille la famille c'est c'que m'a dit un sage J'suis dépositaire d'un message J'vais leur faire c'que tu fais à ta meuf après l'massage J'suis Kratos dans la Grèce Antique Zéro rimes en toc encore moins d'romantique On a grandi bizarres la faute à la rue Ici peu ont les tocs mais tout l'monde a un tic C'est la frappe en direct j'reviens d'Nador C'est pas Christian mais Dieu qu'on adore J'ai jamais sucé c'est mon plus beau disque d'or Dans les tournées pas encore trouvé mon but J'me suis rendu compte qu'hommes ou femmes c'était des putes Tous les jours c'est combat y a jamais eu d'sparring 200 balles sur le compte on parlait de s'barrer Jeunes insouciants tu sais qu'on veut tout manger Ici c'est la vraie vie tmenik on va s'marrer J'compte plus dans la ville les coups d'pression qu'j'ai mis C'est paradoxal j'viens du nord mais j'suis hami Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Ils vis-ser des manos on sert les plus belles S'tu fais l'ordure tu finis à la poubelle On arrive déter' comme les frères Boughanem On t'laisse par-terre, eh c'est ça qu'on aime Augmente le son, fais kiffer les voisons C'pour On passe par l'17 et par Valenciennes On n'appelle pas l'17 on règle ça à l'ancienne Dans la rue y a plus d'règles mais pourtant ça saigne Mon fleh dans l' récupère ma Sacem Nouvel album, nouvelle récolte Ouais ouais c'est d'la bonne un p'tit teh tu décolles K.O Direct j'vise la pointe du menton On a un putain d'vécu ne crois pas qu'nous mentons S'tu fais flops sur flops tu vas pas toucher d'biff' J'enchaîne clopes sur clopes comme Tommy Shelby Bat les couilles d'tes conseils, bat les couilles d'ton avis On veut faire de l'oseille bien kiffer la vie Les condés m'ont pété après un coup d'tel' à vif Nous on rappe pour Gaza eux ils préfèrent Tel Aviv On sort du placard on sort pas d'Saint-Cyr Chasse le naturel il r'vient avec J'défends la cause comme Yasser Arafat Fais trembler l'olivier tu t'mangeras la rafale Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods</t>
+          <t>Lets go, Lets go Grrt Lets go, Lets go Ok j'ai déjà mis les bandes, rebeu, jm'échauffe pas Tête-à-tête avec toute ta bande, bitch me chauffe pas J'attends les échos du ghetto pour mettre les salopes à lamende Y a que la 'dre qui m'alimente khawf te sauve pas La Caille c'est pas TikTok tic-tac p'tite frappe J'ai des tactiques d'attaque j'suis pas dans les cheat-codes Jtire pas sur ls ambulances et jtape pas ls p'tites fiottes Jsuis toujours fidèle à mon opinel et à ma p'tite fiole J'ai les tibias durs, j'fais tomber les bambous Trapu jte take down, j'fais tomber les montagnes J'vais refaire la peinture, le corps suit le mental Sur le champ d'bataille au premier son des tambours J'te laisse par-terre fuck le procès Dans tous les cas y aura Fateh pour te crosser J'peux revenir d'un jour à l'autre comme Ragnar J'suis un rageux comme Ivar le désossé J'marche avec ceinture noire que personne sépare Sur le bitume que ça part en JJB sous JB Nos ruelles sont cruelles ici personne t'épargne On restera des ados remplis de haine, CJD T'auras pas l'temps d'dire Ajdimé Tu manges une rafale dans l'gilet Agité, Algérien d'bâtard obligé d'te giffler D'vant ton gang j'te localise j'y vais You might also like Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods On les tabasse les tartine les marave La dalle d'un seul homme peut exploser des barrages Par principe on t'arrange ou on t'arrache Mais wAllah qu'ça m'arrange quand j'laisse parler ma rage Suce à l'arrivée critique au démarrage L'oseille la famille c'est c'que m'a dit un sage J'suis dépositaire d'un message J'vais leur faire c'que tu fais à ta meuf après l'massage J'suis Kratos dans la Grèce Antique Zéro rimes en toc encore moins d'romantique On a grandi bizarres la faute à la rue Ici peu ont les tocs mais tout l'monde a un tic C'est la frappe en direct j'reviens d'Nador C'est pas Christian mais Dieu qu'on adore J'ai jamais sucé c'est mon plus beau disque d'or Dans les tournées pas encore trouvé mon but J'me suis rendu compte qu'hommes ou femmes c'était des putes Tous les jours c'est combat y a jamais eu d'sparring 200 balles sur le compte on parlait de s'barrer Jeunes insouciants tu sais qu'on veut tout manger Ici c'est la vraie vie tmenik on va s'marrer J'compte plus dans la ville les coups d'pression qu'j'ai mis C'est paradoxal j'viens du nord mais j'suis hami Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Ils vis-ser des manos on sert les plus belles S'tu fais l'ordure tu finis à la poubelle On arrive déter' comme les frères Boughanem On t'laisse par-terre, eh c'est ça qu'on aime Augmente le son, fais kiffer les voisons C'pour On passe par l'17 et par Valenciennes On n'appelle pas l'17 on règle ça à l'ancienne Dans la rue y a plus d'règles mais pourtant ça saigne Mon fleh dans l' récupère ma Sacem Nouvel album, nouvelle récolte Ouais ouais c'est d'la bonne un p'tit teh tu décolles K.O Direct j'vise la pointe du menton On a un putain d'vécu ne crois pas qu'nous mentons S'tu fais flops sur flops tu vas pas toucher d'biff' J'enchaîne clopes sur clopes comme Tommy Shelby Bat les couilles d'tes conseils, bat les couilles d'ton avis On veut faire de l'oseille bien kiffer la vie Les condés m'ont pété après un coup d'tel' à Fif Nous on rappe pour Gaza eux ils préfèrent Tel Aviv On sort du placard on sort pas d'Saint-Cyr Chasse le naturel il r'vient avec J'défends la cause comme Yasser Arafat Fais trembler l'olivier tu t'mangeras la rafale Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods Si t'es chaud on va derrière, boy Si t'es chaud on va derrière, boy Ça peut venir de derrière, boy Quand tu marches avec tes airpods</t>
         </is>
       </c>
     </row>
@@ -3812,7 +3812,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Les temps actuels déçoivent, nous remontent pas le moral Pourquoi on râle, observe mon constat visuel Vis nos vies, tu verras qu'y'a peu de joie dans les ruelles Et ce détail veut nous appâter dans le piège comme des ânes bâtés Si mon ssiste-gro il serait sicilien, je débiterais plus que Tati Je niquerais Carla et Cécilia ainsi que Rachida Dati Diakite, Belmadi m'ont dit de te dire qu'ils sont vénères Si je fais un gosse je l'appelle condi sur la vie de ma mère Cher monsieur le président va niquer tes morts Ton discours est trop amer dehwa va niquer ta mère Trop les crocs gros c'est le remake des Dents de la mer Quand y'a les keufs on dit tous qu'ils veulent nous mettre dans de la merde Cher monsieur le président va niquer tes morts Ton discours est trop amer je répète va niquer ta mère Là on a plus de repères donc on agit anormalement Faire le cher monsieur le président va niquer ta maman You might also like</t>
+          <t>Les temps actuels déçoivent, nous remontent pas le moral Pourquoi on râle, observe mon constat visuel Vis nos vies, tu verras qu'y'a peu de joie dans les ruelles Et ce détail veut nous appâter dans le piège comme des ânes bâtés Si mon ssiste-gro il serait sicilien, je débiterais plus que Tati Je niquerais Carla et Cécilia ainsi que Rachida Dati Diakite, Belmadi m'ont dit de te dire qu'ils sont vénères Si je fais un gosse je l'appelle condi sur la vie de ma mère Cher monsieur le président va niquer tes morts Ton discours est trop amer dehwa va niquer ta mère Trop les crocs gros c'est le remake des Dents de la mer Quand y'a les keufs on dit tous qu'ils veulent nous mettre dans de la merde Cher monsieur le président va niquer tes morts Ton discours est trop amer je répète va niquer ta mère Là on a plus de repères donc on agit anormalement Faire le cher monsieur le président va niquer ta maman Dans ma plume la situation je la résume Sans aucune substance sans diplôme et sans résine Que ceux qui écoutent désapprouvent ou s'en résignent Je m'adresse aux dirigeants et du doigt je les désigne De parent résident j'encule Sarkozy évident Le ghetto on vit dedans On est géman on dupe la juge le gouvernement le proc et la police aisément Aigrement on parle de tous ces faits gênants Cher monsieur le président je m'adresse à oit Dans ton trou de balle je mets le oid J'ai un bon fond à ton égard je peux que rester bad Eh ouais je m'en bats que les RG focalisent sur notre audimat C'est pas le cachot ni leurs poulets qui vont me traumatiser Bah qu'ils viennent c'est de la haine En tirer public on la baise du bout du stylo bic On taffe pour eux pour grailler des pépites You might also like D5 D4 eh chez nous y'a que des P4 Si on respecte Chirac c'est pour ces rottes ca sur les frégates Des payes de tortionnaire et ça sans même lever le petit oid Moi j'suis pas millionnaire dis ça aux stups en bas de chez oim Fais gaffe les gros poissons ils se font hameçonner par un anchois La rue ou la prison à nous de faire le bon choix Message à la secrétaire ta3 monsieur Sarkozy Dites lui qu'il nique sa mère sa sur son père et même sa cousine Le jacuzzi bah ce coup ci il est rempli de champagne Et à cette heure ci Carla elle suce pour 100 grammes Les gendarmes lancent des brigades prennent des clichés sur moi Car j'suis cramé comme un M3 garé à Clichy sous Bois Je m'en bats les couilles j'sors du Zoogataga Ça se douille pour du taga ça s'embrouille pour des thiaga Président de la République sérieux va niquer ta mama Je me verrai bien rouler un petit stick vers Ketama M'en bats les klawis que t'as libéré Bettancourt Pour l'instant je fume de la weed je pense à Mesrine vers Clignancourt Et je me dis que la roue tourne que Allah te le fera payer Et ses contrôles musclés ses réveils à coups de bélier Ze pequeño il vend de la drogue dure les microbes dégoûtent Béné Le grossiste c'est qu'une ordure le 36 c'est un poubellier Esse on t'arrache les dents en guise de mea culpa Cher monsieur président t'es qu'un hijo de puta</t>
         </is>
       </c>
     </row>
@@ -4220,7 +4220,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Non même pas, wAllah, cest juste la rue Cest rien, cest la rue WAllah, cest lamour et la mort SHK Cest compliqué des fois Avec ISK, ça s'passe toujours comme ça, tu connais La rue ma eu très tôt, j'suis tombé dans ses bras ah ouais Cest Dieu qui donne et cest lui qui reprendra En quelques secondes, j'me branche tout seul, en cinq minutes j'fais ta baraque J'fais du bien en f'sant du sale, ils appellent ça travail dArabe Avant dagir, j'pens aux répercussions, les bons, les mauvais tch Un texte, des punch', des percussions, j'te fais tourner la tête Cest nous la street, pas celle quils admirent, celle qui passe sur BFM la vraie Ils sont pas nets comme des immigrés qui vont voter FN Jai mes raisons et jai mes torts, pour eux, jai tort davoir raison Vaut mieux prévenir que guérir, jattends encore la guérison Le cur est sale, noirci par mes crasses, mes douleurs et mes peines ah ouais Dis-moi c'que cest la mort si la vie est une chienne On court après les sous, on en d'vient fou, on 'evient pas des ingrats jamais Guette la taille de leur langue et pas celle de leur bras Moi, j'suis l'même, frérot, jai pas changé, d'mande à la Rose ou Slime Cest les trophées qui cachent tous mes défauts, pas l'revers de la médaille You might also like Jai des frères en cavale et dautres en mandat de dépôt On a vendu l'bédo donc la vie nous a calcinés On est sorti du zoo mais on va pas chez le véto On fait pas les James Bond, 3.5.7, pas d'ciné Cest la rue qui ma eu, j'suis tombé dans ses bras Dans ma tête, cest la vendetta, il faut qu'j'me refasse tout d'suite Cest la rue qui ma eu, j'suis tombé dans ses bras En YZ ou en Clio 3, serein en pleine course-poursuite Arracheur de sacoches, le cauchemar des touristes La voiture cest Porsche, l'assurance, c'est est tous risques Eux, ils connaissent rien du tout mais ils aiment trop faire les puristes Nous, depuis p'tits, on sen bat les couilles et on fait courir la police Je me rappelle de la Santé, tordu comme la Tour de Pise À membrouiller avec les gradés, cette salope de directrice Quatre roues motrices comme Néo dans la matrice Fin d'carrière assez triste quand ça se termine à lOCRTIS Et ouais dahoua, cest la crise, à deux doigts d'chopper un ulcère Tout ce que je sais, cest quon finira poussière Intervention qui te massacrent à plusieurs Fais attention aux garçons, à n'pas finir comme un looser Cest le 7.7 et Belleville, un parigot et un banlieusard Tous les jours, j'fume de lherbe, la richesse est dans les arbres Petit conseil dArabe , ninvestis pas dans les armes Et si tu cherches la merde, tu périras par les armes Jai des frères en cavale et dautres en mandat de dépôt On a vendu l'bédo donc la vie nous a calcinés On est sorti du zoo mais on va pas chez le véto On fait pas les James Bond, 3.5.7, pas d'ciné Cest la rue qui ma eu, j'suis tombé dans ses bras Dans ma tête, cest la vendetta, il faut qu'j'me refasse tout d'suite Cest la rue qui ma eu, j'suis tombé dans ses bras En YZ ou en Clio 3, serein en pleine course-poursuite Jai des frères en cavale et dautres en mandat de dépôt On a vendu l'bédo donc la vie nous a calcinés On est sorti du zoo mais on va pas chez le véto On fait pas les James Bond, 3.5.7, pas d'ciné Cest la rue qui ma eu, j'suis tombé dans ses bras Dans ma tête, cest la vendetta, il faut qu'j'me refasse tout d'suite Cest la rue qui ma eu, j'suis tombé dans ses bras En YZ ou en Clio 3, serein en pleine course-poursuite</t>
+          <t>Non même pas, wAllah, cest juste la rue Cest rien, cest la rue WAllah, cest lamour et la mort SHK Cest compliqué des fois Avec ISK, ça s'passe toujours comme ça, tu connais La rue ma eu Très tôt, j'suis tombé dans ses bras Ah ouais Cest Dieu qui donne et cest lui qui reprendra En quelques secondes, j'me branche tout seul, en cinq minutes j'fais ta baraque J'fais du bien en f'sant du sale, ils appellent ça travail dArabe Ah ouais Avant dagir, j'pens aux répercussions, les bons, les mauvais tch Un texte, des punch', des percussions, j'te fais tourner la tête Cest nous la street, pas celle quils admirent, celle qui passe sur BFM la vraie Ils sont pas nets comme des immigrés qui vont voter FN Jai mes raisons et jai mes torts, pour eux, jai tort davoir raison Vaut mieux prévenir que guérir, jattends encore la guérison Mon cur est sale, noirci par mes crasses, mes douleurs et mes peines ah ouais Dis-moi c'que cest la mort si la vie est une chienne On court après les sous, on en d'vient fou, on d'vient pas des ingrats jamais Guette la taille de leur langue et pas celle de leur bras Moi, j'suis l'même, frérot, jai pas changé, d'mande à la Rose ou Slime Cest les trophées qui cachent tous mes défauts, pas l'revers de la médaille You might also like Jai des frères en cavale et dautres en mandat de dépôt On a vendu l'bédo donc la vie nous a calcinés On est sorti du zoo mais on va pas chez l'véto On fait pas les James Bond, 3.5.7, pas d'ciné Cest la rue qui ma eu, j'suis tombé dans ses bras Dans ma tête, cest la vendetta, il faut qu'j'me refasse tout d'suite Cest la rue qui ma eu, j'suis tombé dans ses bras En YZ ou en Clio 3, serein en pleine course-poursuite Arracheur de sacoches, le cauchemar des touristes La voiture, cest Porsche, l'assurance, c'est tous risques Eux, ils connaissent rien du tout mais ils aiment trop faire les puristes Nous, depuis p'tits, on sen bat les couilles et on fait courir la police Je me rappelle de la Santé, tordu comme la Tour de Pise À membrouiller avec les gradés, cette salope de directrice Quatre roues motrices comme Néo dans la matrice Fin d'carrière assez triste quand ça se termine à lOCRTIS Et ouais dahoua, cest la crise, à deux doigts d'chopper un ulcère Tout ce que je sais, cest quon finira poussière Intervention qui te massacrent à plusieurs Fais attention aux garçons, à n'pas finir comme un looser Cest le 7.7 et Belleville, un parigot et un banlieusard Tous les jours, j'fume de lherbe, la richesse est dans les arbres Petit conseil dArabe , ninvestis pas dans les armes Et si tu cherches la merde, tu périras par les armes Jai des frères en cavale et dautres en mandat de dépôt On a vendu l'bédo donc la vie nous a calcinés On est sorti du zoo mais on va pas chez le véto On fait pas les James Bond, 3.5.7, pas d'ciné Cest la rue qui ma eu, j'suis tombé dans ses bras Dans ma tête, cest la vendetta, il faut qu'j'me refasse tout d'suite Cest la rue qui ma eu, j'suis tombé dans ses bras En YZ ou en Clio 3, serein en pleine course-poursuite Jai des frères en cavale et dautres en mandat de dépôt On a vendu l'bédo donc la vie nous a calcinés On est sorti du zoo mais on va pas chez le véto On fait pas les James Bond, 3.5.7, pas d'ciné Cest la rue qui ma eu, j'suis tombé dans ses bras Dans ma tête, cest la vendetta, il faut qu'j'me refasse tout d'suite Cest la rue qui ma eu, j'suis tombé dans ses bras En YZ ou en Clio 3, serein en pleine course-poursuite</t>
         </is>
       </c>
     </row>
@@ -4470,12 +4470,12 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>RESTE TRANKIL</t>
+          <t>Représente Paname</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Hades Hasta la muerte la vida loca, wesh mon poto Ju-Ju-JuL et Yougataga Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde mais t'es tout seul Les p'tits ils ont grandi, maintenant ils ont les gants Fais pas l', fais pas l'tout seul La roue tourne, les poucaves, t'inquiète pas qu'elles vont payer C'est pour les braves comme les frères du Select à Montpellier C'est l'heure de manger, j'veux des crevettes pili-pili J'passe par Tanger voir David au Bling Bling Faut faire du chiffre, rien à foutre d'l'alphabet Sirote un Jack avec Hamid au Myah Bay, moi Ouais, j'veux des diamants avec beaucoup d'carats Big up , big up tout le Clara Au volant d'un Audi, matrixé J'sors le son même s'il est pas mixé Ici, tu peux t'prendre une balle à force de fixer Y a que quand les gens m'rendent parano que j'fais des fixettes Plein de big soucis, j't'avais dit d'faire comme ça et tu l'as pas fait comme Tony et Sosa Moi c'est anti cé'-cé' et société Moi j'suis pas là pour ces seins, j'sais qui j'étais You might also like Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde mais t'es tout seul Les p'tits ils ont grandi, maintenant ils ont les gants Fais pas l', fais pas l'tout seul Accélération tah Farès Chaïbi, moi Ouais, j'veux des millions à la banque Chaabi J'ai toujours c'qui faut, gros, même au tard-mi Et comme dit 3ami, faut vendre les kil' par mille J'ai pas l'temps d'en perdre vu qu'ça s'rachète pas On a beau viser l'ciel, on finira terre-par Les faux, j'ai pas l'temps pour eux, même Richard Millésé C'qu'ils rêvaient d'faire ? Pour nous c'est normalisé Viens on s'prend pas la tête, béa Après j'ai envie d'tout niquer comme dans GTA C'soir on va au restau', j'sors la CBA dans la sacoche CPA Plusieurs fumées, ça m'reconnaît au péage J'ai pas fumé, j'viens d'me lever, j'suis en serrage Faut voir qui t'es, toi, quand t'es là Faut voir qui t'aide quand c'est large Là j'suis avec Kakou, Danil, Chico et Houariz Ici ça part en couilles, à deux doigts d'faire mes valises C'est loin d'être merveilleux comme le pays d'Alice Les jeunes, ils font des dingueries parce qu'ils ont pas de khaliss Reste tranquille, j'ai pas la tête à ça Reste tranquille ou j'nique tout Reste tranquille, c'est Paris, c'est Marseille Reste tranquille, on n'a plus l'temps Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde mais t'es tout seul Les p'tits ils ont grandi, maintenant ils ont les gants Fais pas l', fais pas l'tout seul J'ai du trier pendant toutes ces années Ça fait mal au cur, des fois, on perd ses amis Va arroser si la fleur s'est fanée C'est qu'j'te considère vraiment si nous deux on s'allie On n'oublie pas les vrais et crois pas que l'on blague Big up Mister You, sous DP en promenade On n'oublie pas les vrais et crois pas que l'on blague Big up Mister You, sous DP en promenade Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde mais t'es tout seul Les p'tits ils ont grandi, maintenant ils ont les gants Fais pas l', fais pas l'tout seul Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde</t>
+          <t>Regarde pas ce que j'écris regarde plutôt ce que je décris À cause du shit j'ai maigri à cause des flics j'suis yégri Y'a pas de taf donc obligé de partir au bonchar 1000 euros par mois tu fais le triple si t'as du bon chav J'suis pas dans le mouv pas de boîte d'audi Q7 Le soir ça groove avec du shit de maudit cul sec C'est la nuit que se déviergent les petites pucelles Mets ta poteca à moins que tu veuilles pousser une poussette Tu veux du bon son bah vois les connaisseurs Toujours souriant mes soucis sont voilés comme mes soeurs OK fumeur de ... qui pousse à faire des grasses mat Faut que je me décrasse J'baise le FN et toute sa propagande Dis leur que je baise des blanches et que j'ai de la drogue à vendre Et puis des comptes à rendre chez moi c'est pas la thanksgiving Les petits sont armés et sache que c'est pas les cents qu'ils visent À 12 sur une pizza on a le sens du partage Paris c'est pas Ibiza y'a pas d'âge pour un paquetage Là c'est Abis je pense prétends pas voyou Mais tu vas bouffer des cailloux ça c'est pour la mixtape à YouYou might also like</t>
         </is>
       </c>
     </row>
@@ -4487,12 +4487,12 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>RETOUR AUX SOURCES</t>
+          <t>RESTE TRANKIL</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Esé Mister Yougataga Que des putains d'péripéties Marvelous Si, si 71 Beats Stef Becker beatmaker Le cercle d'amis s'est rétréci Derrière chaque homme, y a de grosses plaies ou des blessures bénignes Beaucoup d'questions, combien d'réponses s'cachent dans le livre délit ? Un gros joint d'herbe, un caillou d'crack, c'est pas le même délire Dans la vraie vie, c'est pas l riche qu'a lu le plus de livrs Y a pas un seul feignant ici qu'aura sa part de riz Nous on s'amuse pourtant y a pas, on tape des barres de rire La plupart de nos choix divers comporte une part de risques J'connais la plupart de mes s7ab depuis la garderie Me foutre en l'air, j'peux pas, pour un regard ça perd la vie Ne neige pas qu'en décembre, t'expulser, ils en meurent d'envie Depuis ma tendre enfance, j'rêve l'oseille des qataris J'mouille le maillot comme Hakimi, j'représente toujours Paris Bien sûr qu'on est réglo, on veut des billets mauves Jamais sans mes frérots, jamais sans mes loves J'arrache pas la SACEM, j'investis dans la drogue J'défouraille au mic comme si j'tirais sur des opps You might also like Laisse pas tes paluches sur le calibre Sweat à capuche, on fait nos valises Teste le produit, la drogue est balinaise Tout l'monde s'emballe, ils veulent être validés Barbe et qamis, la France panique On perd son il même dans une manif' Fumons-les tous tant qu'c'est d'la qualité On meurt en dragon ou en canidés Chaque jour que Dieu fait, j'essaye d'être mieux qu'la veille J'représente Belleville, j'fume le doré d'la veille Y a pas qu'les grands qui dealent, y a pas qu'les p'tits qui volent J'sais qu'les tarés rêveraient qu'j'finisse comme King Von J'ai fait disque d'roro et disque de platinum J'suis en train d'grailler un kebab sur rue des Batignolles Y a les condés qui passent et d'un coup qui s'arrêtent Ils veulent prendre un selfie, sur moi j'ai quatre barrettes J'suis en train d'sourire, j'ai failli courir J'me rappelle du proc', du réquisitoire, j'croyais qu'j'allais mourir Ils veulent nous pourrir, nan c'est pas pour rire Sous la pluie des balles tirée par la BAC, on aurait pu périr Laisse pas tes paluches sur le calibre Sweat à capuche, on fait nos valises Teste le produit, la drogue est balinaise Tout l'monde s'emballe, ils veulent être validés Barbe et qamis, la France panique On perd son il même dans une manif' Fumons-les tous tant qu'c'est d'la qualité On meurt en dragon ou en canidés Ils veulent m'enterrer, j'suis une graine qui pousse C'est la sécheresse et y a qu'mes larmes qui coulent J'aime trop écrire, même sur des feuilles qui coupent Ils aiment le teh mais c'est d'la merde c'qu'ils touchent Plus d'amitié dès qu'il s'agit d'gros sous On s'ra jugé pour tout c'qui sort d'nos bouches Le jour, on riait, c'est le soir qu'on doute Fonds-moi ton prix comme à cette poule qui couve Laisse pas tes paluches sur le calibre Sweat à capuche, on fait nos valises Teste le produit, la drogue est balinaise Tout l'monde s'emballe, ils veulent être validés Barbe et qamis, la France panique On perd son il même dans une manif' Fumons-les tous tant qu'c'est d'la qualité On meurt en dragon ou en canidés</t>
+          <t>Hades Hasta la muerte la vida loca, wesh mon poto Ju-Ju-JuL et Yougataga Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde mais t'es tout seul Les p'tits ils ont grandi, maintenant ils ont les gants Fais pas l', fais pas l'tout seul La roue tourne, les poucaves, t'inquiète pas qu'elles vont payer C'est pour les braves comme les frères du Select à Montpellier C'est l'heure de manger, j'veux des crevettes pili-pili J'passe par Tanger voir David au Bling Bling Faut faire du chiffre, rien à foutre d'l'alphabet Sirote un Jack avec Hamid au Myah Bay, moi Ouais, j'veux des diamants avec beaucoup d'carats Big up , big up tout le Clara Au volant d'un Audi, matrixé J'sors le son même s'il est pas mixé Ici, tu peux t'prendre une balle à force de fixer Y a que quand les gens m'rendent parano que j'fais des fixettes Plein de big soucis, j't'avais dit d'faire comme ça et tu l'as pas fait comme Tony et Sosa Moi c'est anti cé'-cé' et société Moi j'suis pas là pour ces seins, j'sais qui j'étais You might also like Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde mais t'es tout seul Les p'tits ils ont grandi, maintenant ils ont les gants Fais pas l', fais pas l'tout seul Accélération tah Farès Chaïbi, moi Ouais, j'veux des millions à la banque Chaabi J'ai toujours c'qui faut, gros, même au tard-mi Et comme dit 3ami, faut vendre les kil' par mille J'ai pas l'temps d'en perdre vu qu'ça s'rachète pas On a beau viser l'ciel, on finira terre-par Les faux, j'ai pas l'temps pour eux, même Richard Millésé C'qu'ils rêvaient d'faire ? Pour nous c'est normalisé Viens on s'prend pas la tête, béa Après j'ai envie d'tout niquer comme dans GTA C'soir on va au restau', j'sors la CBA dans la sacoche CPA Plusieurs fumées, ça m'reconnaît au péage J'ai pas fumé, j'viens d'me lever, j'suis en serrage Faut voir qui t'es, toi, quand t'es là Faut voir qui t'aide quand c'est large Là j'suis avec Kakou, Danil, Chico et Houariz Ici ça part en couilles, à deux doigts d'faire mes valises C'est loin d'être merveilleux comme le pays d'Alice Les jeunes, ils font des dingueries parce qu'ils ont pas de khaliss Reste tranquille, j'ai pas la tête à ça Reste tranquille ou j'nique tout Reste tranquille, c'est Paris, c'est Marseille Reste tranquille, on n'a plus l'temps Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde mais t'es tout seul Les p'tits ils ont grandi, maintenant ils ont les gants Fais pas l', fais pas l'tout seul J'ai du trier pendant toutes ces années Ça fait mal au cur, des fois, on perd ses amis Va arroser si la fleur s'est fanée C'est qu'j'te considère vraiment si nous deux on s'allie On n'oublie pas les vrais et crois pas que l'on blague Big up Mister You, sous DP en promenade On n'oublie pas les vrais et crois pas que l'on blague Big up Mister You, sous DP en promenade Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde mais t'es tout seul Les p'tits ils ont grandi, maintenant ils ont les gants Fais pas l', fais pas l'tout seul Nan, nan, nan, c'est plus comme avant Tu connais plein d'monde</t>
         </is>
       </c>
     </row>
@@ -4504,12 +4504,12 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Rien à perdre</t>
+          <t>RETOUR AUX SOURCES</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Wesh, prépare-toi Brams, Mister You C'est Mister You, ok roule un sdeh que jm'échauffe J'veux autant de sous que chez les pauvres que y'a autant de poux chez les chauves Woogataga les Jet-seteuse kiffent la wawa Les femmes courent à notre perte, r'garde c'qu'Adam a fait pour awa J'ai rien à perdre, ni à prendre des sous Du khaba qu'tu grattes, c'est pas ma came J'ai choisi la 'sique J'préfère rester classique Adidas, Asics Corrompez pas mon esprit lucide Mon talent j'le valide, kiffez ma 'sique, les gars ou faites vos valises J'suis un sérieux rival, comme vous j'ai la dalle Comme vous je mange mal, économisez les balles là c'est que le début du bal Yougatabrah, Rebeval, dresser le C'est le ghetto qui parle You, Brams, pas de soucis, à vie, on vous régale J'parle peu, j'suis efficace autant qu'un baveu J'tue le time chez No Time j'tiens pas à baver Toujours rebelle, mic en main dans le Woogataga, êtes-vous d'accord le beat j'le taba' You might also like Producteur, vendeur de coke, j'pisse sur les trois 6 Fuck les stups, sur l'rrain-té posté 24 sur 36 Le contraire de Kamini L'genre de mec qu'arrive faya en te-boi à 4h d'l'après minuit C'est Mister You, ok roule un sdeh que jm'échauffe Kiffez ma 'sique, les gars ou faites vos valises You, Brams, pas de soucis, à vie, on vous régale Fuck les stups, sur l'rrain-té posté 24 sur 36 C'est Mister You, ok roule un sdeh que jm'échauffe J'veux autant de sous que chez les pauvres que y'a autant de poux chez les chauves Woogataga les Jet-seteuse kiffent la wawa Les femmes courent à notre perte, r'garde c'qu'Adam a fait pour awa</t>
+          <t>Esé Mister Yougataga Que des putains d'péripéties Marvelous Si, si 71 Beats Stef Becker beatmaker Le cercle d'amis s'est rétréci Derrière chaque homme, y a de grosses plaies ou des blessures bénignes Beaucoup d'questions, combien d'réponses s'cachent dans le livre délit ? Un gros joint d'herbe, un caillou d'crack, c'est pas le même délire Dans la vraie vie, c'est pas l riche qu'a lu le plus de livrs Y a pas un seul feignant ici qu'aura sa part de riz Nous on s'amuse pourtant y a pas, on tape des barres de rire La plupart de nos choix divers comporte une part de risques J'connais la plupart de mes s7ab depuis la garderie Me foutre en l'air, j'peux pas, pour un regard ça perd la vie Ne neige pas qu'en décembre, t'expulser, ils en meurent d'envie Depuis ma tendre enfance, j'rêve l'oseille des qataris J'mouille le maillot comme Hakimi, j'représente toujours Paris Bien sûr qu'on est réglo, on veut des billets mauves Jamais sans mes frérots, jamais sans mes loves J'arrache pas la SACEM, j'investis dans la drogue J'défouraille au mic comme si j'tirais sur des opps You might also like Laisse pas tes paluches sur le calibre Sweat à capuche, on fait nos valises Teste le produit, la drogue est balinaise Tout l'monde s'emballe, ils veulent être validés Barbe et qamis, la France panique On perd son il même dans une manif' Fumons-les tous tant qu'c'est d'la qualité On meurt en dragon ou en canidés Chaque jour que Dieu fait, j'essaye d'être mieux qu'la veille J'représente Belleville, j'fume le doré d'la veille Y a pas qu'les grands qui dealent, y a pas qu'les p'tits qui volent J'sais qu'les tarés rêveraient qu'j'finisse comme King Von J'ai fait disque d'roro et disque de platinum J'suis en train d'grailler un kebab sur rue des Batignolles Y a les condés qui passent et d'un coup qui s'arrêtent Ils veulent prendre un selfie, sur moi j'ai quatre barrettes J'suis en train d'sourire, j'ai failli courir J'me rappelle du proc', du réquisitoire, j'croyais qu'j'allais mourir Ils veulent nous pourrir, nan c'est pas pour rire Sous la pluie des balles tirée par la BAC, on aurait pu périr Laisse pas tes paluches sur le calibre Sweat à capuche, on fait nos valises Teste le produit, la drogue est balinaise Tout l'monde s'emballe, ils veulent être validés Barbe et qamis, la France panique On perd son il même dans une manif' Fumons-les tous tant qu'c'est d'la qualité On meurt en dragon ou en canidés Ils veulent m'enterrer, j'suis une graine qui pousse C'est la sécheresse et y a qu'mes larmes qui coulent J'aime trop écrire, même sur des feuilles qui coupent Ils aiment le teh mais c'est d'la merde c'qu'ils touchent Plus d'amitié dès qu'il s'agit d'gros sous On s'ra jugé pour tout c'qui sort d'nos bouches Le jour, on riait, c'est le soir qu'on doute Fonds-moi ton prix comme à cette poule qui couve Laisse pas tes paluches sur le calibre Sweat à capuche, on fait nos valises Teste le produit, la drogue est balinaise Tout l'monde s'emballe, ils veulent être validés Barbe et qamis, la France panique On perd son il même dans une manif' Fumons-les tous tant qu'c'est d'la qualité On meurt en dragon ou en canidés</t>
         </is>
       </c>
     </row>
@@ -4521,12 +4521,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Rumoreo</t>
+          <t>Rien à perdre</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Si no lo veo, pues no lo creo Si no lo veo A-LA-LA-LA-LA-LA-LA-LA-LA M-M-M-M.D.L.R A-LA-LA-LA-LA-LA-LA-LA-LA Yougataga Y no me cuentes cuentos que a ti ya te han contao' Aquí se paga o el traslado no se hace Y sobre todo no acepto, nunca lo he fiao por fiarte a veces te la hacen Los niños hace días que yo los tengo montao' Y siguen metiendo lo trabajo Y por fajo tranquilo que yo ya he contao' Así que problemas rápido yo me mojo Si no lo veo nunca lo cojo A veces no lo cojo porque lo veo flojo Porque a veces pa que t coje y se moja Pero m lo tomo todo como un trabajo Me gustan los fajos en gomas Aunque a veces sean mejor en el banco Si no lo veo no es por ciego Y si no lo cojo no ha sido por manco You might also like Que se escuchen solo rumoreo Rumo-reo-reo-reo-reo-reo Rumoreo pero a ninguno lo veo No lo veo-veo-veo-veo-veo Rumoreo pero a ninguno a la cara A la cara-cara-cara-cara-cara-cara A la cara guapo y a la espalda to' feo Todo feo-feo-feo-feo-feo Joder, madre mía, no pasa nada tío Soy caliente, si, tu mujer tiene frío Nosotros en el coche, dime que tu eres mía Chivas por la noche, Sangría por el día Haciendo dinero la policía detrás mío Soy como todos los moros, primero la familia Gucci, Balenciaga, Prada, Louis Vuitton Escúchame guapa, te dedico esta canción No es un rumoreo, dinero te amo Dame la maleta, quemando la goma Si no lo veo, no lo creo Te lo juro hermano, eh, si Dame billete', te doy paquete Que se escuchen solo rumoreo Rumo-reo-reo-reo-reo-reo Rumoreo pero a ninguno lo veo No lo veo-veo-veo-veo-veo Rumoreo pero a ninguno a la cara A la cara-cara-cara-cara-cara-cara A la cara guapo y a la espalda to' feo Todo feo-feo-feo-feo-feo Buscando lo caro, lo gratuito Aunque yo era pequeñito Metido en lo' delito Aunque nunca fuese bonito Y nunca fui al instituto Pero más que ellos era listo En la calle siempre astuto Prefiero siempre estar suelto Buscando lo caro, lo gratuito Aunque yo era pequeñito Metido en lo' delito Aunque nunca fuese bonito Y nunca fui al instituto Pero más que ellos era listo En la calle siempre astuto Prefiero siempre estar suelto Si no lo veo-no lo veo-no lo veo-no lo veo-no lo veo-no lo veo-no lo veo Y no lo creo-no lo creo-no lo creo-no lo creo-no lo creo-no lo creo-no lo creo Si no lo veo-no lo veo-no lo veo-no lo veo-no lo veo-no lo veo-no lo veo Y no lo creo-no lo creo-no lo creo-no lo creo-no lo creo-no lo creo-no lo creo</t>
+          <t>Wesh, prépare-toi Brams, Mister You C'est Mister You, ok roule un sdeh que jm'échauffe J'veux autant de sous que chez les pauvres que y'a autant de poux chez les chauves Woogataga les Jet-seteuse kiffent la wawa Les femmes courent à notre perte, r'garde c'qu'Adam a fait pour awa J'ai rien à perdre, ni à prendre des sous Du khaba qu'tu grattes, c'est pas ma came J'ai choisi la 'sique J'préfère rester classique Adidas, Asics Corrompez pas mon esprit lucide Mon talent j'le valide, kiffez ma 'sique, les gars ou faites vos valises J'suis un sérieux rival, comme vous j'ai la dalle Comme vous je mange mal, économisez les balles là c'est que le début du bal Yougatabrah, Rebeval, dresser le C'est le ghetto qui parle You, Brams, pas de soucis, à vie, on vous régale J'parle peu, j'suis efficace autant qu'un baveu J'tue le time chez No Time j'tiens pas à baver Toujours rebelle, mic en main dans le Woogataga, êtes-vous d'accord le beat j'le taba' You might also like Producteur, vendeur de coke, j'pisse sur les trois 6 Fuck les stups, sur l'rrain-té posté 24 sur 36 Le contraire de Kamini L'genre de mec qu'arrive faya en te-boi à 4h d'l'après minuit C'est Mister You, ok roule un sdeh que jm'échauffe Kiffez ma 'sique, les gars ou faites vos valises You, Brams, pas de soucis, à vie, on vous régale Fuck les stups, sur l'rrain-té posté 24 sur 36 C'est Mister You, ok roule un sdeh que jm'échauffe J'veux autant de sous que chez les pauvres que y'a autant de poux chez les chauves Woogataga les Jet-seteuse kiffent la wawa Les femmes courent à notre perte, r'garde c'qu'Adam a fait pour awa</t>
         </is>
       </c>
     </row>
@@ -4538,12 +4538,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Salir ma cape</t>
+          <t>Rumoreo</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Non!Non!Non! Jpas eu le choix , que je le fasse il fallait Affronter tout les obstacles , a lheure ou tout les autres stagne Si!Si!Si! Tu connais pas, moi cest AL YASS MONEY RIDERZ Pour les connaisseurs Featuring nouvelle fraicheur !! Montréal doit accoucher De A.L sa spourrais 3heur on est pas couché Et si tu pense a mtoucher Tes mieu de ne pas mlouper Ou tu va tfaire cartoucher ARABIZER CAHLOUCHER Sa tapprendra a loucher Tu nous cherche on est partout Disparru comme Ssama-Ou Ya pas 36 solutions Sa va Ou Sa va pas La magouille La Khadma Ta pas dflouz ta pas dfemme Ta wallou ta pas dshab Mister You et Al Yass Fonceeee a 240 Javance en sachant Que le bien sappel GARBRIELLE kIBLISS sallonge dans sa chambre Enfance sans argent Jannonce le gagnant. al yass moenay riderz! La mise aux jeux est tentatrice et nous on est cerné d'dans La vie est un combat alors jla boxe et je serre les dents Encerclé dans une atmosphere sale et macabre Si j'étais super man pour qui j'irais salir ma cape.... Salir ma cape.... salir ma cape Pour qui j'irais salir ma cape.... Salir ma cape.... salir ma cape Pour qui j'irais salir ma cape Si j'étais super man pour qui j'irais salir ma cape! You might also likeAl Yass ''Montréal dois ACCOUCHER De AL SA S'POURRAIS 3h00 on est PAS COUCHER Et si tu pense A M'TOUCHER T'es mieu de ne PAS M'LOUPER Ou tu va t'faire CARTOUCHER ARABISÉCAHLOUCHER Sa t'apprendra A LOUCHER'' Mister You - ''I'm not in the biz ''I'M THE BIZ'' I Fuck the muthafuckin police with my muthafuckin homies sit the fuck down !!'' - ''A cet heur ci , j'crois bien que les jeux sont FAIT la jsuis FAIT j'suis REFAIT j'suis en train de vivre un compte de FÉE my name is YOU GA TA GA... Im not a muthafucker... I'm not a sucker, but I play soccer !!''</t>
+          <t>Si no lo veo, pues no lo creo Si no lo veo A-LA-LA-LA-LA-LA-LA-LA-LA M-M-M-M.D.L.R A-LA-LA-LA-LA-LA-LA-LA-LA Yougataga Y no me cuentes cuentos que a ti ya te han contao' Aquí se paga o el traslado no se hace Y sobre todo no acepto, nunca lo he fiao por fiarte a veces te la hacen Los niños hace días que yo los tengo montao' Y siguen metiendo lo trabajo Y por fajo tranquilo que yo ya he contao' Así que problemas rápido yo me mojo Si no lo veo nunca lo cojo A veces no lo cojo porque lo veo flojo Porque a veces pa que t coje y se moja Pero m lo tomo todo como un trabajo Me gustan los fajos en gomas Aunque a veces sean mejor en el banco Si no lo veo no es por ciego Y si no lo cojo no ha sido por manco You might also like Que se escuchen solo rumoreo Rumo-reo-reo-reo-reo-reo Rumoreo pero a ninguno lo veo No lo veo-veo-veo-veo-veo Rumoreo pero a ninguno a la cara A la cara-cara-cara-cara-cara-cara A la cara guapo y a la espalda to' feo Todo feo-feo-feo-feo-feo Joder, madre mía, no pasa nada tío Soy caliente, si, tu mujer tiene frío Nosotros en el coche, dime que tu eres mía Chivas por la noche, Sangría por el día Haciendo dinero la policía detrás mío Soy como todos los moros, primero la familia Gucci, Balenciaga, Prada, Louis Vuitton Escúchame guapa, te dedico esta canción No es un rumoreo, dinero te amo Dame la maleta, quemando la goma Si no lo veo, no lo creo Te lo juro hermano, eh, si Dame billete', te doy paquete Que se escuchen solo rumoreo Rumo-reo-reo-reo-reo-reo Rumoreo pero a ninguno lo veo No lo veo-veo-veo-veo-veo Rumoreo pero a ninguno a la cara A la cara-cara-cara-cara-cara-cara A la cara guapo y a la espalda to' feo Todo feo-feo-feo-feo-feo Buscando lo caro, lo gratuito Aunque yo era pequeñito Metido en lo' delito Aunque nunca fuese bonito Y nunca fui al instituto Pero más que ellos era listo En la calle siempre astuto Prefiero siempre estar suelto Buscando lo caro, lo gratuito Aunque yo era pequeñito Metido en lo' delito Aunque nunca fuese bonito Y nunca fui al instituto Pero más que ellos era listo En la calle siempre astuto Prefiero siempre estar suelto Si no lo veo-no lo veo-no lo veo-no lo veo-no lo veo-no lo veo-no lo veo Y no lo creo-no lo creo-no lo creo-no lo creo-no lo creo-no lo creo-no lo creo Si no lo veo-no lo veo-no lo veo-no lo veo-no lo veo-no lo veo-no lo veo Y no lo creo-no lo creo-no lo creo-no lo creo-no lo creo-no lo creo-no lo creo</t>
         </is>
       </c>
     </row>
@@ -4555,12 +4555,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Session freestyle</t>
+          <t>Salir ma cape</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Elle a vomi sa blanquette sur ma banquette Obligé d'mettre tempête les 3atay enquêtent l'hypothèque, saperlipopette T'es même pas foutu d'faire partir une plaquette J'suis sous neurones stimulateur, han Calibré, j'simule la peur Avant d'immaculer d'hémoglobine ton débardeur, han J'te remonte grâce au traceur, la chatte à ta sur Joue pas trop les mousquetaires wAllah étranglement coup du mousqueton Tu peux pas fumer ça c'est d'la mousse, le teh Fuck les suceurs, bouffe tes ongles J'roule des pétards et des mécaniques J'baise des panthères et des méga milfs J'rappe plus que toi c'est ma thématique Un seul couplet téma t'es ma bitch Tu jouais aux légo devant l'instit' On comptait plus de kichtas que d'élastiques Petit reste tranquille fais pas la street Fais le sportif l'entrepreneur fait l'artiste, han J'suis dans les astres, la voie lactée surnommée l'Hayce des Hayce Les yeux rouge sang, les idées noires comme J'm'endors sur la voix d'Arte avec une p'tite Kendale J'ai un nine tout neuf t'sais quoi J'crois qu'j'vais t'pull up chez toi Askip j'suis aud-ch c'est tout Les graille, les boire, j'sais pas J'ai jeté le Magnum Champagne écrire au cur d'une grasse campagne Moi j' j'sais comment les ingrats s'comportent La vérité dérange toujours le même qui en parle J'recompte pas, bordel de merde Gouvernement nous divise depuis le bord de mer Manipulent depuis piscine à débordement Des manuels à la file de nos bandes de merde Langue de Molière comme un prof de lettres Vieillit bien comme le vin Bordelais Ils sont là Aucun fils de putain ne m'apporte de l'aide Au bord de l'eau, verre de Crystal Poitrine généreuse pleine de lait J'suis au bord de l'eau j'ai moins peur de l'autre Et j'ai fini d'acheter ma villa en bord de mer Hasta la Muerte Hasta la Muerte Hasta la Muerte Hasta la Muerte H.L.M 2 dans les bacs', le 5 H.L.M 2 dans les bacs', le 5 H.L.M 2 dans les bacs', le 5 H.L.M 2 dans les bacs', le 5, le zinc' You might also like Ici tout l'monde a une guitare, pourtant, personne ne connait les Beatles Bac-térie veut brûler les étapes, han, le gérant jadis était guetteur T'entendras pas de Grrr-Grrr, quand j'enverrai l'missile sol-air J'essaie d'm'approcher du ciel mais le poids d'mes péchés me ramène vers le sol, hey Cimetière de mauvais pêchers vient pyramide de Benjamin Franklin J'marche avec les requins j'danse avec les loups rage et folie ne feront qu'un La bavette a frotté la police a frappé déféré au parquet j'fais couler son fond d'teint Algérien toujours effronté entrainé pour tenir le hebs et les temps pleins J'viens d'là où la drogue est un tremplin, chargeur est trop plein si tu portes te-plain H.L.M 2 dans les bacs', Yeah Hoe H.L.M 2 dans les bacs', Yeah Hoe H.L.M 2 dans les bacs', Yeah Hoe C'est l'retour du grand méchant You J'ai demandé le chemin d'la gloire, on m'a indiqué celui d'la gare Brr-t, Brr-t, hey J'ai demandé le chemin d'la gloire, on m'a indiqué celui d'la gare Gare au Tokarev chargé sous le manteau noir Tu vas ravaler ton venin par l'entonnoir Moi j'ai donné sans jamais recevoir j'les ai vus pleurer avant qu'il s'mette à pleuvoir Beaucoup de pouvoir mais très peu d'argent, ou beaucoup d'argent mais très peu de pouvoir Vallet baise la Reine pour devenir le Roi, le gladiateur sur un cheval de Troie J'sors le que-tru j'vais compter jusqu'à trois, Juste un scato de plus, viens chercher la merde dans une fosse septique petit grand c'est la même Sur le rain-té d'une démarche solennelle y a la mache en en lamelles Rebeu j'suis trop éclectique, j'ai le biff' et la fiche technique J'ai ché-cra pour ton vieille pute, que j'te cite Shakespire Ou qu'j'te vêtisse de chic textile sans la bulle bleue j'sais pas si j' Nébuleuse affiche Big Lemsi rafale pluvieuse peureuse ineptie Et je sais qu'j'les ai choqués Mon shooteur arrive en chuchotant fait crier le Grr-ah les jaloux vont s'affiner La canon du 11-43 te faire perdre le bras J'suis toujours là pour le fight, hey H.L.M 2 dans les bacs', han H.L.M 2 dans les bacs', hey H.L.M 2 dans les bacs', han, hey Dans quel tiroir tu vas ranger l'polichinelle On t'a vu garer voiture de sport t'introduire dans les stores deux jumelles full Chanel Poussé par mon père hermano j'récupère depuis qu'j'suis prépubère, dans l'four sa mère Algéria recherche de Martin Luther humain faire depuis l'pêcher originel Toujours vers solitaire, j'veux pilot' l'hélicoptère sans mis-per Une kichta deux kichtas j'récupère une , premier bikow qui donne un prix qui perd Wo, crochet du gauche plus d'lumière wo, sagittaire mal luné Tout droit sorti d'une tempête de sable noir on m'a trouvé dans un berceau sublunaire Pas de Subutex pas de S dans les sinus Est-ce que la vida vaut d'être vécue sans Urus la télévision j'ai la vision depuis la fusée folie passionnelle et métaphores en fusion J'ai refusé j'ai mes raisons d'envisager de les rafaler tous de les voler leurs maisons Méga Husstler, gros SLR, gros SLS dans l'parking Bingston, chargé comme Kinston marche avec des mercenaires en kaki Elle veut qu'j'lui paye tout elle m'prend pour un chien Trop curieuse elle m'demande combien j'prends pour un show Ces bikow pourraient sucer pour un shoot j'vais t'éclater si ces bikow t'prennent pour un chaud Elle sait très bien comment j'aime la vitesse elle dégueule à 320 sur les marées-chau' Les plus timides ils savent pas s'arrêter La sur les réchauds Big gauche pop Henni, j'vais pull up ces ops à la Henneni Pas très magnanime pas de bel3ani Big bad Hayce fait les bails 3ami À la base moi j'suis là pour déconner J'ai commencé dans l'parking avec les rats tu connais On mène la vie d'tess, tous les jours, c'est pas du comique Et puis c'est moi j'sais qu'j'suis l'acteur de c'que j'ai commis Eh 2020 c'est fini, qu'est-ce qu'il nous attend le kho Parce qu'on sait pas d'quoi s'ra fait demain dans c'monde c'est bizarre Ils nous envoient des virus, ils nous enferment au mitard Ils nous font croire que l'bonheur il s'est perdu vers Ibiza Mais bon on est que de passage, j'ai soufflé 26 bougies C'est loin l'époque où on dansaient tous sur du Boogie Woogie J'ai mon crâne sur l'appui-tête, y'a mon pied collé au plancher J'ai vu des mecs qui suivent des mecs et même quand ils vont pisser C'est quoi la tess sans le shit c'est quoi la vie sans les flics C'est quoi L'Allemand sans ses potos, sans sa famille, son équipe Walou, walou, walou, walou, 6.9 la trik ouais pelo Représentant d'la ville j'mets des buts comme El Fenomeno Dans ce fils de pute de rap j'suis v'nu avec les potos Si c'était 15 piges en arrière t'écouterais dans ta Punto Dans un 406 V6 ou une Golf IV R32 Avec ton pack de 12, d'l'a fume à 50 de beuh Pour toutes les cités Love and Peace, personne va nous diviser Avant l'showcase, la boule au ventre, ça passe pas quand j'vais pisser J'suis pas du côté d'la victime, j'suis du côté d'l'accusé C'est nous on t'nique et c'est toi qui repars cicatrices au visage Et aujourd'hui c'est une époque où tout l'monde il est bizarre Ils veulent le beurre, ils veulent le buzz, ils veulent la beurette qui passe Eh pelo moi j'veux m'en sortir et j'men balec' de qui reste Ouais c'est fini les promesses, tu peux rien quand t'agonises Mais toi j'sais pas, t'es un fils de traître comme Bafétimbi Gomis J'aime bien les khos qui ont des couilles et qui les portent en qamis Pas ceux qui jactent trop à tout l'monde et même à ta miss Tu nous connais, nous les ratus on la met trois fois ta mise J'mets mon tapis comme Bernard, rêvant d'une vie plus peinard C'est moi qui provoque toute l'action et j'te laisse tirer l'péno Chez nous y'a pas d'numéro 10 y'a qu'des numéros d'écrou Y'a des frérots qui deviennent fous et qui ramassent des mégots Ça vend du shit et d'la beuh, mélangés à l'ecstasy Ouais vers chez nous tu trouves de tout, le four c'est la pharmacie Du jaune teh la Seleção, enfume toi si t'es primaire Moi j'suis comme toi, j'ai fais d'la taule, enfermé tout un hiver</t>
+          <t>Non!Non!Non! Jpas eu le choix , que je le fasse il fallait Affronter tout les obstacles , a lheure ou tout les autres stagne Si!Si!Si! Tu connais pas, moi cest AL YASS MONEY RIDERZ Pour les connaisseurs Featuring nouvelle fraicheur !! Montréal doit accoucher De A.L sa spourrais 3heur on est pas couché Et si tu pense a mtoucher Tes mieu de ne pas mlouper Ou tu va tfaire cartoucher ARABIZER CAHLOUCHER Sa tapprendra a loucher Tu nous cherche on est partout Disparru comme Ssama-Ou Ya pas 36 solutions Sa va Ou Sa va pas La magouille La Khadma Ta pas dflouz ta pas dfemme Ta wallou ta pas dshab Mister You et Al Yass Fonceeee a 240 Javance en sachant Que le bien sappel GARBRIELLE kIBLISS sallonge dans sa chambre Enfance sans argent Jannonce le gagnant. al yass moenay riderz! La mise aux jeux est tentatrice et nous on est cerné d'dans La vie est un combat alors jla boxe et je serre les dents Encerclé dans une atmosphere sale et macabre Si j'étais super man pour qui j'irais salir ma cape.... Salir ma cape.... salir ma cape Pour qui j'irais salir ma cape.... Salir ma cape.... salir ma cape Pour qui j'irais salir ma cape Si j'étais super man pour qui j'irais salir ma cape! You might also likeAl Yass ''Montréal dois ACCOUCHER De AL SA S'POURRAIS 3h00 on est PAS COUCHER Et si tu pense A M'TOUCHER T'es mieu de ne PAS M'LOUPER Ou tu va t'faire CARTOUCHER ARABISÉCAHLOUCHER Sa t'apprendra A LOUCHER'' Mister You - ''I'm not in the biz ''I'M THE BIZ'' I Fuck the muthafuckin police with my muthafuckin homies sit the fuck down !!'' - ''A cet heur ci , j'crois bien que les jeux sont FAIT la jsuis FAIT j'suis REFAIT j'suis en train de vivre un compte de FÉE my name is YOU GA TA GA... Im not a muthafucker... I'm not a sucker, but I play soccer !!''</t>
         </is>
       </c>
     </row>
@@ -4572,12 +4572,12 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Solide</t>
+          <t>Session freestyle</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>Ouh, ouh J'fais réveiller des couche tards, éveiller des vrais Hmar , rhabiller des petites kehs avec un Q.I de calamar J'ai fait évader des taulards à l'Aide de mes cordes vocales Message à la racaille, qui vole et vend de la caille Incapable d'être réglo, tu tailles un jour avant que tu die Questions de principes l'argent n'est qu'un détail Personne se mouill pour une race de morts mais pour un frèr en or, on s'embrouille annule des représailles Ils ont étudié nos failles, 9-4 mentale, On fait des bébés parloir pour la condi parentale J'entends mes sons quand je cavale en promenade Je fais pas la resta, c'est d'égal à égal Les fouilles sont brutales, même pour une heja Que Dieu nous pardonne, nous aides à zapper illicite et chicha On est des mecs Hnine, d'origine, j'essaie de suivre le Dine Des fois je perds la main comme mel-Ja J'Marche plus sur des ufs mais sur des poussins, Je suis passé du Georges V au foyer des maliens Les portes du coeur sont nos yeux, mais on ne voit rien Sans la barakah ta richesse ne vaut rien La street nous a éduqués Agis comme un homme, on t'donne le respect On vient d'en bas réussite méritée Assume comme un homme et ne sois pas mauvais C'est pour les gars solide solide, Solide, solide Pour les gars solide solide, Solide, solide You might also like Je me rappelle de ma cavale quand mes potes m'esquivaient Quand je vois les yeux de mon fils bah faut que je le fasse kiffer Nan nan, crois pas que tout est carré des fois je me sens trop égaré Quand j'suis confiant avec une paire d'As madame la juge sort le carré Je passe en conseil de discipline, collège école primaire ensuite j'suis passé par Fleury ce putain de quartier disciplinaire Les panneaux de portes rempli de sel3a je revenais de Rotter d'un air serein Solo comme un mercenaire je me fait péter, m'en fou c'est rien En vrai ma mère à trop souffert je l'ai fait vieillir avant l'âge Non crois pas que je suis fier d'être dans ce putain d'engrenage Petit fréro fais gaffe à oi-t car l'amitié vaut que 30 euros Ton meilleur pote pourrait te fumer et venir pleurer à ton enterrement J'suis comme un mec qui sur j'ai serré que des paquets, bon la plupart c'était des connes niveau dialogue c'était claqué Darwa toi t'as perdu ta perle parce que t'aimais trop les rées-soi Aujourd'hui chacun sa merde chacun doit s'occuper de soi Hier ça parlait d'amour aujourd'hui ça parle de pension Cette folle t'as fait du shour, elle t'as fait boire sa potion Dans la rue, t'es le toubib, frérot, viens chez le patient La rue m'a pris du temps et m'a appris à être patient La street nous a éduqués Agis comme un homme on t'donne le respect On vient d'en bas réussite méritée Assume comme un homme et ne sois pas mauvais C'est pour les gars solide solide, solide solide Pour les gars solide solide, solide solide Reste polie polie, on a évité la folie, folie La sorcière est jolie jolie, à cause d'elle tu t'es ramolli-moli Reste polie polie, on à évité la folie, folie La sorcière est jolie jolie, à cause d'elle tu t'es ramolli-moli C'est pour les gars solide solide, solide solide Pour les gars solide solide, solide solide La street qui nous a éduqués Agis comme un homme on donne le respect On vient d'en bas réussite méritée Assume comme un homme et ne sois pas mauvais C'est pour les gars solide solide, Solide, solide Pour les gars solide solide, Solide, solide C'est pour les gars solide ma gueule, lourd les mecs de la street. En chaire et en shit Woogataga Quand on dofmait parterre ma gueule Roh2guerre On s'est cassé le dos sur le terrain Wallah Aujourd'hui palace, hélicoptère, jet privé ma gueule Rolls Royce, Limousine Ça bouge pas une oreille À l'aise en Clio 1 comme en Bentley Ta mère C'est la street gros en chaire et en shit wallah Accélération. Ça pars, ça reviens Accélération sur la A7 ta mère. hahaha Pour les Vrai de Vrai gros, ceux qui ont charbonnés qui ont tout donné Pas pour les girouettes faire Woogataga les gars C'est pour les hommes POUR LES GARS SOLIDE,SOLIDE !</t>
+          <t>Elle a vomi sa blanquette sur ma banquette Obligé d'mettre tempête les 3atay enquêtent l'hypothèque, saperlipopette T'es même pas foutu d'faire partir une plaquette J'suis sous neurones stimulateur, han Calibré, j'simule la peur Avant d'immaculer d'hémoglobine ton débardeur, han J'te remonte grâce au traceur, la chatte à ta sur Joue pas trop les mousquetaires wAllah étranglement coup du mousqueton Tu peux pas fumer ça c'est d'la mousse, le teh Fuck les suceurs, bouffe tes ongles J'roule des pétards et des mécaniques J'baise des panthères et des méga milfs J'rappe plus que toi c'est ma thématique Un seul couplet téma t'es ma bitch Tu jouais aux légo devant l'instit' On comptait plus de kichtas que d'élastiques Petit reste tranquille fais pas la street Fais le sportif l'entrepreneur fait l'artiste, han J'suis dans les astres, la voie lactée surnommée l'Hayce des Hayce Les yeux rouge sang, les idées noires comme J'm'endors sur la voix d'Arte avec une p'tite Kendale J'ai un nine tout neuf t'sais quoi J'crois qu'j'vais t'pull up chez toi Askip j'suis aud-ch c'est tout Les graille, les boire, j'sais pas J'ai jeté le Magnum Champagne écrire au cur d'une grasse campagne Moi j' j'sais comment les ingrats s'comportent La vérité dérange toujours le même qui en parle J'recompte pas, bordel de merde Gouvernement nous divise depuis le bord de mer Manipulent depuis piscine à débordement Des manuels à la file de nos bandes de merde Langue de Molière comme un prof de lettres Vieillit bien comme le vin Bordelais Ils sont là Aucun fils de putain ne m'apporte de l'aide Au bord de l'eau, verre de Crystal Poitrine généreuse pleine de lait J'suis au bord de l'eau j'ai moins peur de l'autre Et j'ai fini d'acheter ma villa en bord de mer Hasta la Muerte Hasta la Muerte Hasta la Muerte Hasta la Muerte H.L.M 2 dans les bacs', le 5 H.L.M 2 dans les bacs', le 5 H.L.M 2 dans les bacs', le 5 H.L.M 2 dans les bacs', le 5, le zinc' You might also like Ici tout l'monde a une guitare, pourtant, personne ne connait les Beatles Bac-térie veut brûler les étapes, han, le gérant jadis était guetteur T'entendras pas de Grrr-Grrr, quand j'enverrai l'missile sol-air J'essaie d'm'approcher du ciel mais le poids d'mes péchés me ramène vers le sol, hey Cimetière de mauvais pêchers vient pyramide de Benjamin Franklin J'marche avec les requins j'danse avec les loups rage et folie ne feront qu'un La bavette a frotté la police a frappé déféré au parquet j'fais couler son fond d'teint Algérien toujours effronté entrainé pour tenir le hebs et les temps pleins J'viens d'là où la drogue est un tremplin, chargeur est trop plein si tu portes te-plain H.L.M 2 dans les bacs', Yeah Hoe H.L.M 2 dans les bacs', Yeah Hoe H.L.M 2 dans les bacs', Yeah Hoe C'est l'retour du grand méchant You J'ai demandé le chemin d'la gloire, on m'a indiqué celui d'la gare Brr-t, Brr-t, hey J'ai demandé le chemin d'la gloire, on m'a indiqué celui d'la gare Gare au Tokarev chargé sous le manteau noir Tu vas ravaler ton venin par l'entonnoir Moi j'ai donné sans jamais recevoir j'les ai vus pleurer avant qu'il s'mette à pleuvoir Beaucoup de pouvoir mais très peu d'argent, ou beaucoup d'argent mais très peu de pouvoir Vallet baise la Reine pour devenir le Roi, le gladiateur sur un cheval de Troie J'sors le que-tru j'vais compter jusqu'à trois, Juste un scato de plus, viens chercher la merde dans une fosse septique petit grand c'est la même Sur le rain-té d'une démarche solennelle y a la mache en en lamelles Rebeu j'suis trop éclectique, j'ai le biff' et la fiche technique J'ai ché-cra pour ton vieille pute, que j'te cite Shakespire Ou qu'j'te vêtisse de chic textile sans la bulle bleue j'sais pas si j' Nébuleuse affiche Big Lemsi rafale pluvieuse peureuse ineptie Et je sais qu'j'les ai choqués Mon shooteur arrive en chuchotant fait crier le Grr-ah les jaloux vont s'affiner La canon du 11-43 te faire perdre le bras J'suis toujours là pour le fight, hey H.L.M 2 dans les bacs', han H.L.M 2 dans les bacs', hey H.L.M 2 dans les bacs', han, hey Dans quel tiroir tu vas ranger l'polichinelle On t'a vu garer voiture de sport t'introduire dans les stores deux jumelles full Chanel Poussé par mon père hermano j'récupère depuis qu'j'suis prépubère, dans l'four sa mère Algéria recherche de Martin Luther humain faire depuis l'pêcher originel Toujours vers solitaire, j'veux pilot' l'hélicoptère sans mis-per Une kichta deux kichtas j'récupère une , premier bikow qui donne un prix qui perd Wo, crochet du gauche plus d'lumière wo, sagittaire mal luné Tout droit sorti d'une tempête de sable noir on m'a trouvé dans un berceau sublunaire Pas de Subutex pas de S dans les sinus Est-ce que la vida vaut d'être vécue sans Urus la télévision j'ai la vision depuis la fusée folie passionnelle et métaphores en fusion J'ai refusé j'ai mes raisons d'envisager de les rafaler tous de les voler leurs maisons Méga Husstler, gros SLR, gros SLS dans l'parking Bingston, chargé comme Kinston marche avec des mercenaires en kaki Elle veut qu'j'lui paye tout elle m'prend pour un chien Trop curieuse elle m'demande combien j'prends pour un show Ces bikow pourraient sucer pour un shoot j'vais t'éclater si ces bikow t'prennent pour un chaud Elle sait très bien comment j'aime la vitesse elle dégueule à 320 sur les marées-chau' Les plus timides ils savent pas s'arrêter La sur les réchauds Big gauche pop Henni, j'vais pull up ces ops à la Henneni Pas très magnanime pas de bel3ani Big bad Hayce fait les bails 3ami À la base moi j'suis là pour déconner J'ai commencé dans l'parking avec les rats tu connais On mène la vie d'tess, tous les jours, c'est pas du comique Et puis c'est moi j'sais qu'j'suis l'acteur de c'que j'ai commis Eh 2020 c'est fini, qu'est-ce qu'il nous attend le kho Parce qu'on sait pas d'quoi s'ra fait demain dans c'monde c'est bizarre Ils nous envoient des virus, ils nous enferment au mitard Ils nous font croire que l'bonheur il s'est perdu vers Ibiza Mais bon on est que de passage, j'ai soufflé 26 bougies C'est loin l'époque où on dansaient tous sur du Boogie Woogie J'ai mon crâne sur l'appui-tête, y'a mon pied collé au plancher J'ai vu des mecs qui suivent des mecs et même quand ils vont pisser C'est quoi la tess sans le shit c'est quoi la vie sans les flics C'est quoi L'Allemand sans ses potos, sans sa famille, son équipe Walou, walou, walou, walou, 6.9 la trik ouais pelo Représentant d'la ville j'mets des buts comme El Fenomeno Dans ce fils de pute de rap j'suis v'nu avec les potos Si c'était 15 piges en arrière t'écouterais dans ta Punto Dans un 406 V6 ou une Golf IV R32 Avec ton pack de 12, d'l'a fume à 50 de beuh Pour toutes les cités Love and Peace, personne va nous diviser Avant l'showcase, la boule au ventre, ça passe pas quand j'vais pisser J'suis pas du côté d'la victime, j'suis du côté d'l'accusé C'est nous on t'nique et c'est toi qui repars cicatrices au visage Et aujourd'hui c'est une époque où tout l'monde il est bizarre Ils veulent le beurre, ils veulent le buzz, ils veulent la beurette qui passe Eh pelo moi j'veux m'en sortir et j'men balec' de qui reste Ouais c'est fini les promesses, tu peux rien quand t'agonises Mais toi j'sais pas, t'es un fils de traître comme Bafétimbi Gomis J'aime bien les khos qui ont des couilles et qui les portent en qamis Pas ceux qui jactent trop à tout l'monde et même à ta miss Tu nous connais, nous les ratus on la met trois fois ta mise J'mets mon tapis comme Bernard, rêvant d'une vie plus peinard C'est moi qui provoque toute l'action et j'te laisse tirer l'péno Chez nous y'a pas d'numéro 10 y'a qu'des numéros d'écrou Y'a des frérots qui deviennent fous et qui ramassent des mégots Ça vend du shit et d'la beuh, mélangés à l'ecstasy Ouais vers chez nous tu trouves de tout, le four c'est la pharmacie Du jaune teh la Seleção, enfume toi si t'es primaire Moi j'suis comme toi, j'ai fais d'la taule, enfermé tout un hiver</t>
         </is>
       </c>
     </row>
@@ -4589,12 +4589,12 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Son coeur (Marvin - Coktail de Rue)</t>
+          <t>Solide</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Quand les anges brillent dans le ciel le diable s'agite sur le trottoir C'est trop tard le mal fait, me bouleverse la haine est gratuite J'entend des coup d'feu, les âmes quittent leurs corps et gravitent On navigue, on parle d'million virtuel avec le ventre vide C'est Koh-Lanta j'part en expédition même sans vivre Moi jespère vivre jusquà la destruction de Belleville J'relativise, vise pas la tête ou c'est lhémorragie Je réagis, kill plutôt le mic comme Bilel Nadjib Quand on m'dit coronaire j'sais que c'est d'un mort qu'il s'agit Quand j'voit ma mère en pleur je ne voit pas le drapeau qui s'agite Laisser pour compte, toujours les même qui tombe pour coke La même misère en bas j'te refait le monde avec un cône Très désorienté, j'veux sortir en indé Je n'm'interdit plus rien faut faire du chiffre sur le terrain Indigent, on rêve de faire sauter la diligence Baiser les dirigeant qui nous croient en manque d'intelligence On rêve d'un harem, niquer la meuf d'Pharrell Et on s'questionne, Dieu, comment a tu fait un monde pareil ? On aimes toucher et coucher, regarder l'coucher su soleil Approcher nos rêve, pouvoir s'réveiller du sommeil J'aime, la vie qu'je mène même si c'est l'bordel Avec la volonté tout sa mènera au bord d'la mer Bref, j'réve, d'authentifier mon existence Mais le rap est pris pour cible comparé pour délinquance Quand j'pense au disparu, a la beuh ou au charrue A ses kilo d'coco qui sont écouler dans nos rue La Russie n'est qu'a deux pat sais-tu que la roulette aussi On rêve dêtre docile, tout autour tout est nocif On signe d'un Z avec un zeste de poésie Souvent on s'arme pour pas laisser notre peau ici Donc ? la vie en bas elle nous sidère On s'croit dans count striker et on aime tirer au ? A force de traîner on s'y perd Dans nos peine, on s'y baigne, on fera péter ton sasse au décibel On ressasse le bon et l'mauvais, on chekera José Bové Le bonheur n'est pas loin il est difficile a trouver Éprouver par cette vie y a comme un gout de mélancolie J'suis seul sur ma colline moi et mon taux d'alcoolémie J'les laisse me blesser, croire qu'ils mont mis en laisse Mais la rue m'a plus appris que leur Pythagore est a l'est Donc jespère vivre libre tant qu'je respire J'vie a Belleville de mon ghetto je m'inspire M'en méfie comme de la peste, de la belle, de la bête J'reste humble car je perdrai si j'me la pète La perte est proche le diable appel et on décroche On veux s'la faire pépère jusqu'au dernier coup de cross On a toujours les crocs, on partira sans un centimes Si j'doit cané demain Younes m'enterra en Guyane Cest gentiment que je t'exprime juste un ressentiment Garde le pour toi lEurope n'est pas mon continent 22 ans, maintenant, encore en vie c'est étonnant J'aide toujours mon prochain car j'aime recevoir en donnant J'suis précis, j'ai des principes j'ai surtout des valeur De l'honneur mais, s'il vont tous au sud j'irai au Nord Mon cur renferme tant d'haine et de joie a la fois Père, je pense a toi je l'jure Aussi fort que j'pense au poto You A la renaissance Pataya, linnocence des Ghetto Youth On court vers un avenir surement incertain Pour un ? j'peu m'prendre une balle comme a Verdun Et j'souhaite remplacé l'sky J'souhaite, contre les verre d'eau Préserver ma famille de la dépendance et de l'overdose J'ose faire parler de moi d'effrayer la chronique J'reste pas là sans bouger le cul poser sur le granit C'est grave, ? nous interdit pas au dicave Chaque journée ? je cotoie le handicap Des fois mon coeur gueule me dit de n'pas baisser les bras Qu'un jour tout se payera Et nique sa mère l'jour où on se sépare J'te dit à taleur mais on sais pas De l'autre coté d'la rue je peux me prendre un coup d'barre Partir, y'a 1000 kalash de raisons d'mourir Ma mère, rien ne remplace son sourireYou might also like</t>
+          <t>Ouh, ouh J'fais réveiller des couche tards, éveiller des vrais Hmar , rhabiller des petites kehs avec un Q.I de calamar J'ai fait évader des taulards à l'Aide de mes cordes vocales Message à la racaille, qui vole et vend de la caille Incapable d'être réglo, tu tailles un jour avant que tu die Questions de principes l'argent n'est qu'un détail Personne se mouill pour une race de morts mais pour un frèr en or, on s'embrouille annule des représailles Ils ont étudié nos failles, 9-4 mentale, On fait des bébés parloir pour la condi parentale J'entends mes sons quand je cavale en promenade Je fais pas la resta, c'est d'égal à égal Les fouilles sont brutales, même pour une heja Que Dieu nous pardonne, nous aides à zapper illicite et chicha On est des mecs Hnine, d'origine, j'essaie de suivre le Dine Des fois je perds la main comme mel-Ja J'Marche plus sur des ufs mais sur des poussins, Je suis passé du Georges V au foyer des maliens Les portes du coeur sont nos yeux, mais on ne voit rien Sans la barakah ta richesse ne vaut rien La street nous a éduqués Agis comme un homme, on t'donne le respect On vient d'en bas réussite méritée Assume comme un homme et ne sois pas mauvais C'est pour les gars solide solide, Solide, solide Pour les gars solide solide, Solide, solide You might also like Je me rappelle de ma cavale quand mes potes m'esquivaient Quand je vois les yeux de mon fils bah faut que je le fasse kiffer Nan nan, crois pas que tout est carré des fois je me sens trop égaré Quand j'suis confiant avec une paire d'As madame la juge sort le carré Je passe en conseil de discipline, collège école primaire ensuite j'suis passé par Fleury ce putain de quartier disciplinaire Les panneaux de portes rempli de sel3a je revenais de Rotter d'un air serein Solo comme un mercenaire je me fait péter, m'en fou c'est rien En vrai ma mère à trop souffert je l'ai fait vieillir avant l'âge Non crois pas que je suis fier d'être dans ce putain d'engrenage Petit fréro fais gaffe à oi-t car l'amitié vaut que 30 euros Ton meilleur pote pourrait te fumer et venir pleurer à ton enterrement J'suis comme un mec qui sur j'ai serré que des paquets, bon la plupart c'était des connes niveau dialogue c'était claqué Darwa toi t'as perdu ta perle parce que t'aimais trop les rées-soi Aujourd'hui chacun sa merde chacun doit s'occuper de soi Hier ça parlait d'amour aujourd'hui ça parle de pension Cette folle t'as fait du shour, elle t'as fait boire sa potion Dans la rue, t'es le toubib, frérot, viens chez le patient La rue m'a pris du temps et m'a appris à être patient La street nous a éduqués Agis comme un homme on t'donne le respect On vient d'en bas réussite méritée Assume comme un homme et ne sois pas mauvais C'est pour les gars solide solide, solide solide Pour les gars solide solide, solide solide Reste polie polie, on a évité la folie, folie La sorcière est jolie jolie, à cause d'elle tu t'es ramolli-moli Reste polie polie, on à évité la folie, folie La sorcière est jolie jolie, à cause d'elle tu t'es ramolli-moli C'est pour les gars solide solide, solide solide Pour les gars solide solide, solide solide La street qui nous a éduqués Agis comme un homme on donne le respect On vient d'en bas réussite méritée Assume comme un homme et ne sois pas mauvais C'est pour les gars solide solide, Solide, solide Pour les gars solide solide, Solide, solide C'est pour les gars solide ma gueule, lourd les mecs de la street. En chaire et en shit Woogataga Quand on dofmait parterre ma gueule Roh2guerre On s'est cassé le dos sur le terrain Wallah Aujourd'hui palace, hélicoptère, jet privé ma gueule Rolls Royce, Limousine Ça bouge pas une oreille À l'aise en Clio 1 comme en Bentley Ta mère C'est la street gros en chaire et en shit wallah Accélération. Ça pars, ça reviens Accélération sur la A7 ta mère. hahaha Pour les Vrai de Vrai gros, ceux qui ont charbonnés qui ont tout donné Pas pour les girouettes faire Woogataga les gars C'est pour les hommes POUR LES GARS SOLIDE,SOLIDE !</t>
         </is>
       </c>
     </row>
@@ -4606,12 +4606,12 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Suce mes boules</t>
+          <t>Son coeur (Marvin - Coktail de Rue)</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Suce ma bite Lèche mes boules Lèche ma bite Suce mes boules Suce mes boules, lèche ma bite Lèche ma bite, suce mes boules Suce mes boules, suce mes boules Lèche ma bite, lèche ma bite Lèche mes boules, lèche mes boules Suce ma bite, suce ma bite Suce ma bite, lèch mes boules, lèche ms boules C'était pas prévu au programme Mais tu vas cé-su nos godasses Car c'est du trop haut de gamme Jonathan H la mitrailleuse Envoie des rimes mafieuses Et fourre des filles hargneuses Taille-moi une pipe sale chieuse si t'as la gueule de Nathalie Baye Laisse-moi faire mes bails pour que la famille graille salope Trop dhéroïnomanes et de ravissantes demoiselles Cocaïnomane transforme leurs narines en toilettes J'décapite ta tête de pute comme Marie-Antoinette C'est rapide atteste le but, gros, j'arrive en touareg J'te fascine en trois seize, que j'manigance moi-même encore Qu'est-ce que tu crois, mec encore, lèche mes noisettes encore Je me fais contrôler par des blondinets J'ai combiné la drogue, l'alcool et j'ai sacrifié mon dîner J'suis pas allé à la fac mais à la Fnac J'suis pas rasé sale macaque, j'passe à l'attaque ! You might also like Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Avec ma queue j'fais c'que j'veux alors tu m'laisses ball Avec ma queue, on joue pas au billard on fait du baseball Caresse la batte, mets toi à quatre pattes et j'tire au paintball Avec mon gun tu passes aux assiettes si t'as pas d'bol Avec ma gueule, ma gueule, t'es sur d'être mis sur l'té-co Fuck la plage, j'veux un château avec une vue sur l'ghetto Avec Michael, j'gueule, le mic', rime avec Tyson Devant lautre Michael, jrajoute Daniels pour que Jackson Wilkinson tranchants dès lors où la perquise sonne Jredoute personne à part les shtars de peur qu'ils m'saignent Jsuis pisté par les pe-stu, en X5 Le micro j'le fais bler-trem, il attrape Parkinson Le crack imprègne mes disques sans passer par Kingston Si deux PD préméditent, c'est 100 pour qu'ils s'donnent Armé dun uzi, l'esprit lucide quand les gens rentrent solo Si la vie s'rait une pute, ouais, je l'appellerais Sharon Stone Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Ce son, cest comme cette putain de chaine cryptée la nuit le samedi Que des fous, que des loups même prêts à ler-vio le cro-mi Le 20ème, cest mon réseau, les keufs nous té-ma avec trop d'ces-vi Va dire à ces batards qu'on restera là sans les servir J'vais sévir sur l'beat, appelle ça violence gratuite J'vais te buter sans but pourquoi pas pécho des thunes Si j'pécho une pute ce qu'on fera, c'est du bite à bouche On fuck les dirigeants Français en glissant capotes dans l'urne Ils disent tes lyrics sont dun vulgaire Fermes ta gueule, cest soit ça ou bien ma bulle dair Dans ta bouche, ton crew Vas-y bouge ou tauras la même impression quaprès-avoir laissé lsavon dans la douche Mon équipe, te liquide, te rend fou, comme deux shits Eh reste cool face au futur leader Nouvelle école, Alcailllou, jcrois que tas vu la couleur Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous</t>
+          <t>Quand les anges brillent dans le ciel le diable s'agite sur le trottoir C'est trop tard le mal fait, me bouleverse la haine est gratuite J'entend des coup d'feu, les âmes quittent leurs corps et gravitent On navigue, on parle d'million virtuel avec le ventre vide C'est Koh-Lanta j'part en expédition même sans vivre Moi jespère vivre jusquà la destruction de Belleville J'relativise, vise pas la tête ou c'est lhémorragie Je réagis, kill plutôt le mic comme Bilel Nadjib Quand on m'dit coronaire j'sais que c'est d'un mort qu'il s'agit Quand j'voit ma mère en pleur je ne voit pas le drapeau qui s'agite Laisser pour compte, toujours les même qui tombe pour coke La même misère en bas j'te refait le monde avec un cône Très désorienté, j'veux sortir en indé Je n'm'interdit plus rien faut faire du chiffre sur le terrain Indigent, on rêve de faire sauter la diligence Baiser les dirigeant qui nous croient en manque d'intelligence On rêve d'un harem, niquer la meuf d'Pharrell Et on s'questionne, Dieu, comment a tu fait un monde pareil ? On aimes toucher et coucher, regarder l'coucher su soleil Approcher nos rêve, pouvoir s'réveiller du sommeil J'aime, la vie qu'je mène même si c'est l'bordel Avec la volonté tout sa mènera au bord d'la mer Bref, j'réve, d'authentifier mon existence Mais le rap est pris pour cible comparé pour délinquance Quand j'pense au disparu, a la beuh ou au charrue A ses kilo d'coco qui sont écouler dans nos rue La Russie n'est qu'a deux pat sais-tu que la roulette aussi On rêve dêtre docile, tout autour tout est nocif On signe d'un Z avec un zeste de poésie Souvent on s'arme pour pas laisser notre peau ici Donc ? la vie en bas elle nous sidère On s'croit dans count striker et on aime tirer au ? A force de traîner on s'y perd Dans nos peine, on s'y baigne, on fera péter ton sasse au décibel On ressasse le bon et l'mauvais, on chekera José Bové Le bonheur n'est pas loin il est difficile a trouver Éprouver par cette vie y a comme un gout de mélancolie J'suis seul sur ma colline moi et mon taux d'alcoolémie J'les laisse me blesser, croire qu'ils mont mis en laisse Mais la rue m'a plus appris que leur Pythagore est a l'est Donc jespère vivre libre tant qu'je respire J'vie a Belleville de mon ghetto je m'inspire M'en méfie comme de la peste, de la belle, de la bête J'reste humble car je perdrai si j'me la pète La perte est proche le diable appel et on décroche On veux s'la faire pépère jusqu'au dernier coup de cross On a toujours les crocs, on partira sans un centimes Si j'doit cané demain Younes m'enterra en Guyane Cest gentiment que je t'exprime juste un ressentiment Garde le pour toi lEurope n'est pas mon continent 22 ans, maintenant, encore en vie c'est étonnant J'aide toujours mon prochain car j'aime recevoir en donnant J'suis précis, j'ai des principes j'ai surtout des valeur De l'honneur mais, s'il vont tous au sud j'irai au Nord Mon cur renferme tant d'haine et de joie a la fois Père, je pense a toi je l'jure Aussi fort que j'pense au poto You A la renaissance Pataya, linnocence des Ghetto Youth On court vers un avenir surement incertain Pour un ? j'peu m'prendre une balle comme a Verdun Et j'souhaite remplacé l'sky J'souhaite, contre les verre d'eau Préserver ma famille de la dépendance et de l'overdose J'ose faire parler de moi d'effrayer la chronique J'reste pas là sans bouger le cul poser sur le granit C'est grave, ? nous interdit pas au dicave Chaque journée ? je cotoie le handicap Des fois mon coeur gueule me dit de n'pas baisser les bras Qu'un jour tout se payera Et nique sa mère l'jour où on se sépare J'te dit à taleur mais on sais pas De l'autre coté d'la rue je peux me prendre un coup d'barre Partir, y'a 1000 kalash de raisons d'mourir Ma mère, rien ne remplace son sourireYou might also like</t>
         </is>
       </c>
     </row>
@@ -4623,12 +4623,12 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Summer Zoo</t>
+          <t>Suce mes boules</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>J'touche pas aux vlo-tra j'baise qu'les go sans triques Je suis, comment vous dites ? égocentrique Sucer des bites, c'est pas autoriser J'ai écris c'texte à Fleury, à Fresnes j'vais le remastériser Vaporisez les billets, comme à ça ils auront une odeur Les 3ineurs s'que j'sais c'est qu'ils volent mieux qu'Harry Potter Un répondeur, ça sert à vesqui les gens Tu veux qu'on dorme ? t'es folle, écarte un peu les jambes Le feu d'l'amour on l'éteint pas en l'attisant Houbi, t'a un regard traumatisant Zebi, à la barre j'fais l'mec til-gen Mais l'juge s'bâtard il veut m'mettre 10 ans Woogataga Belleville grosse dédicace Miss reste en chatte et graille des whiskas Y'a l'36 postiché en bas d'la house Moi, j'm'en fiche là j'suis en train d'danser sur d'la house What in the world is a girl to do? When in this smokey place I only see you Was far away when you caught my eye You've brought me back and now you're making me high I was alone out there, with no one else around Now I've fallen for you gataga and there's no coming down Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes What can I do? I'm looking right at you This feeling is all new, I want you addicted to me Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes What can I do? I'm looking right at you This feeling is all new, I want you addicted to me You might also like C'soir évite les embrouilles même si on t'parles mal C'est la fête soit cool paye un verre au barman Sur la piste y'a qu'des missiles, c'est la guerre mondiale J'les aimes fines et sportives genre Sophie Thalmann C'est pour ceux et aussi celles qu'on pris la vie sur un coup d'tête Les voyous à la table qui enchaîne les bouteilles C'est pour Steve, Mamadou et Be-be-bechir J'ai entendu un pull up, pull up ça dé-dé-déchire C'est l'94 gataga connexion, Rap de barj' en action pour les braves On fais du son pure en illicite Marre d'voir XXX XXX Malfrat dans la boite ça peut douiller Gare aux mésaventure si t'espérais me fouiller J'ai le biff dans les fouilles si y'a heja J'vais faire des dégâts avec poto Tadja Eh excuse moi, eh demoiselle, wesh t'es sérieuse ? eh wallah j'vais t'charrier hey Anorexique 44 kilos poids net Tu fais pas d'pipi tu sniff dans les toilettes Gucci, Versace, Dolce Gabanna A la bouche un gare-ci tah la Havana Faya sous vodka j'préfère le whisky Suivi d'une lahsa d'Monica Lewinsky I was alone out there, with no one else around Now I've fallen for you gataga and there's no coming down Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes What can I do? I'm looking right at you This feeling is all new, I want you addicted to me Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes What can I do? I'm looking right at you This feeling is all new, I want you addicted to me Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes</t>
+          <t>Suce ma bite Lèche mes boules Lèche ma bite Suce mes boules Suce mes boules, lèche ma bite Lèche ma bite, suce mes boules Suce mes boules, suce mes boules Lèche ma bite, lèche ma bite Lèche mes boules, lèche mes boules Suce ma bite, suce ma bite Suce ma bite, lèch mes boules, lèche ms boules C'était pas prévu au programme Mais tu vas cé-su nos godasses Car c'est du trop haut de gamme Jonathan H la mitrailleuse Envoie des rimes mafieuses Et fourre des filles hargneuses Taille-moi une pipe sale chieuse si t'as la gueule de Nathalie Baye Laisse-moi faire mes bails pour que la famille graille salope Trop dhéroïnomanes et de ravissantes demoiselles Cocaïnomane transforme leurs narines en toilettes J'décapite ta tête de pute comme Marie-Antoinette C'est rapide atteste le but, gros, j'arrive en touareg J'te fascine en trois seize, que j'manigance moi-même encore Qu'est-ce que tu crois, mec encore, lèche mes noisettes encore Je me fais contrôler par des blondinets J'ai combiné la drogue, l'alcool et j'ai sacrifié mon dîner J'suis pas allé à la fac mais à la Fnac J'suis pas rasé sale macaque, j'passe à l'attaque ! You might also like Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Avec ma queue j'fais c'que j'veux alors tu m'laisses ball Avec ma queue, on joue pas au billard on fait du baseball Caresse la batte, mets toi à quatre pattes et j'tire au paintball Avec mon gun tu passes aux assiettes si t'as pas d'bol Avec ma gueule, ma gueule, t'es sur d'être mis sur l'té-co Fuck la plage, j'veux un château avec une vue sur l'ghetto Avec Michael, j'gueule, le mic', rime avec Tyson Devant lautre Michael, jrajoute Daniels pour que Jackson Wilkinson tranchants dès lors où la perquise sonne Jredoute personne à part les shtars de peur qu'ils m'saignent Jsuis pisté par les pe-stu, en X5 Le micro j'le fais bler-trem, il attrape Parkinson Le crack imprègne mes disques sans passer par Kingston Si deux PD préméditent, c'est 100 pour qu'ils s'donnent Armé dun uzi, l'esprit lucide quand les gens rentrent solo Si la vie s'rait une pute, ouais, je l'appellerais Sharon Stone Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Ce son, cest comme cette putain de chaine cryptée la nuit le samedi Que des fous, que des loups même prêts à ler-vio le cro-mi Le 20ème, cest mon réseau, les keufs nous té-ma avec trop d'ces-vi Va dire à ces batards qu'on restera là sans les servir J'vais sévir sur l'beat, appelle ça violence gratuite J'vais te buter sans but pourquoi pas pécho des thunes Si j'pécho une pute ce qu'on fera, c'est du bite à bouche On fuck les dirigeants Français en glissant capotes dans l'urne Ils disent tes lyrics sont dun vulgaire Fermes ta gueule, cest soit ça ou bien ma bulle dair Dans ta bouche, ton crew Vas-y bouge ou tauras la même impression quaprès-avoir laissé lsavon dans la douche Mon équipe, te liquide, te rend fou, comme deux shits Eh reste cool face au futur leader Nouvelle école, Alcailllou, jcrois que tas vu la couleur Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous Suce nos bites, salope, lèche nos boules de bowling Fais nous plaisir et mets la langue, ouais, utilise ton piercing Là c'est Still Fresh, Alkpote et Mister You Zougataga mon pote, eh ouais c'est l'rap tah les voyous</t>
         </is>
       </c>
     </row>
@@ -4640,12 +4640,12 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Sur le toit</t>
+          <t>Summer Zoo</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Eh ma gueule, ouais, ouais, ouais Eh, eh Eh, eh, eh Nique ta mère et ton re-pè Ah-ah Le jour où j'ai raté mon BEP Mister Yougataga, ALP Alpha Lima Pedro Eh, eh, eh Rah J'me réveille, j'suis dans les hautes sphères, dans des problèmes, dans mon domaine Elle veut mon visage en poster, que j'la balade, que j'lui promette J'vois son sourire jusqu'aux pommettes, ses yeux bridés, j'vois ses fossettes J'suis trop distant, j'fais mon possible, l re-noi est violent t docile Lima a grandi à Bercy, volé à Bercy, chanté à Bercy J'vais pas t'quémander un merci pour un service, j'ai des principes On fait la rue, on fait la té-ci, on est très précis si tu persistes Heures du matin, c'est les perquises, t'as pas coffré, ils t'ont saisi Ma daronne a confiance en moi, j'peux pas flancher, j'peux pas lâcher J'finis un jet, donner mon cur, ils ont tout gâché, ils l'ont cassé Pas une nuit sans penser à brasser, à brasser, à embrasser J'aimais la rue donc j'l'ai embrassé, embrassé, la rue embrassée Ils nous reconnaissent tous ou qui nous pointent du doigt J'suis sur le toit d'la tour, je sais qu'on compte sur moi Ils m'ont pris pour un fou, les jaloux ont peur du poids Elle veut qu'j'lui fasse la cour, elle veut être la femme du roi You might also like Ce soir, j'me suis endormi dans l'bain Dans l'bain J'me réveille le matin dans la cuisine Dans la cuisine Ce soir, j'me suis endormi dans l'bain Dans l'bain J'me réveille le matin dans la cuisine Oh ouais, oh ouais, oh ouais, oh ouais J'me réveille le matin dans la cuisine Oh ouais, oh ouais, oh ouais, oh ouais J'me réveille le matin dans la cuisine Quand y a drah, on n'a jamais balisé Balisé, les keufs sont v'nus nous faire baliser Baliser Chez nous, ça traîne qu'en bande organisée Organisée d'la maternelle au lycée Ouais, yeah Grosse Ferrari, r'présente Paris, doublé d'Mbappé, feinte de frappe tah Neymar crari J'fais tmenick j'ai mal au dos et bicyclette dans vos grands-mères C'est Mister You, Alpha Lima Pedro, y a d'la frappe d'Outre-Mer On fait d'l'oseille, on sort les armes, les keufs sans hlel dans la lasagne J'suis d'ceux qu'investissent en Lausanne, y a les ch'vaux d'course et y a les ânes Yeah, yeah Ils nous reconnaissent tous ou qui nous pointent du doigt J'suis sur le toit d'la tour, je sais qu'on compte sur moi Ils m'ont pris pour un fou, les jaloux ont peur du poids Elle veut qu'j'lui fasse la cour, elle veut être la femme du roi Ce soir, j'me suis endormi dans l'bain Dans l'bain J'me réveille le matin dans la cuisine Dans la cuisine Ce soir, j'me suis endormi dans l'bain Dans l'bain J'me réveille le matin dans la cuisine Oh ouais, oh ouais, oh ouais, oh ouais J'me réveille le matin dans la cuisine Oh ouais, oh ouais, oh ouais, oh ouais J'me réveille le matin dans la cuisine</t>
+          <t>J'touche pas aux vlo-tra j'baise qu'les go sans triques Je suis, comment vous dites ? égocentrique Sucer des bites, c'est pas autoriser J'ai écris c'texte à Fleury, à Fresnes j'vais le remastériser Vaporisez les billets, comme à ça ils auront une odeur Les 3ineurs s'que j'sais c'est qu'ils volent mieux qu'Harry Potter Un répondeur, ça sert à vesqui les gens Tu veux qu'on dorme ? t'es folle, écarte un peu les jambes Le feu d'l'amour on l'éteint pas en l'attisant Houbi, t'a un regard traumatisant Zebi, à la barre j'fais l'mec til-gen Mais l'juge s'bâtard il veut m'mettre 10 ans Woogataga Belleville grosse dédicace Miss reste en chatte et graille des whiskas Y'a l'36 postiché en bas d'la house Moi, j'm'en fiche là j'suis en train d'danser sur d'la house What in the world is a girl to do? When in this smokey place I only see you Was far away when you caught my eye You've brought me back and now you're making me high I was alone out there, with no one else around Now I've fallen for you gataga and there's no coming down Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes What can I do? I'm looking right at you This feeling is all new, I want you addicted to me Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes What can I do? I'm looking right at you This feeling is all new, I want you addicted to me You might also like C'soir évite les embrouilles même si on t'parles mal C'est la fête soit cool paye un verre au barman Sur la piste y'a qu'des missiles, c'est la guerre mondiale J'les aimes fines et sportives genre Sophie Thalmann C'est pour ceux et aussi celles qu'on pris la vie sur un coup d'tête Les voyous à la table qui enchaîne les bouteilles C'est pour Steve, Mamadou et Be-be-bechir J'ai entendu un pull up, pull up ça dé-dé-déchire C'est l'94 gataga connexion, Rap de barj' en action pour les braves On fais du son pure en illicite Marre d'voir XXX XXX Malfrat dans la boite ça peut douiller Gare aux mésaventure si t'espérais me fouiller J'ai le biff dans les fouilles si y'a heja J'vais faire des dégâts avec poto Tadja Eh excuse moi, eh demoiselle, wesh t'es sérieuse ? eh wallah j'vais t'charrier hey Anorexique 44 kilos poids net Tu fais pas d'pipi tu sniff dans les toilettes Gucci, Versace, Dolce Gabanna A la bouche un gare-ci tah la Havana Faya sous vodka j'préfère le whisky Suivi d'une lahsa d'Monica Lewinsky I was alone out there, with no one else around Now I've fallen for you gataga and there's no coming down Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes What can I do? I'm looking right at you This feeling is all new, I want you addicted to me Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes What can I do? I'm looking right at you This feeling is all new, I want you addicted to me Till there was you, I know what you're needing My thoughts are leading, me straight into your eyes</t>
         </is>
       </c>
     </row>
@@ -4657,12 +4657,12 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Teh les premiers soirs</t>
+          <t>Sur le toit</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>Dj Kayz Paris,Oran New York Bimbim Mister You Braaah Donne-moi la main ma chérie j'vais te faire danser Ce soir c'est moi qui paye j'ai tout financé J'vais t'faire oublier ton mari ou ton fiancé Si t'es célibataire laisse-moi t'ambiancer, essai Fais-moi kiffer scoue ton fessier Ralenti 2 secondes fais pas ta pressée Toi-même tu sais j'suis par la pour te stresser J'aime pas profiter d'mon succès J'crois qu'elle veut boire, elle regarde le bar J'vois qu'il est 4h sur sa montre chopard J'me dis qu'il s'fait tard, j'lemmène à ma table Et place à la magie tah les premiers soirs Scuse-moi désolé de te déranger J'ai rêvé de nous tous les deux allongés sous un oranger Si tes copines elles m'aimes pas C'est pas grave laisse les rager De toute façon j'suis courageux Timinik j'me suis rangé Une heure dans tes bras c'est mieux que le tour du monde Ouai Pour toi j'ferais la guerre J'pourrais tuer tout le monde Non c'est pas vrai, t'sais bien que j'fais le tomi Ce que j'veux c'est te serrer et finir dans ton lit Accroche toi direction le septième ciel Dans tes petits yeux j'ai vu l'étincelle Mets tes porte-jarretelles jt'emmène en balade Ouai J'vais t'faire passer une soirée de malade... You might also like Donne-moi la main ma chérie j'vais te faire danser Ce soir c'est moi qui paye j'ai tout financé J'vais t'faire oublier ton mari ou ton fiancé Si t'es célibataire laisse-moi t'ambiancer, essai Fais-moi kiffer scoue ton fessier Ralenti 2 secondes fais pas ta pressée Toi-même tu sais j'suis par la pour te stresser J'aime pas profiter d'mon succès J'crois qu'elle veut boire, elle regarde le bar J'vois qu'il est 4h sur sa montre chopard J'me dis qu'il s'fait tard, j'lemmène à ma table Et place à la magie tah les premiers soirs Bienvenue dans ma city tu vas faire des saltos Tellement t'es mimi moi j'ai sorti le smalto FENDI, ZILLI J'suis sous col-al On fini au sommet on est parti des halls crades Si tu fais du sale un jour ou l'autre tu paye Évidemment j'voulais pas que les keufs nous pètent Tu m'as fait du charme quand t'as vu les billets Ma montre briller, et là jt'ai grillé! Cette meuf est maléfique ouai elle aime les grossistes Le biffe les profits, les hits les gros feats Tu m'a donné ton cur pour une coupe de champagne J'ai laissé 30 balles j'partirai pas sans toi... Elle m'a mis les menottes pris de vitesse Ce soir tu conduis, moi j'suis dans l'ivresse On s'retrouve au parking On s'fait pas remarquer J'peux oublier la tess et le business Les galères les drames et la tristesse C'est pas la fin dla partie Rizer remet le paquet! Donne-moi la main ma chérie j'vais te faire danser Ce soir c'est moi qui paye j'ai tout financé J'vais t'faire oublier ton mari ou ton fiancé Si t'es célibataire laisse-moi t'ambiancer, essai Fais-moi kiffer scoue ton fessier Ralenti 2 secondes fais pas ta pressée Toi-même tu sais j'suis par la pour te stresser J'aime pas profiter d'mon succès J'crois qu'elle veut boire, elle regarde le bar J'vois qu'il est 4h sur sa montre chopard J'me dis qu'il s'fait tard, j'lemmène à ma table Et place à la magie tah les premiers soirs</t>
+          <t>Eh ma gueule, ouais, ouais, ouais Eh, eh Eh, eh, eh Nique ta mère et ton re-pè Ah-ah Le jour où j'ai raté mon BEP Mister Yougataga, ALP Alpha Lima Pedro Eh, eh, eh Rah J'me réveille, j'suis dans les hautes sphères, dans des problèmes, dans mon domaine Elle veut mon visage en poster, que j'la balade, que j'lui promette J'vois son sourire jusqu'aux pommettes, ses yeux bridés, j'vois ses fossettes J'suis trop distant, j'fais mon possible, l re-noi est violent t docile Lima a grandi à Bercy, volé à Bercy, chanté à Bercy J'vais pas t'quémander un merci pour un service, j'ai des principes On fait la rue, on fait la té-ci, on est très précis si tu persistes Heures du matin, c'est les perquises, t'as pas coffré, ils t'ont saisi Ma daronne a confiance en moi, j'peux pas flancher, j'peux pas lâcher J'finis un jet, donner mon cur, ils ont tout gâché, ils l'ont cassé Pas une nuit sans penser à brasser, à brasser, à embrasser J'aimais la rue donc j'l'ai embrassé, embrassé, la rue embrassée Ils nous reconnaissent tous ou qui nous pointent du doigt J'suis sur le toit d'la tour, je sais qu'on compte sur moi Ils m'ont pris pour un fou, les jaloux ont peur du poids Elle veut qu'j'lui fasse la cour, elle veut être la femme du roi You might also like Ce soir, j'me suis endormi dans l'bain Dans l'bain J'me réveille le matin dans la cuisine Dans la cuisine Ce soir, j'me suis endormi dans l'bain Dans l'bain J'me réveille le matin dans la cuisine Oh ouais, oh ouais, oh ouais, oh ouais J'me réveille le matin dans la cuisine Oh ouais, oh ouais, oh ouais, oh ouais J'me réveille le matin dans la cuisine Quand y a drah, on n'a jamais balisé Balisé, les keufs sont v'nus nous faire baliser Baliser Chez nous, ça traîne qu'en bande organisée Organisée d'la maternelle au lycée Ouais, yeah Grosse Ferrari, r'présente Paris, doublé d'Mbappé, feinte de frappe tah Neymar crari J'fais tmenick j'ai mal au dos et bicyclette dans vos grands-mères C'est Mister You, Alpha Lima Pedro, y a d'la frappe d'Outre-Mer On fait d'l'oseille, on sort les armes, les keufs sans hlel dans la lasagne J'suis d'ceux qu'investissent en Lausanne, y a les ch'vaux d'course et y a les ânes Yeah, yeah Ils nous reconnaissent tous ou qui nous pointent du doigt J'suis sur le toit d'la tour, je sais qu'on compte sur moi Ils m'ont pris pour un fou, les jaloux ont peur du poids Elle veut qu'j'lui fasse la cour, elle veut être la femme du roi Ce soir, j'me suis endormi dans l'bain Dans l'bain J'me réveille le matin dans la cuisine Dans la cuisine Ce soir, j'me suis endormi dans l'bain Dans l'bain J'me réveille le matin dans la cuisine Oh ouais, oh ouais, oh ouais, oh ouais J'me réveille le matin dans la cuisine Oh ouais, oh ouais, oh ouais, oh ouais J'me réveille le matin dans la cuisine</t>
         </is>
       </c>
     </row>
@@ -4674,12 +4674,12 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Tosma</t>
+          <t>Teh les premiers soirs</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>Mister Yougataga On vie dans une putain d'époque, on vend dla drogue, on fuck le proc' Bois d'Arcy, nes-Fres, la té-San ouais, ouais, ouais, on pourrait tourner pendant dix ans Fuck les jaloux, on va les écraser, Bentley ou Testarossa, ça vend le shit, ça vend la CC, ça mène une putain dvie de laud-sa J'te jure frérot crois-moi, j'ai vu des trucs insensés, ils sont bés-tom deux-trois mois, ils veulent m'apprendre à danser Si j'me suis mis à faire du son, c'est pour ne pas qu'les flics m'arrêtent Jai commencé par fumer lpilon avant de bédave la cigarette, ouais, ouais, ouais J'ai pas commencé guetteur, nan, nan, nan, jai détaillé direct Avec ma clique, le tos-ma j'le mettais dans les boîtes aux lettres Eh Yougataga, cette année on va racoller d'la tchagua Bye bye à toutes celles qui voulaient pas y a des hauts, y a des bas J'reviens mettre la fessée au rap français, les trois quarts des MC peuvent mappeler papa Y'a qu'au dispatching que l'froc est baissé Et si tu nous crois pas, rendez-vous là-bas Pas b'soin d' ou de psychanalyse pour savoir qu'y a du khaliss dans la valise Quand y a les keufs, crois pas que j'balise You c'est la Tour Eiffel à Bériz You might also like Pu-pu-putain mais dis moi qu'est ce que tu croyais ? Au chtar, les avocats se font soudoyer À la base, j'suis pas là pour festoyer S't'as bu la tasse, moi, j'me suis noyé Si j'me suis mis à faire du son, c'est pour ne pas qu'les flics m'arrêtent J'ai commencé par fumer l'pilon avant de bédave la cigarette, ouais, ouais, ouais J'ai pas commencé guetteur, nan, nan, nan, j'ai détaillé direct Avec ma clique, le tos-ma j'le mettais dans les boîtes aux lettres Eh Yougataga, cette année on va racoller d'la tchagua Bye bye à toutes celles qui voulaient pas y a des hauts, y a des bas Pu-pu-putain mais dis moi qu'est ce que tu croyais ? Au chtar, les avocats se font soudoyer À la base, j'suis pas là pour festoyer S't'as bu la tasse, moi, j'me suis noyé Mister Yougataga</t>
+          <t>Dj Kayz Paris,Oran New York Bimbim Mister You Braaah Donne-moi la main ma chérie j'vais te faire danser Ce soir c'est moi qui paye j'ai tout financé J'vais t'faire oublier ton mari ou ton fiancé Si t'es célibataire laisse-moi t'ambiancer, essai Fais-moi kiffer scoue ton fessier Ralenti 2 secondes fais pas ta pressée Toi-même tu sais j'suis par la pour te stresser J'aime pas profiter d'mon succès J'crois qu'elle veut boire, elle regarde le bar J'vois qu'il est 4h sur sa montre chopard J'me dis qu'il s'fait tard, j'lemmène à ma table Et place à la magie tah les premiers soirs Scuse-moi désolé de te déranger J'ai rêvé de nous tous les deux allongés sous un oranger Si tes copines elles m'aimes pas C'est pas grave laisse les rager De toute façon j'suis courageux Timinik j'me suis rangé Une heure dans tes bras c'est mieux que le tour du monde Ouai Pour toi j'ferais la guerre J'pourrais tuer tout le monde Non c'est pas vrai, t'sais bien que j'fais le tomi Ce que j'veux c'est te serrer et finir dans ton lit Accroche toi direction le septième ciel Dans tes petits yeux j'ai vu l'étincelle Mets tes porte-jarretelles jt'emmène en balade Ouai J'vais t'faire passer une soirée de malade... You might also like Donne-moi la main ma chérie j'vais te faire danser Ce soir c'est moi qui paye j'ai tout financé J'vais t'faire oublier ton mari ou ton fiancé Si t'es célibataire laisse-moi t'ambiancer, essai Fais-moi kiffer scoue ton fessier Ralenti 2 secondes fais pas ta pressée Toi-même tu sais j'suis par la pour te stresser J'aime pas profiter d'mon succès J'crois qu'elle veut boire, elle regarde le bar J'vois qu'il est 4h sur sa montre chopard J'me dis qu'il s'fait tard, j'lemmène à ma table Et place à la magie tah les premiers soirs Bienvenue dans ma city tu vas faire des saltos Tellement t'es mimi moi j'ai sorti le smalto FENDI, ZILLI J'suis sous col-al On fini au sommet on est parti des halls crades Si tu fais du sale un jour ou l'autre tu paye Évidemment j'voulais pas que les keufs nous pètent Tu m'as fait du charme quand t'as vu les billets Ma montre briller, et là jt'ai grillé! Cette meuf est maléfique ouai elle aime les grossistes Le biffe les profits, les hits les gros feats Tu m'a donné ton cur pour une coupe de champagne J'ai laissé 30 balles j'partirai pas sans toi... Elle m'a mis les menottes pris de vitesse Ce soir tu conduis, moi j'suis dans l'ivresse On s'retrouve au parking On s'fait pas remarquer J'peux oublier la tess et le business Les galères les drames et la tristesse C'est pas la fin dla partie Rizer remet le paquet! Donne-moi la main ma chérie j'vais te faire danser Ce soir c'est moi qui paye j'ai tout financé J'vais t'faire oublier ton mari ou ton fiancé Si t'es célibataire laisse-moi t'ambiancer, essai Fais-moi kiffer scoue ton fessier Ralenti 2 secondes fais pas ta pressée Toi-même tu sais j'suis par la pour te stresser J'aime pas profiter d'mon succès J'crois qu'elle veut boire, elle regarde le bar J'vois qu'il est 4h sur sa montre chopard J'me dis qu'il s'fait tard, j'lemmène à ma table Et place à la magie tah les premiers soirs</t>
         </is>
       </c>
     </row>
@@ -4691,12 +4691,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Totti</t>
+          <t>Tosma</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>J'ai fini l'jeu éteins ta console, j'suis la tête de gondole T'arrête pas d'parler chinois mais t'as une tête de mongole Rhalala qu'est-ce qu'elle est bonne mais khey qu'est-ce qu'elle consomme Elle veut faire un gosse dans l'dos mais j'oublie pas les condoms Ils portent l'il ils ont du mal à m'localiser Ils veulent tous rapper, miskine j'vais les traumatiser Vive le ter-ter niqu son père la retraite j'ai pas cotisé Alcoolisé du soir au soir y a trop d'brouillons à corrigr J'vais leur faire l'effet d'une bombe, tu vas t'croire à Bagdad Quand j'enverrais la purée ils sentiront pas la patate J'baise vos grandes surs comme si j'étais à Pattaya J'm'endors tranquillement à l'hôtel en sirotant mon Ruinart sale bâtard Ils vont s'en mordre les doigts à en devenir manchots J'viens d'paname un peu d'respect m'appelle pas l'sancho J'vais pas retourner ma veste j'ai déjà c'qu'y faut sous l'manteau J'fais flipper comme un revenant quand tu m'vois dans l'Rolls Phantom C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide You might also like J'me noie dans l'alcool tu crois que tout baigne Tu sors la poubelle je sers la plus belle En vrai jusqu'à mon dernier souffle, comme Abdelhak et Youssouf Quand y a les portières qui s'ouvrent, ben y a plein de mères qui souffrent Là j'suis posé sur le sofa, j'te refroidis fuck le chauffage Tu m'testes tu pers l'sophage, j'ai grandi avec les sauvages Spécialiste tah les go fast, j'suis chargé comme une gova Armé d'kalashnikov, là ça sécurise les convois Y a ceux qui envoient et ceux qu'on voit Y a ceux qui mordent y a ceux qui aboient Y a ceux qui assurent et ceux qui foirent Une chose est sûre c'est que ce soir on va foutre le feu avec mes enfoirés Ouais l'surveillant Oh zehma tu fais pas passer hein Eh j'te revois dehors j'te nique ta mère C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide Faut le diamant de la couronne, tah la reine Elisabeth Tu claques ton 'seille dans le miel, j'investis sur les abeilles Ca casse du sucre les hypocrites vont finir avec le diabète Gros tu connais dans la street faut chiffrer avant que ça pète Tu peux pas m'la faire, tu la fais qu'aux p'tits Jamais j'trahirai ma team comme Totti Si tu m'as taclé dans l'dos c'est qu'entre nous t'es l'fautif Arrête de casser les couilles ou j'désactive les notifs Paraît que j'suis pas trop émotif Y a que les gros chiffres qui me motivent J'veux pas vieillir comme un pauvre type J'avais huit piges j'écoutais Mob Deep Fuck tous tes rappeurs de merde, moi t'inquiète pas j'me démerde J'ai grandi dans le de-mer, quatre boites dans scooter des mers Y a pas d'règles ça pue l'urine, j'suis avec You en featuring J'veux une oseille de JR Ewing, j'te fume ta mère sur le ring C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide Trop de dos d'âne il faudrait qu'on pile Parle pas en face sois un peu comme pile Copain copine il faudrait qu'on pine Faut qu't'arrête tah Mary Poppins C'est l'album qui baise ta compil' C'est Mister You c'est BimBim C'est nous les best t'as compris? C'est Mister You c'est BimBim T'inquiète pas ça gère le style, de Verollot à Rebeval La street sur un pied d'estale, il n'y a que la maille qui maille</t>
+          <t>Mister Yougataga On vie dans une putain d'époque, on vend dla drogue, on fuck le proc' Bois d'Arcy, nes-Fres, la té-San ouais, ouais, ouais, on pourrait tourner pendant dix ans Fuck les jaloux, on va les écraser, Bentley ou Testarossa, ça vend le shit, ça vend la CC, ça mène une putain dvie de laud-sa J'te jure frérot crois-moi, j'ai vu des trucs insensés, ils sont bés-tom deux-trois mois, ils veulent m'apprendre à danser Si j'me suis mis à faire du son, c'est pour ne pas qu'les flics m'arrêtent Jai commencé par fumer lpilon avant de bédave la cigarette, ouais, ouais, ouais J'ai pas commencé guetteur, nan, nan, nan, jai détaillé direct Avec ma clique, le tos-ma j'le mettais dans les boîtes aux lettres Eh Yougataga, cette année on va racoller d'la tchagua Bye bye à toutes celles qui voulaient pas y a des hauts, y a des bas J'reviens mettre la fessée au rap français, les trois quarts des MC peuvent mappeler papa Y'a qu'au dispatching que l'froc est baissé Et si tu nous crois pas, rendez-vous là-bas Pas b'soin d' ou de psychanalyse pour savoir qu'y a du khaliss dans la valise Quand y a les keufs, crois pas que j'balise You c'est la Tour Eiffel à Bériz You might also like Pu-pu-putain mais dis moi qu'est ce que tu croyais ? Au chtar, les avocats se font soudoyer À la base, j'suis pas là pour festoyer S't'as bu la tasse, moi, j'me suis noyé Si j'me suis mis à faire du son, c'est pour ne pas qu'les flics m'arrêtent J'ai commencé par fumer l'pilon avant de bédave la cigarette, ouais, ouais, ouais J'ai pas commencé guetteur, nan, nan, nan, j'ai détaillé direct Avec ma clique, le tos-ma j'le mettais dans les boîtes aux lettres Eh Yougataga, cette année on va racoller d'la tchagua Bye bye à toutes celles qui voulaient pas y a des hauts, y a des bas Pu-pu-putain mais dis moi qu'est ce que tu croyais ? Au chtar, les avocats se font soudoyer À la base, j'suis pas là pour festoyer S't'as bu la tasse, moi, j'me suis noyé Mister Yougataga</t>
         </is>
       </c>
     </row>
@@ -4708,12 +4708,12 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Touche pas à mon biff</t>
+          <t>Totti</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>Hades Hasta la muerte, on a connu le meilleur et le pire On va se démerder, solo pour bâtir un empire Qu'est-ce que j'voulais dire ? Y a du lourd dans le ffre-co de la tire On aboie pas, on mord rect-di, on braque pas, on ré-ti J'descends du Rif, j'descends pas du singe et pourtant j'suis khfif J'dois faire du biff, pour ça faut faire passer la marchandise Samantha, Bogota, Véronique, Point-à-Pitre, que des litres Adeline, Medellín, Hanane, Paname, Dominique, Pierrefitte, han Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Touche à mon biff, je t'allume ta mère petit fils de timp Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Une boîte plus deux plus trois plus quatre Il m'faut un zodiac, pas juste un scooter des mers Sous Jack, Dom Pé, Chivas, Toucas Que ces fils de timp aillent tous niquer leurs mères On fume du shit et de l'herbe On a grandi dans la merde Quand t'es en chien, personne t'aide Les gens veulent même te voir dead Vida loca, vida vida loca Fuck les condés venus vider la ve-ca Ils ont pris le pilon, ils ont pris la me-ca Ces putains de fils de pute font péter un ble-câ ah Pas de krav-maga, j'ai mon bouche-ca gé-char pour calmer tous tes gars crr, crr Yougataga, tu connais Yougataga ah, brrrah You might also like Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Touche à mon biff, je t'allume ta mère petit fils de timp Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non J'suis défoncé, mes pensées deviennent diaboliques Pied au plancher, j'accélère dans un bolide J'ai la potion, j'vais la bicrave au druide Plus noir que la weed Le caviar, le saumon, le foie gars vont remplacer les frites, on rêve d'être millionnaires On fume de la bonne résine, de la putain de ganja histoire de calmer nos nerfs L'oseille, l'argent, les lovés On a fait des trucs de fou pour en trouver Parfois, j'ai même failli en crever Gros, tu peux remballer J'ai fait tout ce qu'il fallait, non, j'ai plus rien à prouver Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Touche à mon biff, je t'allume ta mère petit fils de timp Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non</t>
+          <t>J'ai fini l'jeu éteins ta console, j'suis la tête de gondole T'arrête pas d'parler chinois mais t'as une tête de mongole Rhalala qu'est-ce qu'elle est bonne mais khey qu'est-ce qu'elle consomme Elle veut faire un gosse dans l'dos mais j'oublie pas les condoms Ils portent l'il ils ont du mal à m'localiser Ils veulent tous rapper, miskine j'vais les traumatiser Vive le ter-ter niqu son père la retraite j'ai pas cotisé Alcoolisé du soir au soir y a trop d'brouillons à corrigr J'vais leur faire l'effet d'une bombe, tu vas t'croire à Bagdad Quand j'enverrais la purée ils sentiront pas la patate J'baise vos grandes surs comme si j'étais à Pattaya J'm'endors tranquillement à l'hôtel en sirotant mon Ruinart sale bâtard Ils vont s'en mordre les doigts à en devenir manchots J'viens d'paname un peu d'respect m'appelle pas l'sancho J'vais pas retourner ma veste j'ai déjà c'qu'y faut sous l'manteau J'fais flipper comme un revenant quand tu m'vois dans l'Rolls Phantom C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide You might also like J'me noie dans l'alcool tu crois que tout baigne Tu sors la poubelle je sers la plus belle En vrai jusqu'à mon dernier souffle, comme Abdelhak et Youssouf Quand y a les portières qui s'ouvrent, ben y a plein de mères qui souffrent Là j'suis posé sur le sofa, j'te refroidis fuck le chauffage Tu m'testes tu pers l'sophage, j'ai grandi avec les sauvages Spécialiste tah les go fast, j'suis chargé comme une gova Armé d'kalashnikov, là ça sécurise les convois Y a ceux qui envoient et ceux qu'on voit Y a ceux qui mordent y a ceux qui aboient Y a ceux qui assurent et ceux qui foirent Une chose est sûre c'est que ce soir on va foutre le feu avec mes enfoirés Ouais l'surveillant Oh zehma tu fais pas passer hein Eh j'te revois dehors j'te nique ta mère C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide Faut le diamant de la couronne, tah la reine Elisabeth Tu claques ton 'seille dans le miel, j'investis sur les abeilles Ca casse du sucre les hypocrites vont finir avec le diabète Gros tu connais dans la street faut chiffrer avant que ça pète Tu peux pas m'la faire, tu la fais qu'aux p'tits Jamais j'trahirai ma team comme Totti Si tu m'as taclé dans l'dos c'est qu'entre nous t'es l'fautif Arrête de casser les couilles ou j'désactive les notifs Paraît que j'suis pas trop émotif Y a que les gros chiffres qui me motivent J'veux pas vieillir comme un pauvre type J'avais huit piges j'écoutais Mob Deep Fuck tous tes rappeurs de merde, moi t'inquiète pas j'me démerde J'ai grandi dans le de-mer, quatre boites dans scooter des mers Y a pas d'règles ça pue l'urine, j'suis avec You en featuring J'veux une oseille de JR Ewing, j'te fume ta mère sur le ring C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide C'est qui les best, tu devines Yougata Gangst to the Bim Arrête ton rap de débile on va t'la mettre dans le bide Trop de dos d'âne il faudrait qu'on pile Parle pas en face sois un peu comme pile Copain copine il faudrait qu'on pine Faut qu't'arrête tah Mary Poppins C'est l'album qui baise ta compil' C'est Mister You c'est BimBim C'est nous les best t'as compris? C'est Mister You c'est BimBim T'inquiète pas ça gère le style, de Verollot à Rebeval La street sur un pied d'estale, il n'y a que la maille qui maille</t>
         </is>
       </c>
     </row>
@@ -4725,12 +4725,12 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Tranquillement</t>
+          <t>Touche pas à mon biff</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>Premièrement, tranquillement j'arrive et j'vous affranchis Deuxiémement tu connais moi j'suis pas un apprenti Troisiemement à st'heure ci j'viens d'prendre une peine de bandit Quatriemement j'connais du monde j'sortirais donc en condi Woogataga dahwa t'sais ce qu'on dit Plutôt que d'squatter l'palace d'une pute et beh vaut mieux son ptit taudis Mon soce fait peter l'son dans ton Porshe ou ton Audi C'est Mister you rap de barge ouais freestyle d'antologie Commissaire j'madresse à oit, ouais arrêtes moi si tu peux Paris woogataga nique la Bac et les stupeux Sous sky dans les virages ça joue les Raïkkonen Les faux c'est des fils de pute mais t'inquiéte les vrais y connaissent 96 heures operationnel mais c'est pas fini Mandat de depot criminel j'freestyle jusqu'à l'infinie Woogataa'rtfou sur la gueule des batards les matons Ainsi que les gradés qui revent que d'nous foutre au mitard J'ai du rétrogradé vus qu'les an-ges étaient en retard J'ai enclanché la marche arrière ils arrivent toujours pas a m'guélar Quand j'cris Bébébelleville tout l'tier-quar bébébégaye T'es une belle fille jt'ai dit hobbi c'étais juste pour tkékékéne - Refrain - Y se acabó la diversión Llegó el Comandante y mandó a parar X2 You might also like Premièrement, tranquillement j'arrive et j'vous affranchis Deuxiémement tu connais moi j'suis pas un apprenti Troisiemement à st'heure ci j'viens d'prendre une peine de bandit Quatriemement j'connais du monde j'sortirais donc en condi Woogataga dahwa t'sais c'qu'on dit La parole vaut l'homme mais nous n'sommes pas des Carabantes Faut pas s'mentir jsuis pas d'ceux qui cassent des brinks C'est pour ceux qui brise le ter-ter que j'casse-dedi Les suceurs ils ont de l'herpes j'crois pas qu'ils gouteront a ma tise Les vrais j'les respecte par contre les faux j'les traumatise J'ai trop squatté la street j'en ai attrapé des rhumatismes C'est les Bloods et les Crips entre Alphonse Kert et Rue Mathys J'suis d'lautre côté du mouchoir celui qu'est remplie de khnouna Le revers d'la medaille si on trahit n'3el bouna A Belleville en mémoire à Zyad et Bouna On a graillé les poulets une boite de 4 par laguna - Refrain - Y se acabó la diversión Llegó el Comandante y mandó a parar X2 Y se acabó la di... J'arrive et j'vous affranchis Tranquillement tu connais moi j'suis pas un apprenti C'est la merde A st'heure ci j'vien d'prendre une peine de bandit Inch'Allah j'connais du monde j'sortirais donc en condi Woogataga eh mon gars viens j'te dis Crame mon blaze une, deux,trois fois et j'deviens mal Kandi J'arrive trop lourd donc les rappeurs s'inscrivent à la gym Ils crient tous A3oudou Billah mina shaytan ar rajim Tranquillement j'arrive et j'les affranchis J'suis faya j'suis fonc-dé mais j'réfrite un ptit bout d'shit Demande aux gars d'la street c'est qui le best des best ils t'diront Woogataga you wanna gangst to gangst Quand sa sent l'Must ou bien l'Pasha tèh Cartier Bah y'a 36 fois plus de keufs que d'meufs dans l'quartier Il nous faut Monica Bellucci Eh ouais c'est çà p'tit on boycott Fabio Lucci pour Gianni Versace Leche ma eue'qu et t'auras ptetre un ech de one Enchanté Laziza mais nan jm'appelle pas Balavoine Wesh me gusta la vida me gusta tu J'laisse les aufx en levrette et les vrais j'leurs dedicasse tous Si elle m'kiff la rue c'est parce qu'elle est pas conne MrYOU.SKYROCK.COM Si t'es un batard tu peux garder tes commentaires J'rap pour l'placard pour Fleury pour Fresnes pour Nanterre Pour Aboubakar, pour Abdelkader Ma plus belle nuit à moi c'était Laylat al-Qadr Akhi nan j'finirais pas comme De Villepin Moi j'terminrais comme les frères qui sortent de Villepinte J'rap pour No times fansdé Moh aux platines A la gloire Inch'allah du dispatching au disque platine T'as qu'a demander a la street c'est qui le best des best Bebebelleville zoo wanna gangst to gangst - Refrain - Y se acabó la diversión Llegó el Comandante y mandó a parar X2</t>
+          <t>Hades Hasta la muerte, on a connu le meilleur et le pire On va se démerder, solo pour bâtir un empire Qu'est-ce que j'voulais dire ? Y a du lourd dans le ffre-co de la tire On aboie pas, on mord rect-di, on braque pas, on ré-ti J'descends du Rif, j'descends pas du singe et pourtant j'suis khfif J'dois faire du biff, pour ça faut faire passer la marchandise Samantha, Bogota, Véronique, Point-à-Pitre, que des litres Adeline, Medellín, Hanane, Paname, Dominique, Pierrefitte, han Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Touche à mon biff, je t'allume ta mère petit fils de timp Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Une boîte plus deux plus trois plus quatre Il m'faut un zodiac, pas juste un scooter des mers Sous Jack, Dom Pé, Chivas, Toucas Que ces fils de timp aillent tous niquer leurs mères On fume du shit et de l'herbe On a grandi dans la merde Quand t'es en chien, personne t'aide Les gens veulent même te voir dead Vida loca, vida vida loca Fuck les condés venus vider la ve-ca Ils ont pris le pilon, ils ont pris la me-ca Ces putains de fils de pute font péter un ble-câ ah Pas de krav-maga, j'ai mon bouche-ca gé-char pour calmer tous tes gars crr, crr Yougataga, tu connais Yougataga ah, brrrah You might also like Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Touche à mon biff, je t'allume ta mère petit fils de timp Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non J'suis défoncé, mes pensées deviennent diaboliques Pied au plancher, j'accélère dans un bolide J'ai la potion, j'vais la bicrave au druide Plus noir que la weed Le caviar, le saumon, le foie gars vont remplacer les frites, on rêve d'être millionnaires On fume de la bonne résine, de la putain de ganja histoire de calmer nos nerfs L'oseille, l'argent, les lovés On a fait des trucs de fou pour en trouver Parfois, j'ai même failli en crever Gros, tu peux remballer J'ai fait tout ce qu'il fallait, non, j'ai plus rien à prouver Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non Touche à mon biff, je t'allume ta mère petit fils de timp Toucher mon biff, non, non, non, non Faut pas toucher mon biff, non, non</t>
         </is>
       </c>
     </row>
@@ -4742,12 +4742,12 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Tremblement de ter-ter</t>
+          <t>Tranquillement</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Cent mille euross Pour mes Los Bastardos Seth Guekoss Saint-Ouen-l'Aumôn'ss Chrome-Néoss Fait péter les euross Pour mes Los Racaillos C'est un tremblement d'ter-toss Amène ta clique on les couche tous On arrive dans l'rap tout schuss, lourd comme la patate à Mouss Diouf Drive-by en pouce-pouce, ajoute du caviar dans l'couscous Nous on porte nos couilles sans coup d'pouce On a l'vent en poupe quand toi tu pompes dans l'vent Rassasie les poucaves à coups d'pompe dans l'ventre On vend pas l'chocolat d'Genève, mais de Ouarzazate Le rap game dis-lui que ma zézète veut voir sa chatte La concurrence, on la baise, la rabaisse, mec Passe, passe le pèze, c'est tout c'qui nous apaise, mec Pousse le volume du son qui t'agresse dans ta caisse, mec Tu trouveras pas plus lourd, pas plus vrai, pas plus tess, mec Encaisse le clap comme une claque sur ta fesse, mec Personne nous teste wesh, tout l'monde nous respecte, mec Simuler des coups d'tête c'est ton premier réflexe, mec We're so hood, so bad, so ruffneck, yeah ! Tremblement d'ter-ter C'est un tremblement d'ter-ter Rebeus, Renois, Caraïs, Berbères C'est un tremblement d'ter-ter, check c'est la terre-mère Tremblement d'ter-ter C'est un tremblement d'ter-ter Kalos, Cainfris, nouches-Ma et Gwères C'est un tremblement d'ter-ter La gloire suce pour un kif, dans un J9 dégueulasse Température absolue quand le quartier se glace Ouais M.C ton rap ne casse pas des briques Donc laisse pas traîner ta serviette hygiénique dans les chiottes du Quick Reste reur-ti, meurtri par les échecs Coquards et grosses lèvres lendemain d'un jour de fête Dans chaque tiex', c'est la hass Jure pas sur la Mecque, tu veux m'la mettre je te baise Neuf-Cinq, S.O.A., Banlieue d'Paris c'est là qu'on est Ma ville tu la connais, par ici la monnaie J'veux la daronne assise a la son-mai L'khalis il doit tomber, l'raciste on va plomber Pas d'cinéma, pas d'carte UGC Barbare oui je sais, j'ai ma capuche baissée J'arrive zgègue de Galsène, j'baise de la chienne J'reste moi-même Nourou, say my name Un truc spécial pour mes cailles que j'étale sur mes cahiers J'envoie des mots comme des balles en métal vaut mieux tailler Zes' mec de tess, nous on fait trembler ton palier J'débarque, Vitry, Neuf-Quatre, on a l'talent pour t'braquer ou freestyler J'suis dans un hall, gros j'suis calé, avec l'équipe, dans une allée Mange du bitume toute l'année, veulent voir nos rôles ici caner On a choisi, on s'est cramés Par les soucis, gros j'suis gavé, viens pas m'check si t'as trop parlé T'as trop parlé, bâtard ? Nique ta mère, la chatte à ta grand-mère, bâtard On va t'niquer ta mère On va t'jeter dans une cave dans l'Neuf-Cinq Hé, Tonton Seth, j'ai huit mesures en or si tu m'l'autorises J'arrive plus lourd qu'une orgie d'sumotoris À mon mariage c'est moi qu'j'aurai l'plus beau jogging Le plus gros bolide une R19 avec un turbo d'Boeing Les MC encaissent mieux les pruneaux qu'Tony Zekwé chie des rafales d'obus, le F.C. Porto va droit au but Ouh caralhou, teste pas les cailleras d'nos rues Ou l'addition sera salée comme un accra d'morue J'arrive en balle, mon excursion sera expéditive Écoute je ne mens pas, c'est bien pour ça qu'j'obtiens l'respect des p'tits Toujours au top moi, j'ai la bonne recette On prend les mêmes et on recommence, j'te mets en transe sur l'album de Seth En une phase, le ter-ter subit un tremblement J't'ai vu dans l'angle mort, tu kiffais pas, au final t'en redemandes J'suis une bombe à retardement Ça fait brrraaah, zdedededex, ouvre pas tes fesses, j'te la mets tendrement On a des têtes comme dans l' Dernier Gang Oufs à la Spaggiari, on est des barbares, que des 7 sur le code-barre Ambiance Audiard ou Tarantino, touche pas à nos bambinos On t'aura, comme dans Gomorra cache pas l'butin sous l'Dunlopillo Demande à Al Poelvoordino wanted pour murder Nique ta mère la Police, nique ta race Fox Mulder On y croit tous comme Ribéry, fout l'dawa comme au Bayern J'baiserai la France jusqu'à c'qu'elle m'aime comme Mac Tyer C'est pour les malfrats, les ghetto youths Entre la mosquée et la muscul', ou sur Neptune via d'la ppe-fra Absolut Insolents, on sait vi-sèr' des sons lourds Prêts a salir, coûte que coûte on veut les salaires Coups d'couteau dans sa mère, l'rap crève, arme, guerre Micros en l'air, tout l'monde à terre temblement d'ter-ter C'est Aulnay, 2SK'Prod, tes potos connaissent 93.6, pé-cou tes cojones Tremblement d'ter-ter C'est un tremblement d'ter-ter Rebeus, Renois, Caraïs, Berbères C'est un tremblement d'ter-ter, check c'est la terre-mère Tremblement d'ter-ter C'est un tremblement d'ter-ter Kalos, Cainfris, nouches-Ma et Gwères C'est un tremblement d'ter-ter On roule dans des caisses d'occase, la marijuana vient d'Tijuana Les balles qu'on tire, wallah, viennent du Caucase La fumée s'propage comme des phéromones Starfoullah l'héritage qu'on a offert aux mômes Avec classe, on s'échappe par l'vasistas Face au fisc on balise pas, vu qu'à la douane les valises passent T'façon on a jamais aimé Rambo, Tarzan Nos idoles sont ceux qui vendent des kilos d'pavot afghan J'suis le côté diabolique de Serge Gainsbourg J'connais le diagnostic mais j'espère que les médecins s'gourent J'festoie fils serre-moi un verre d'vin rouge J'm'esquinte, j'souffre, j'suis quelqu'un d'louche Je fatigue Satan, crois pas qu'la Police arrive à temps Ou qu'ça tire à blanc dans la galerie marchande Je fabrique l'argent, la famille attend Qu'j'ramène entre les dents le string de Fanny Ardant Envoie les clefs du TT, j'me transforme en virtuose J'mets des grosses fessées sur des p'tits culs roses Vote pour moi sur chien-d'la-casse.fr J'te regarde de travers si tu cherches moi les vers J'pue l'Jack Daniel, j'suis l'fils caché d'Gargamel J'm'en vais danser l'disco avec deux-trois chattes d'Asnières On s'entraîne au tir au bois d'Achères, ambiance murder Pas d'voice au vocoder, c'est Giorgio Moroder Sur moi, ne lé-par pas Car chez nous la trahison ne se répare pas On prend les sens interdits T'rentre dedans comme la vachette d'Intervilles Crois pas qu'chez nous c'est fantastique À mettre la cagoule, les gants en plastique Les 'tasses de tess', c'est pas ma tasse de thé Pour les p'tis gars du Seize fais des traces de C Quand on était p'tits, les anciens nous envoyaient acheter des canettes Aujourd'hui ils nous sucent la bite pour qu'on leur avance une galette C'est la galère ouais, mais nique sa mère, on a l'feeling Investir dans un calibre c'est mieux que d'faire d'l'haltérophilie À la mairie, on leur a demandé un terrain d'foot Ils ont refusé, on s'est mis à bicrave et on a ouvert un terrain d'chnouf Bouffe pas la galette des rois, tu trouveras pas la fève J'ai vendu la galette darwa, j'ai fini au Quai des Orfèvres Laissez passer les têtes de cabochards Enfouraillés au 79, rue Quentin Bauchart Donne toujours une pièce quand tu rencontres un clochard Wesh, éteins ton char, échange pas des années d'liberté contre un bon-char En bon couche-tard, j'ai la gueule du Capitaine Caverne Va niquer ta mère si t'es un kouffar On a la même beu-bar qu'Jacques-Oussama Mess'Laden Au tier-quar on baise la mère de Papy Broussard Tremblement d'ter-ter Morsay, Seth Gueko Eh, ça vient tout droit du Neuf-Cinq, cousin Néochrome, Truands 2 La Galère On bicrave sec à Clignancourt Tu peux pas test c'est les vrais voyous, mon pote Eh l'Neuf-Cinq les vrais sauvages !You might also like</t>
+          <t>Premièrement, tranquillement j'arrive et j'vous affranchis Deuxiémement tu connais moi j'suis pas un apprenti Troisiemement à st'heure ci j'viens d'prendre une peine de bandit Quatriemement j'connais du monde j'sortirais donc en condi Woogataga dahwa t'sais ce qu'on dit Plutôt que d'squatter l'palace d'une pute et beh vaut mieux son ptit taudis Mon soce fait peter l'son dans ton Porshe ou ton Audi C'est Mister you rap de barge ouais freestyle d'antologie Commissaire j'madresse à oit, ouais arrêtes moi si tu peux Paris woogataga nique la Bac et les stupeux Sous sky dans les virages ça joue les Raïkkonen Les faux c'est des fils de pute mais t'inquiéte les vrais y connaissent 96 heures operationnel mais c'est pas fini Mandat de depot criminel j'freestyle jusqu'à l'infinie Woogataa'rtfou sur la gueule des batards les matons Ainsi que les gradés qui revent que d'nous foutre au mitard J'ai du rétrogradé vus qu'les an-ges étaient en retard J'ai enclanché la marche arrière ils arrivent toujours pas a m'guélar Quand j'cris Bébébelleville tout l'tier-quar bébébégaye T'es une belle fille jt'ai dit hobbi c'étais juste pour tkékékéne - Refrain - Y se acabó la diversión Llegó el Comandante y mandó a parar X2 You might also like Premièrement, tranquillement j'arrive et j'vous affranchis Deuxiémement tu connais moi j'suis pas un apprenti Troisiemement à st'heure ci j'viens d'prendre une peine de bandit Quatriemement j'connais du monde j'sortirais donc en condi Woogataga dahwa t'sais c'qu'on dit La parole vaut l'homme mais nous n'sommes pas des Carabantes Faut pas s'mentir jsuis pas d'ceux qui cassent des brinks C'est pour ceux qui brise le ter-ter que j'casse-dedi Les suceurs ils ont de l'herpes j'crois pas qu'ils gouteront a ma tise Les vrais j'les respecte par contre les faux j'les traumatise J'ai trop squatté la street j'en ai attrapé des rhumatismes C'est les Bloods et les Crips entre Alphonse Kert et Rue Mathys J'suis d'lautre côté du mouchoir celui qu'est remplie de khnouna Le revers d'la medaille si on trahit n'3el bouna A Belleville en mémoire à Zyad et Bouna On a graillé les poulets une boite de 4 par laguna - Refrain - Y se acabó la diversión Llegó el Comandante y mandó a parar X2 Y se acabó la di... J'arrive et j'vous affranchis Tranquillement tu connais moi j'suis pas un apprenti C'est la merde A st'heure ci j'vien d'prendre une peine de bandit Inch'Allah j'connais du monde j'sortirais donc en condi Woogataga eh mon gars viens j'te dis Crame mon blaze une, deux,trois fois et j'deviens mal Kandi J'arrive trop lourd donc les rappeurs s'inscrivent à la gym Ils crient tous A3oudou Billah mina shaytan ar rajim Tranquillement j'arrive et j'les affranchis J'suis faya j'suis fonc-dé mais j'réfrite un ptit bout d'shit Demande aux gars d'la street c'est qui le best des best ils t'diront Woogataga you wanna gangst to gangst Quand sa sent l'Must ou bien l'Pasha tèh Cartier Bah y'a 36 fois plus de keufs que d'meufs dans l'quartier Il nous faut Monica Bellucci Eh ouais c'est çà p'tit on boycott Fabio Lucci pour Gianni Versace Leche ma eue'qu et t'auras ptetre un ech de one Enchanté Laziza mais nan jm'appelle pas Balavoine Wesh me gusta la vida me gusta tu J'laisse les aufx en levrette et les vrais j'leurs dedicasse tous Si elle m'kiff la rue c'est parce qu'elle est pas conne MrYOU.SKYROCK.COM Si t'es un batard tu peux garder tes commentaires J'rap pour l'placard pour Fleury pour Fresnes pour Nanterre Pour Aboubakar, pour Abdelkader Ma plus belle nuit à moi c'était Laylat al-Qadr Akhi nan j'finirais pas comme De Villepin Moi j'terminrais comme les frères qui sortent de Villepinte J'rap pour No times fansdé Moh aux platines A la gloire Inch'allah du dispatching au disque platine T'as qu'a demander a la street c'est qui le best des best Bebebelleville zoo wanna gangst to gangst - Refrain - Y se acabó la diversión Llegó el Comandante y mandó a parar X2</t>
         </is>
       </c>
     </row>
@@ -4759,12 +4759,12 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Triste Époque</t>
+          <t>Tremblement de ter-ter</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>11ème 19ème 20ème Triste époque mon pote ! Eh ouuuais aaaaaaaaaaaaaah tention' Bébébébélleville Wesh dahwa parait que ta fait ton halal zooogataga Psartek en ce qui m'concerne moi J'ai fait le haram avec ma rue quand j'ai bédave ma première barrette On s'est marié direct le jour où j'ai bicrave la première galette C'est pour les braves comme Nas, comme Sidyou, comme Toumi, Khaled À tous ceux que j'aurais oublié les mecs qui auront su m'venir en aide Khabta mon bien être j'suis pas net j'fuck toute la planète Y'a trop de sky dans ma canette regarde ma gueule sur internet À trop écouter du rap de merde tu peux en devenir carrément sourd J'regarde ma montre Ohh il est dejà l'heure j'big up Shakar El Mansour Triste Epoque, mon pote le monde il part en glawi oui oui J'me verrai bien au bled avec Abderrazak El Mahraoui Blanchir juste un lion-mi léjéh el baraka L'rap français pour moi c'est comme du bachi pour un maraka J'oublie pas No Times Records Boubakar Tristan Comme dit Wisla fuck les bâtards qu'ils fument tout seul leurs tipisla Un conseil joue pas le voyou arrête le rap et fais du basket C'est Mister You sur écoute comme Avon barksdale You might also like Woogataga le refré Yaston À Slimane a Souleymane, ah woogatabraaaaaaaaaaaaaaaa J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assess Triste époque mon pote j'te jure demande à Aladin J'fume du seum, j'ai du plomb et donc du monde dans la tête Les mecs pour une barrette ils te mettent une peine exemplaire Rachida il faut qu'elle s'en va, Sarko faut qui nique son père J'me sens seul comme cette goutte d'huile dans l'océan J'essaie en vain de rentabiliser les séances Là j'tourne en rond autant qu'un taulard en promenade Ou un mec qui cherche un bête de taf, mais qu'a le teint trop mat Moi quand j'sors de gard'av c'est que j'rentre au placard V.I.P en chaussette, nique les 3asses bande de batard Ils sont là pour t'faire la misère fouille cellulaire à 6h J'ai pas le profil de l'auxiliaire moi c'est pour ça qu'ils m'ont dans le viseur Le rôle j'vais m'l'accaparer çà j'te l'dit fih seh Y'a plus de coke à Paris qu'y a de neige dans le Val dIsère C'est Mister Youu Gataga pour les intimes Pour tous les mecs cramés, comme les dramé baka ou Latifi J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses1</t>
+          <t>Cent mille euross Pour mes Los Bastardos Seth Guekoss Saint-Ouen-l'Aumôn'ss Chrome-Néoss Fait péter les euross Pour mes Los Racaillos C'est un tremblement d'ter-toss Amène ta clique on les couche tous On arrive dans l'rap tout schuss, lourd comme la patate à Mouss Diouf Drive-by en pouce-pouce, ajoute du caviar dans l'couscous Nous on porte nos couilles sans coup d'pouce On a l'vent en poupe quand toi tu pompes dans l'vent Rassasie les poucaves à coups d'pompe dans l'ventre On vend pas l'chocolat d'Genève, mais de Ouarzazate Le rap game dis-lui que ma zézète veut voir sa chatte La concurrence, on la baise, la rabaisse, mec Passe, passe le pèze, c'est tout c'qui nous apaise, mec Pousse le volume du son qui t'agresse dans ta caisse, mec Tu trouveras pas plus lourd, pas plus vrai, pas plus tess, mec Encaisse le clap comme une claque sur ta fesse, mec Personne nous teste wesh, tout l'monde nous respecte, mec Simuler des coups d'tête c'est ton premier réflexe, mec We're so hood, so bad, so ruffneck, yeah ! Tremblement d'ter-ter C'est un tremblement d'ter-ter Rebeus, Renois, Caraïs, Berbères C'est un tremblement d'ter-ter, check c'est la terre-mère Tremblement d'ter-ter C'est un tremblement d'ter-ter Kalos, Cainfris, nouches-Ma et Gwères C'est un tremblement d'ter-ter La gloire suce pour un kif, dans un J9 dégueulasse Température absolue quand le quartier se glace Ouais M.C ton rap ne casse pas des briques Donc laisse pas traîner ta serviette hygiénique dans les chiottes du Quick Reste reur-ti, meurtri par les échecs Coquards et grosses lèvres lendemain d'un jour de fête Dans chaque tiex', c'est la hass Jure pas sur la Mecque, tu veux m'la mettre je te baise Neuf-Cinq, S.O.A., Banlieue d'Paris c'est là qu'on est Ma ville tu la connais, par ici la monnaie J'veux la daronne assise a la son-mai L'khalis il doit tomber, l'raciste on va plomber Pas d'cinéma, pas d'carte UGC Barbare oui je sais, j'ai ma capuche baissée J'arrive zgègue de Galsène, j'baise de la chienne J'reste moi-même Nourou, say my name Un truc spécial pour mes cailles que j'étale sur mes cahiers J'envoie des mots comme des balles en métal vaut mieux tailler Zes' mec de tess, nous on fait trembler ton palier J'débarque, Vitry, Neuf-Quatre, on a l'talent pour t'braquer ou freestyler J'suis dans un hall, gros j'suis calé, avec l'équipe, dans une allée Mange du bitume toute l'année, veulent voir nos rôles ici caner On a choisi, on s'est cramés Par les soucis, gros j'suis gavé, viens pas m'check si t'as trop parlé T'as trop parlé, bâtard ? Nique ta mère, la chatte à ta grand-mère, bâtard On va t'niquer ta mère On va t'jeter dans une cave dans l'Neuf-Cinq Hé, Tonton Seth, j'ai huit mesures en or si tu m'l'autorises J'arrive plus lourd qu'une orgie d'sumotoris À mon mariage c'est moi qu'j'aurai l'plus beau jogging Le plus gros bolide une R19 avec un turbo d'Boeing Les MC encaissent mieux les pruneaux qu'Tony Zekwé chie des rafales d'obus, le F.C. Porto va droit au but Ouh caralhou, teste pas les cailleras d'nos rues Ou l'addition sera salée comme un accra d'morue J'arrive en balle, mon excursion sera expéditive Écoute je ne mens pas, c'est bien pour ça qu'j'obtiens l'respect des p'tits Toujours au top moi, j'ai la bonne recette On prend les mêmes et on recommence, j'te mets en transe sur l'album de Seth En une phase, le ter-ter subit un tremblement J't'ai vu dans l'angle mort, tu kiffais pas, au final t'en redemandes J'suis une bombe à retardement Ça fait brrraaah, zdedededex, ouvre pas tes fesses, j'te la mets tendrement On a des têtes comme dans l' Dernier Gang Oufs à la Spaggiari, on est des barbares, que des 7 sur le code-barre Ambiance Audiard ou Tarantino, touche pas à nos bambinos On t'aura, comme dans Gomorra cache pas l'butin sous l'Dunlopillo Demande à Al Poelvoordino wanted pour murder Nique ta mère la Police, nique ta race Fox Mulder On y croit tous comme Ribéry, fout l'dawa comme au Bayern J'baiserai la France jusqu'à c'qu'elle m'aime comme Mac Tyer C'est pour les malfrats, les ghetto youths Entre la mosquée et la muscul', ou sur Neptune via d'la ppe-fra Absolut Insolents, on sait vi-sèr' des sons lourds Prêts a salir, coûte que coûte on veut les salaires Coups d'couteau dans sa mère, l'rap crève, arme, guerre Micros en l'air, tout l'monde à terre temblement d'ter-ter C'est Aulnay, 2SK'Prod, tes potos connaissent 93.6, pé-cou tes cojones Tremblement d'ter-ter C'est un tremblement d'ter-ter Rebeus, Renois, Caraïs, Berbères C'est un tremblement d'ter-ter, check c'est la terre-mère Tremblement d'ter-ter C'est un tremblement d'ter-ter Kalos, Cainfris, nouches-Ma et Gwères C'est un tremblement d'ter-ter On roule dans des caisses d'occase, la marijuana vient d'Tijuana Les balles qu'on tire, wallah, viennent du Caucase La fumée s'propage comme des phéromones Starfoullah l'héritage qu'on a offert aux mômes Avec classe, on s'échappe par l'vasistas Face au fisc on balise pas, vu qu'à la douane les valises passent T'façon on a jamais aimé Rambo, Tarzan Nos idoles sont ceux qui vendent des kilos d'pavot afghan J'suis le côté diabolique de Serge Gainsbourg J'connais le diagnostic mais j'espère que les médecins s'gourent J'festoie fils serre-moi un verre d'vin rouge J'm'esquinte, j'souffre, j'suis quelqu'un d'louche Je fatigue Satan, crois pas qu'la Police arrive à temps Ou qu'ça tire à blanc dans la galerie marchande Je fabrique l'argent, la famille attend Qu'j'ramène entre les dents le string de Fanny Ardant Envoie les clefs du TT, j'me transforme en virtuose J'mets des grosses fessées sur des p'tits culs roses Vote pour moi sur chien-d'la-casse.fr J'te regarde de travers si tu cherches moi les vers J'pue l'Jack Daniel, j'suis l'fils caché d'Gargamel J'm'en vais danser l'disco avec deux-trois chattes d'Asnières On s'entraîne au tir au bois d'Achères, ambiance murder Pas d'voice au vocoder, c'est Giorgio Moroder Sur moi, ne lé-par pas Car chez nous la trahison ne se répare pas On prend les sens interdits T'rentre dedans comme la vachette d'Intervilles Crois pas qu'chez nous c'est fantastique À mettre la cagoule, les gants en plastique Les 'tasses de tess', c'est pas ma tasse de thé Pour les p'tis gars du Seize fais des traces de C Quand on était p'tits, les anciens nous envoyaient acheter des canettes Aujourd'hui ils nous sucent la bite pour qu'on leur avance une galette C'est la galère ouais, mais nique sa mère, on a l'feeling Investir dans un calibre c'est mieux que d'faire d'l'haltérophilie À la mairie, on leur a demandé un terrain d'foot Ils ont refusé, on s'est mis à bicrave et on a ouvert un terrain d'chnouf Bouffe pas la galette des rois, tu trouveras pas la fève J'ai vendu la galette darwa, j'ai fini au Quai des Orfèvres Laissez passer les têtes de cabochards Enfouraillés au 79, rue Quentin Bauchart Donne toujours une pièce quand tu rencontres un clochard Wesh, éteins ton char, échange pas des années d'liberté contre un bon-char En bon couche-tard, j'ai la gueule du Capitaine Caverne Va niquer ta mère si t'es un kouffar On a la même beu-bar qu'Jacques-Oussama Mess'Laden Au tier-quar on baise la mère de Papy Broussard Tremblement d'ter-ter Morsay, Seth Gueko Eh, ça vient tout droit du Neuf-Cinq, cousin Néochrome, Truands 2 La Galère On bicrave sec à Clignancourt Tu peux pas test c'est les vrais voyous, mon pote Eh l'Neuf-Cinq les vrais sauvages !You might also like</t>
         </is>
       </c>
     </row>
@@ -4776,12 +4776,12 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Trocadero</t>
+          <t>Triste Époque</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Nabz, nigga, what's up? Bellek track Jfais danser ta mère, ton père, ta cousine, c'est Mister You avec Uzi L'salaire du procureur ne vaut pas ma paire de Gucci Veulent voir la vie en rose, on va leur bicrave dla toussi Des bulles, v'là les pa-pages, sur les chèques et dans le jacuzzi Dahwa, on a trop de soucis, on a mis du Jack dans le smoothie Remballe ta gueule de shneck, remballe ta gueule d pussy J'rappe pour mes Congolais, mes Algérins, mes Mgharba Tounsi Dans la zone, j'transforme tous mes billets bleus J'suis comme on en fait plus, on fait la diff', on fait les eu' J'te laisse pas perdre, si on prend la gratte à deux Jveux tlaisser par terre, t'as vu la haine dans mes yeux On sconnaît bien mais j'suis plus trop dans les sentiments Ça vendait la mort comme à Balti' dans mon bâtiment Cinq étoiles, business class, changement d'continent Reste le même, ça sen bat les oiseaux quand tu manges J'connais l'affaire, ils vont t'trahir pour un billet J'ai des choses à faire, j'reprends ma route, j'aimerais oublier On veut l'million d'euro, million d'euro Boîte à vendre à trois-quatre zéros, trois-quatre zéros On veut l'million d'euro, million d'euro Deux-trois pièces au Trocadéro, Trocadéro, eh, eh You might also like Tu lui dis je t'aime habibi, elle t'demande combien tu poses pour la dote Donc y'a qu'nos mères qu'on aime, et il n'y'a qu'Allah qu'on adore Pied au plancher, j'suis déjà à 3.40, même Bugs Bunny s'est fait carotte Ce qui fait l'homme, c'est la parole ce qui fait l'homme, c'est la parole C'est pour de vrai quand ça rafale, devant les keufs, ça parlera pas J'continue, c'est pas pour l'rap, c'est pour faire rentrer des oiseaux Regarder mon fils graille le gratin, quand sur ces catins Debout à seize heures, tous les matins, j'suis trop loin plus rien ne m'atteint T'as ouvert ton clapet, ils s'étaient broliqués, wow, yo, yo, yo T'as joué les cros-ma, tu t'es fais niquer, wow, yo, yo, yo On s'connaît bien mais j'suis plus trop dans les sentiments Ça vendait la mort comme à Balti' dans mon bâtiment Cinq étoiles, business class, changement d'continent Reste le même, ça s'en bat les oiseaux quand tu manges J'connais l'affaire, ils vont t'trahir pour un billet J'ai des choses à faire, j'reprends ma route, j'aimerais oublier On veut l'million d'euro, million d'euro Boîte à vendre à trois-quatre zéros, trois-quatre zéros On veut l'million d'euro, million d'euro Deux-trois pièces au Trocadéro, Trocadéro, eh, eh</t>
+          <t>11ème 19ème 20ème Triste époque mon pote ! Eh ouuuais aaaaaaaaaaaaaah tention' Bébébébélleville Wesh dahwa parait que ta fait ton halal zooogataga Psartek en ce qui m'concerne moi J'ai fait le haram avec ma rue quand j'ai bédave ma première barrette On s'est marié direct le jour où j'ai bicrave la première galette C'est pour les braves comme Nas, comme Sidyou, comme Toumi, Khaled À tous ceux que j'aurais oublié les mecs qui auront su m'venir en aide Khabta mon bien être j'suis pas net j'fuck toute la planète Y'a trop de sky dans ma canette regarde ma gueule sur internet À trop écouter du rap de merde tu peux en devenir carrément sourd J'regarde ma montre Ohh il est dejà l'heure j'big up Shakar El Mansour Triste Epoque, mon pote le monde il part en glawi oui oui J'me verrai bien au bled avec Abderrazak El Mahraoui Blanchir juste un lion-mi léjéh el baraka L'rap français pour moi c'est comme du bachi pour un maraka J'oublie pas No Times Records Boubakar Tristan Comme dit Wisla fuck les bâtards qu'ils fument tout seul leurs tipisla Un conseil joue pas le voyou arrête le rap et fais du basket C'est Mister You sur écoute comme Avon barksdale You might also like Woogataga le refré Yaston À Slimane a Souleymane, ah woogatabraaaaaaaaaaaaaaaa J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assess Triste époque mon pote j'te jure demande à Aladin J'fume du seum, j'ai du plomb et donc du monde dans la tête Les mecs pour une barrette ils te mettent une peine exemplaire Rachida il faut qu'elle s'en va, Sarko faut qui nique son père J'me sens seul comme cette goutte d'huile dans l'océan J'essaie en vain de rentabiliser les séances Là j'tourne en rond autant qu'un taulard en promenade Ou un mec qui cherche un bête de taf, mais qu'a le teint trop mat Moi quand j'sors de gard'av c'est que j'rentre au placard V.I.P en chaussette, nique les 3asses bande de batard Ils sont là pour t'faire la misère fouille cellulaire à 6h J'ai pas le profil de l'auxiliaire moi c'est pour ça qu'ils m'ont dans le viseur Le rôle j'vais m'l'accaparer çà j'te l'dit fih seh Y'a plus de coke à Paris qu'y a de neige dans le Val dIsère C'est Mister Youu Gataga pour les intimes Pour tous les mecs cramés, comme les dramé baka ou Latifi J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses J'suis pas enrayé comme une kalash datant de l'ex U.R.S.S Briiidchal j'prends 20 ans j'serais obligé de tuer un 3assses1</t>
         </is>
       </c>
     </row>
@@ -4793,12 +4793,12 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>TROIS PETITS CHATS</t>
+          <t>Trocadero</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Ok, j'commence tout doux j'big up le roc-Ma Mamadou Comme il dit woogataga Mister You do what you gonna do Vas-y fous le feu tant que tu représentes Belleville-Zoo Et tant que les gens de la zone se rassasient chez toi et Bazoo Demande à Sanbou, à Siyabou, à Hibou, à Chikabou Comment faire pour s'en sortir quand c'est le système qui nous pousse à bout ? J'sais qu'une cave-pou au ste-po ça fait pas de crise d'épilepsie Ça ravale pas sa langue nan ça surveille pas son lexique Comme dit Nass Belleville c'est aud-ch y'a plus de keufs qu'à l'avenue Foch Les RG ça pourrait être tes proches alors conseil surveille tes poches J'ai fait du flouze big up Pinus Madifili J'sais qu'investir dans une rafleuse c'est mieux qu'faire de l'haltérophilie Williams Tookie beh il a la même mort que Zied et Bouna Les coups de talkies moi j'en ai mangé j'avais de la khnouna C'est Mister You là, mauvaise graine de Belleville zoo là Seule femme que j'aime c'est celle qui m'a fait tété l'bzoula Quiero un poco de vodka con zumo de naranja C'est Mister Yougataga moi j'ai grandi dans le khra Dans le haram à Paris pas à Marly-Gomont Crois-moi pour percer j'aurais pas un style ta3 les gol-mon J'compte démonter les barrières nique la mère aux détectives Avec Lajdi et Bakaou derrière c'est impossible tu peux test Yves Envers la race humaine j'aurais peut être un peu d'estime frère Quand l'état d'Israël il s'appellera enfin Palestine J'aime pas les stups Woogataga depuis belle lurette c'est déclaré C'est moi le king qui maque la reine je suis Räikkönnen sans McLaren Mon Dieu tout comme Mathieu j'compte réussir avec la haine Et si j'y arrive pas c'est qu'un bâtard ma mis l'3ain À la barre prendre une peine à 2 chiffre ça me ferait de la peine Au placard tout comme la bête bah j'rêverais que de me faire la belle Le seum et la beuh c'est mon label je vend de la wawa je suis producteur J'représente les hors-la-loi je suis leur traducteur Fuck les pointeurs les boycotteurs ainsi que les menteurs Sur le ter-ter quand ça détourne fuck le trois quart des rabatteurs Ma première phrase au loir-pa c'est j'espère lghosba moujoud L'avenir m'appartient pas pourtant je suis debout depuis l'eau chaude Nique les juges, la justice les stups et j'insinue Que c'est bien des fils de putes car fallait pas me mettre en cellule Voir toutes ces lunes graviter, en solo cogiter Méditer à m'demander quand liberté voudra m'inviter À péter les plombs impressionner l'auxi-télé L'argent fait pas le bonheur mais ça attire les putes même si t'es laid Cette année il y a des MC qui vont gouter une sale tannée J'compte m'installer, fuck M6 vive Hassan Tani J'rackette que le pe-ra mon meilleur sport c'est le tennis C'est pas aux anglais la promenade t'as cru que le shtar c'était Nice Fuck la police et les poucaves qui leur tapent des te-po Moi mes seuls autographes c'est la gard'av' où le mandat de dépôt C'est Youuugataga alias Latifi pour les 3essess J'suis à la recherche d'une fille bien pour faire passer 10 kilos de cess Bientôt le sperme y pourra se crave-bi tellement y'a des lahèss Yasse7 au tar-mi on a tous rencard avec la hass On sort pas de la tèce non non on reste H24 dedans On rêve que de Benz et de Runner 180 deux temps Tout le temps faya Thug Life formée par 2Pac Shakur Dédié à Daddy, à tout le quartier à mon poto Shakir J'vois que les petits ils tirent plus d'un sac devant ma tour J'ai plus d'un tour dans mon sac y'a plus d'un shlag devant ma tour Un marocain quand il va s'baigner même un requin il crie au secours Il a pas besoin de costard mais d'un gros z'déh pour les discours On sera pas hardcore en étant cool les heures passent le temps coule Les médias salissent l'islam on encule la race à Betancourt grosse salope Dédicace à Yass alias le renard dans la basse cour Bazou et oi-m on brasse des liasses donc à notre vue les pétasses courent Vu qu'souris, il est sur le ter-ter vers orto ça miaule comme des chats J'vends de la mort j'sors avec Aicha Qandisha Fasciné par l'pavé beh même les gosses ils veulent vendre Be-belleville on a tous les couilles plus grosses que le ventre Fasciné par l'pavé beh même les gosses ils veulent vendre Be-belleville on a tous les couilles plus grosses que le ventre Fasciné par l'pavé beh même les gosses ils veulent vendre Be-belleville on a tous les couilles plus grosses que le ventre You might also like Quiere un poco de vokda con zumo de naranja C'est Mister Yougataga moi j'ai grandi dans le khra Dans le haram à Paris pas à Marly-Gomont Crois-moi pour percer j'aurais pas un style tah les gol-mon Quiere un poco de vodka con zumo de naranja C'est Mister Yougataga moi j'ai grandi dans le khra Dans le haram à Paris pas à Marly-Gomont À croire que pour percer il faut avoir un style ta3 les gol-mon</t>
+          <t>Nabz, nigga, what's up? Bellek track Jfais danser ta mère, ton père, ta cousine, c'est Mister You avec Uzi L'salaire du procureur ne vaut pas ma paire de Gucci Veulent voir la vie en rose, on va leur bicrave dla toussi Des bulles, v'là les pa-pages, sur les chèques et dans le jacuzzi Dahwa, on a trop de soucis, on a mis du Jack dans le smoothie Remballe ta gueule de shneck, remballe ta gueule d pussy J'rappe pour mes Congolais, mes Algérins, mes Mgharba Tounsi Dans la zone, j'transforme tous mes billets bleus J'suis comme on en fait plus, on fait la diff', on fait les eu' J'te laisse pas perdre, si on prend la gratte à deux Jveux tlaisser par terre, t'as vu la haine dans mes yeux On sconnaît bien mais j'suis plus trop dans les sentiments Ça vendait la mort comme à Balti' dans mon bâtiment Cinq étoiles, business class, changement d'continent Reste le même, ça sen bat les oiseaux quand tu manges J'connais l'affaire, ils vont t'trahir pour un billet J'ai des choses à faire, j'reprends ma route, j'aimerais oublier On veut l'million d'euro, million d'euro Boîte à vendre à trois-quatre zéros, trois-quatre zéros On veut l'million d'euro, million d'euro Deux-trois pièces au Trocadéro, Trocadéro, eh, eh You might also like Tu lui dis je t'aime habibi, elle t'demande combien tu poses pour la dote Donc y'a qu'nos mères qu'on aime, et il n'y'a qu'Allah qu'on adore Pied au plancher, j'suis déjà à 3.40, même Bugs Bunny s'est fait carotte Ce qui fait l'homme, c'est la parole ce qui fait l'homme, c'est la parole C'est pour de vrai quand ça rafale, devant les keufs, ça parlera pas J'continue, c'est pas pour l'rap, c'est pour faire rentrer des oiseaux Regarder mon fils graille le gratin, quand sur ces catins Debout à seize heures, tous les matins, j'suis trop loin plus rien ne m'atteint T'as ouvert ton clapet, ils s'étaient broliqués, wow, yo, yo, yo T'as joué les cros-ma, tu t'es fais niquer, wow, yo, yo, yo On s'connaît bien mais j'suis plus trop dans les sentiments Ça vendait la mort comme à Balti' dans mon bâtiment Cinq étoiles, business class, changement d'continent Reste le même, ça s'en bat les oiseaux quand tu manges J'connais l'affaire, ils vont t'trahir pour un billet J'ai des choses à faire, j'reprends ma route, j'aimerais oublier On veut l'million d'euro, million d'euro Boîte à vendre à trois-quatre zéros, trois-quatre zéros On veut l'million d'euro, million d'euro Deux-trois pièces au Trocadéro, Trocadéro, eh, eh</t>
         </is>
       </c>
     </row>
@@ -4810,12 +4810,12 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>VACANZA A MARBELLA</t>
+          <t>TROIS PETITS CHATS</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>Et ça fait rom pom pom j'suis dans l'carré Elle est belle, elle est bonne j'vais la démarrer Et ça fait rom pom pom j'suis dans l'carré Elle est belle, elle est bonne j'vais la démarrer J't'ai tout donné mais t'as douté d'moi Maintenant dans mon cur tout est noir J'ai déjà enfreint toutes les lois J'ai tourné j'ai coffré l'pénav J'ai pas vendu des cinquenta C'est moi qui paie toutes les cuenta Dans le VIP d'Olivia Valere Versace jusque sur l'peignoir J'ai sorti un gros gamos J'descends sur Puerto Bañus J'vais rjoindre mes hermanos Ma p'tit andalouse est jalouse Ma p'tite andalouse est jalouse J'passe les vacances à Marbella You might also like J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza a Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Partito dalla cite Oui oui, comment tu t'appelles Ma chérie, je suis italien Con il binks binks, fino a Malaga Ah Marbella, All' Habana Jack Daniel's le sere mon bebe Quiere fumar conmigo Amigo, mentalita' don Vito Una bebecita zero cellulite a Cadiz Vetri neri sopra l'AMG Mangio pasta al Olivia Valere Otto mafia tu non sei mio frere Philip, Mister You, Hayce Lemsi J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Meute de loups suivie par des hyènes Sdeh Marocain chemise Italienne J'passe de l'opinel à la mitraillette Le jet s'arrête à l'hôtel Hyat Pour un dollar c'est lance-roquettes Ou finir en chien graille des croquettes Y a un gros calibre dans les discothèques Genre du si j'veux je rentre en claquettes J'ai sorti un gros gamos J'descends sur Puerto Bañus J'vais rejoindre mes hermanos Ma p'tite andalouse est jalouse Ma p'tite andalouse est jalouse J'passe les vacances à Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella</t>
+          <t>Ok, j'commence tout doux j'big up le roc-Ma Mamadou Comme il dit woogataga Mister You do what you gonna do Vas-y fous le feu tant que tu représentes Belleville-Zoo Et tant que les gens de la zone se rassasient chez toi et Bazoo Demande à Sanbou, à Siyabou, à Hibou, à Chikabou Comment faire pour s'en sortir quand c'est le système qui nous pousse à bout ? J'sais qu'une cave-pou au ste-po ça fait pas de crise d'épilepsie Ça ravale pas sa langue nan ça surveille pas son lexique Comme dit Nass Belleville c'est aud-ch y'a plus de keufs qu'à l'avenue Foch Les RG ça pourrait être tes proches alors conseil surveille tes poches J'ai fait du flouze big up Pinus Madifili J'sais qu'investir dans une rafleuse c'est mieux qu'faire de l'haltérophilie Williams Tookie beh il a la même mort que Zied et Bouna Les coups de talkies moi j'en ai mangé j'avais de la khnouna C'est Mister You là, mauvaise graine de Belleville zoo là Seule femme que j'aime c'est celle qui m'a fait tété l'bzoula Quiero un poco de vodka con zumo de naranja C'est Mister Yougataga moi j'ai grandi dans le khra Dans le haram à Paris pas à Marly-Gomont Crois-moi pour percer j'aurais pas un style ta3 les gol-mon J'compte démonter les barrières nique la mère aux détectives Avec Lajdi et Bakaou derrière c'est impossible tu peux test Yves Envers la race humaine j'aurais peut être un peu d'estime frère Quand l'état d'Israël il s'appellera enfin Palestine J'aime pas les stups Woogataga depuis belle lurette c'est déclaré C'est moi le king qui maque la reine je suis Räikkönnen sans McLaren Mon Dieu tout comme Mathieu j'compte réussir avec la haine Et si j'y arrive pas c'est qu'un bâtard ma mis l'3ain À la barre prendre une peine à 2 chiffre ça me ferait de la peine Au placard tout comme la bête bah j'rêverais que de me faire la belle Le seum et la beuh c'est mon label je vend de la wawa je suis producteur J'représente les hors-la-loi je suis leur traducteur Fuck les pointeurs les boycotteurs ainsi que les menteurs Sur le ter-ter quand ça détourne fuck le trois quart des rabatteurs Ma première phrase au loir-pa c'est j'espère lghosba moujoud L'avenir m'appartient pas pourtant je suis debout depuis l'eau chaude Nique les juges, la justice les stups et j'insinue Que c'est bien des fils de putes car fallait pas me mettre en cellule Voir toutes ces lunes graviter, en solo cogiter Méditer à m'demander quand liberté voudra m'inviter À péter les plombs impressionner l'auxi-télé L'argent fait pas le bonheur mais ça attire les putes même si t'es laid Cette année il y a des MC qui vont gouter une sale tannée J'compte m'installer, fuck M6 vive Hassan Tani J'rackette que le pe-ra mon meilleur sport c'est le tennis C'est pas aux anglais la promenade t'as cru que le shtar c'était Nice Fuck la police et les poucaves qui leur tapent des te-po Moi mes seuls autographes c'est la gard'av' où le mandat de dépôt C'est Youuugataga alias Latifi pour les 3essess J'suis à la recherche d'une fille bien pour faire passer 10 kilos de cess Bientôt le sperme y pourra se crave-bi tellement y'a des lahèss Yasse7 au tar-mi on a tous rencard avec la hass On sort pas de la tèce non non on reste H24 dedans On rêve que de Benz et de Runner 180 deux temps Tout le temps faya Thug Life formée par 2Pac Shakur Dédié à Daddy, à tout le quartier à mon poto Shakir J'vois que les petits ils tirent plus d'un sac devant ma tour J'ai plus d'un tour dans mon sac y'a plus d'un shlag devant ma tour Un marocain quand il va s'baigner même un requin il crie au secours Il a pas besoin de costard mais d'un gros z'déh pour les discours On sera pas hardcore en étant cool les heures passent le temps coule Les médias salissent l'islam on encule la race à Betancourt grosse salope Dédicace à Yass alias le renard dans la basse cour Bazou et oi-m on brasse des liasses donc à notre vue les pétasses courent Vu qu'souris, il est sur le ter-ter vers orto ça miaule comme des chats J'vends de la mort j'sors avec Aicha Qandisha Fasciné par l'pavé beh même les gosses ils veulent vendre Be-belleville on a tous les couilles plus grosses que le ventre Fasciné par l'pavé beh même les gosses ils veulent vendre Be-belleville on a tous les couilles plus grosses que le ventre Fasciné par l'pavé beh même les gosses ils veulent vendre Be-belleville on a tous les couilles plus grosses que le ventre You might also like Quiere un poco de vokda con zumo de naranja C'est Mister Yougataga moi j'ai grandi dans le khra Dans le haram à Paris pas à Marly-Gomont Crois-moi pour percer j'aurais pas un style tah les gol-mon Quiere un poco de vodka con zumo de naranja C'est Mister Yougataga moi j'ai grandi dans le khra Dans le haram à Paris pas à Marly-Gomont À croire que pour percer il faut avoir un style ta3 les gol-mon</t>
         </is>
       </c>
     </row>
@@ -4827,12 +4827,12 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Vie de voyou</t>
+          <t>VACANZA A MARBELLA</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>La nouvelle école décolle future patronne du rap Chez nous ca bicrave tous c'qui s'fume nique sa mère les biens durables Négro ca vient du zoo tous les frelots s'mette debout Pour les darons qu'on deux femmes dix gosses mais qu'arrive pas à joindre les deux bouts Elle est loin l'insouciance d'la maternelle Maintenant mes potes plaident coupable rien est éternel Si tu poucaves les coups partent et tu l'sais rheys Les problèmes partent mais reviennent agravés et tu l'sais rheys Le 7.5 c'est frais zinks surtout quand t'as du bif L'argent fait pas l'bonheur c'est que si j'en ai qu'j'vais t'le dire Mais j'me sens seul sans ça comme Gainsbourg sans sa Havanne Lil Wayne sans son sureau Biggie sans sa canne Négro on cherche ça on cherche les dames on cherche le drame En gros on cherche la merde comme un mec bourré en boîte Pour régler ça dans les équipes toujours un casse machoire Si c'est pas avec 10 keums c'est avec un gun qu'on marche le soir On vent d'la merde pour sortir de la merde Les clients veulent donc on les sert monsieur le commissaire On n'est pas fou ni saoul tout c'qu'on veut nous c'est des sous Zoogataga mon pote dahwa c'est l'rap tah les voyous x2 2010 faites de la place que j'pète le tympan des puristes Putain putain d'dédicaces a tous les frérots qui prennent des risques Qui s'en battent les cojones qui restent posés sur l'pavé J'me présente moi c'est Youness c'lui qui r'ssort jamais d'GAV J't'ai dis surveille tes seufs j'suis d'ceux qui rentre direct au hebs A 200 000 Km dahwa j'peut t'dire qu'ca va très deus Aïe aïe aïe Saddam Husen non il est pas mort C'est la vengeance d'la guerre du golfe j'enfonce un club dans l'bide des porcs J'suis venu sodomisé leur maman l'rap j'suis comme son médicaments D'mande à Fialso ou bien Still fresh comment on représente nos département? C'est hasta la muerte comue Guevara cha Hasta la victoria siempre comme dirait Da Djé Het p'tit sur la mecque sa rigole ap Et sur la tombe de mon grand pere qu'on nique la mere a c'putain d'rap Dahwa c'est d'la frappe donc faut l'écouter par le zen J'répete c'est d'la frappe don c c'est normal que ca passe creme You might also likeOn vent d'la merde pour sortir de la merde Les clients veulent donc on les sert monsieur le commissaire On n'est pas fou ni saoul tout c'qu'on veut nous c'est des sous Zoogataga mon pote dahwa c'est l'rap tah les voyous x2 Le rap c'était mieux avant jusqu'a c'que You et Fresh arrive Deux gars qui cherche du liquide pour arrosé nos terre aride Man ils nous font perdre la santé on nous enferment a Bois D'Arcy La mauvaise graine a frennes et c'est plus de haine qui fleuris On perd trop d'espoir dans cette vie la Moi j'veux vite croire au mot victoire Donc fuck la proc appelle tes potes défoce les portes Pour qui nous entendes desfois obligé d'lancer l'coktail molotov Merde un con gamberge Un seul faux pas et tu peut etre a 20 000 lieues dans la merde Nouvelle école ca vient d'Paris pur black MC Dis pas qu't'aime si mon teint t'gene comme un barbu dans un jet petit T'attache pas a la vie c'est une garce on m'a dit Que des gars qui médisent et des tass qui font les garcons manqués Pff dédicace a Mister You Une vie d'voyou implique des peines de voyous On vent d'la merde pour sortir de la merde Les clients veulent donc on les sert monsieur le commissaire On n'est pas fou ni saoul tout c'qu'on veut nous c'est des sous Zoogataga mon pote dahwa c'est l'rap tah les voyous x4</t>
+          <t>Et ça fait rom pom pom j'suis dans l'carré Elle est belle, elle est bonne j'vais la démarrer Et ça fait rom pom pom j'suis dans l'carré Elle est belle, elle est bonne j'vais la démarrer J't'ai tout donné mais t'as douté d'moi Maintenant dans mon cur tout est noir J'ai déjà enfreint toutes les lois J'ai tourné j'ai coffré l'pénav J'ai pas vendu des cinquenta C'est moi qui paie toutes les cuenta Dans le VIP d'Olivia Valere Versace jusque sur l'peignoir J'ai sorti un gros gamos J'descends sur Puerto Bañus J'vais rjoindre mes hermanos Ma p'tit andalouse est jalouse Ma p'tite andalouse est jalouse J'passe les vacances à Marbella You might also like J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza a Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Partito dalla cite Oui oui, comment tu t'appelles Ma chérie, je suis italien Con il binks binks, fino a Malaga Ah Marbella, All' Habana Jack Daniel's le sere mon bebe Quiere fumar conmigo Amigo, mentalita' don Vito Una bebecita zero cellulite a Cadiz Vetri neri sopra l'AMG Mangio pasta al Olivia Valere Otto mafia tu non sei mio frere Philip, Mister You, Hayce Lemsi J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Meute de loups suivie par des hyènes Sdeh Marocain chemise Italienne J'passe de l'opinel à la mitraillette Le jet s'arrête à l'hôtel Hyat Pour un dollar c'est lance-roquettes Ou finir en chien graille des croquettes Y a un gros calibre dans les discothèques Genre du si j'veux je rentre en claquettes J'ai sorti un gros gamos J'descends sur Puerto Bañus J'vais rejoindre mes hermanos Ma p'tite andalouse est jalouse Ma p'tite andalouse est jalouse J'passe les vacances à Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella Sono in vacanza Marbella J'passe les vacances à Marbella</t>
         </is>
       </c>
     </row>
@@ -4844,12 +4844,12 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Vieille meuf</t>
+          <t>Vie de voyou</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>J'suis déconseillé aux mines-ga Aux michtonneuses et de manière générale A toutes les meufs zine-ga J'ai pas de temps et encore moins de tunes à perdre Donc si t'es bonne et que tu frimes pas, faut que tu m'appelles John Steed Espèce de vieille meuf, t'as senti l'odeur des tunes et des véhicules Ca y est, t'es prête à échanger ton cul Mister You Espèce de vieille meuf, j'voulais t'laisser mon numéro Tu m'as dit OK mais si de côté t'a mis au moins 100 000 euros Dry Espèce de vieille meuf, ici nos sacs sont remplis de billets Tu veux ton Louis Vuitton? Viens taffer, on va te rhabiller Wira Espèce de vieille meuf, si y'a que les biftons qui t'attirent Arrête de faire des manières et viens nous faire une petite gâterie J'suis pas un plouc arrache toi Je chante pas la Cucaracha Moi j'suis un loup, j'tire mon coup et j'natchave C'est aussi simple que d'dire bonjour Tu t'es fais belle coquine, là c'est sur ton boule qu'on zoome Dis-le moi si ça te déplait, arrête de faire ta mijaurée steuplait J'te manque pas d'respect, tu fais exprès, j'ai cramé ton vice Je sais bien où tu veux en venir mais oublie c'est pas méthodique C'est bon, on les connait les meufs comme toi Qui font leurs coups en douce et ont des airs de psychopathe Tu trompes ton gars avec le premier venu Tu seras bien près de mes burnes, attends que je m'occupe de ton cas là Et puis merde, j'm'en tape, t'as 2 ans d'âge mental Les ta-tass comme toi ça court les rues J'préfère les filles sérieuses qui se respectent Pas celles qui se laissent faire et qui se comportent comme des chiennes J'balance des 16 en vrac pour les gros comiques qui m'font gol-ri Lorsqu'ils me parlent d'hydroponic C'est Wira Zaka, enchanté mesdames et mesdames J'me fous de leurs médailles, venez juste embrasser mes burnes You might also like John Steed Espèce de vieille meuf, t'as senti l'odeur des tunes et des véhicules Ca y est, t'es prête à échanger ton cul Dry Espèce de vieille meuf, ici nos sacs sont remplis de billets Tu veux ton Louis Vuitton? Viens taffer, on va te rhabiller Wira Espèce de vieille meuf, si y'a que les biftons qui t'attirent Arrête de faire des manières et viens nous faire une petite gâterie Mister You Espèce de vieille meuf, j'voulais t'laisser mon numéro Tu m'as dit OK mais si de côté t'a mis au moins 100 000 euros Madame n'est pas une michtonneuse mais elle n'sort pas avec les pauvres Il en faut plein pour être heureuse, elle ouvre son cur devant une clé de coffre Elle est pas là pour ton argent car c'est clair, elle préfère l'or A la recherche de l'espoir, rallume tes phares, il pourrait faire noir Woogataga, j'ai vu et là j'vous raconte ce qu'elles m'ont fait voir Elles m'ont montré que l'avenir rime avec gent-ar donc désespoir Si timide puis si vulgaire, si si, j'vous pousse à l'croire C'est le nerf de la guerre, wallah les meufs c'est que des histoires La vérité c'est peu plaisant, c'est blessant tels des rasoirs La liberté s'cache en prison, si j'guide mon peuple ça s'ra dérisoire On dirait le soir dans ma tête même quand il est 14 heures Une folle m'a dit faut faire la fête, c'est à bronzer que l'équateur sert Dieu est grand, le monde est petit, tu connais tous les coins tah sah Yes, sah el sbah, sans mascara t'as l'air bizarre Une fois à l'hotel bah tu ressort plus avant 13 heures C'est plus Lancôme ton trésor vu que t'as l'cul dans le compresseur Et c'est le désordre dans ta tête et encore t'as que 20 piges T'as une reput' de vraie pute mais bon toi tu t'en fiches Tu veux être riche, shab tu sniffes, tu veux faire partie d'la jet-set Tu mérites qu'un tour d'YZ, espèce de vieille khenzete John Steed Espèce de vieille meuf, t'as senti l'odeur des tunes et des véhicules Ca y est, t'es prête à échanger ton cul Mister You Espèce de vieille meuf, j'voulais t'laisser mon numéro Tu m'as dit OK mais si de côté t'a mis au moins 100 000 euros Wira Espèce de vieille meuf, si y'a que les biftons qui t'attirent Arrête de faire des manières et viens nous faire une petite gâterie Dry Espèce de vieille meuf, ici nos sacs sont remplis de billets Tu veux ton Louis Vuitton? Viens taffer, on va te rhabiller Moi j'kiffe pas les fouffes qui ont une bite dans le veau-cer Une liasse à la place du cur, qui s'frottent devant les gangsters Les Holster de ma garde les font mouiller En soirée, sous vodka, ma clique elles aimeraient souiller Espèce de vieille meuf, tu m'as rodave avec une poupée genre Halle Berry Comme Vanessa, t'as choqué J'ai pare-choqué la rue avec mes rimes et mes crochets Les crasseuses s'accrochent à mon zgeg comme un trophée Elles en ont trop fait, cramées comme les vil-ci Hassoul, par tié-pi, cassez-vous loin d'ici Laissez donc la place à ses dames qui ont la classe Qui déclassent la number one des michtos en place J'vous fracasse a coup de hanches Veux tu ton x dans le merco benz, dans ton benz La puissance du beau negro, après mon passage tu crieras Woogataga Nous ce qu'on aime c'est les boules qui s'font pas hagra, mon gars John Steed Espèce de vieille meuf, t'as senti l'odeur des tunes et des véhicules Ca y est, t'es prête à échanger ton cul Mister You Espèce de vieille meuf, j'voulais t'laisser mon numéro Tu m'as dit OK mais si de côté t'a mis au moins 100 000 euros Wira Espèce de vieille meuf, si y'a que les biftons qui t'attirent Arrête de faire des manières et viens nous faire une petite gâterie Dry Espèce de vieille meuf, ici nos sacs sont remplis de billets Tu veux ton Louis Vuitton? Viens taffer, on va te rhabiller</t>
+          <t>La nouvelle école décolle future patronne du rap Chez nous ca bicrave tous c'qui s'fume nique sa mère les biens durables Négro ca vient du zoo tous les frelots s'mette debout Pour les darons qu'on deux femmes dix gosses mais qu'arrive pas à joindre les deux bouts Elle est loin l'insouciance d'la maternelle Maintenant mes potes plaident coupable rien est éternel Si tu poucaves les coups partent et tu l'sais rheys Les problèmes partent mais reviennent agravés et tu l'sais rheys Le 7.5 c'est frais zinks surtout quand t'as du bif L'argent fait pas l'bonheur c'est que si j'en ai qu'j'vais t'le dire Mais j'me sens seul sans ça comme Gainsbourg sans sa Havanne Lil Wayne sans son sureau Biggie sans sa canne Négro on cherche ça on cherche les dames on cherche le drame En gros on cherche la merde comme un mec bourré en boîte Pour régler ça dans les équipes toujours un casse machoire Si c'est pas avec 10 keums c'est avec un gun qu'on marche le soir On vent d'la merde pour sortir de la merde Les clients veulent donc on les sert monsieur le commissaire On n'est pas fou ni saoul tout c'qu'on veut nous c'est des sous Zoogataga mon pote dahwa c'est l'rap tah les voyous x2 2010 faites de la place que j'pète le tympan des puristes Putain putain d'dédicaces a tous les frérots qui prennent des risques Qui s'en battent les cojones qui restent posés sur l'pavé J'me présente moi c'est Youness c'lui qui r'ssort jamais d'GAV J't'ai dis surveille tes seufs j'suis d'ceux qui rentre direct au hebs A 200 000 Km dahwa j'peut t'dire qu'ca va très deus Aïe aïe aïe Saddam Husen non il est pas mort C'est la vengeance d'la guerre du golfe j'enfonce un club dans l'bide des porcs J'suis venu sodomisé leur maman l'rap j'suis comme son médicaments D'mande à Fialso ou bien Still fresh comment on représente nos département? C'est hasta la muerte comue Guevara cha Hasta la victoria siempre comme dirait Da Djé Het p'tit sur la mecque sa rigole ap Et sur la tombe de mon grand pere qu'on nique la mere a c'putain d'rap Dahwa c'est d'la frappe donc faut l'écouter par le zen J'répete c'est d'la frappe don c c'est normal que ca passe creme You might also likeOn vent d'la merde pour sortir de la merde Les clients veulent donc on les sert monsieur le commissaire On n'est pas fou ni saoul tout c'qu'on veut nous c'est des sous Zoogataga mon pote dahwa c'est l'rap tah les voyous x2 Le rap c'était mieux avant jusqu'a c'que You et Fresh arrive Deux gars qui cherche du liquide pour arrosé nos terre aride Man ils nous font perdre la santé on nous enferment a Bois D'Arcy La mauvaise graine a frennes et c'est plus de haine qui fleuris On perd trop d'espoir dans cette vie la Moi j'veux vite croire au mot victoire Donc fuck la proc appelle tes potes défoce les portes Pour qui nous entendes desfois obligé d'lancer l'coktail molotov Merde un con gamberge Un seul faux pas et tu peut etre a 20 000 lieues dans la merde Nouvelle école ca vient d'Paris pur black MC Dis pas qu't'aime si mon teint t'gene comme un barbu dans un jet petit T'attache pas a la vie c'est une garce on m'a dit Que des gars qui médisent et des tass qui font les garcons manqués Pff dédicace a Mister You Une vie d'voyou implique des peines de voyous On vent d'la merde pour sortir de la merde Les clients veulent donc on les sert monsieur le commissaire On n'est pas fou ni saoul tout c'qu'on veut nous c'est des sous Zoogataga mon pote dahwa c'est l'rap tah les voyous x4</t>
         </is>
       </c>
     </row>
@@ -4861,12 +4861,12 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Viens pas test</t>
+          <t>Vieille meuf</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>AAAAAh attention B.I.L.E.L Mr Yougataga John Steed petrodollar AAAAAAAH, bbrrrrrraaaa Belleville viens surtout pas test l'équipe Le ptit yas Un coup de fil, on débarque on t'baise, on t'liquide Dédicace Belleville viens surtout pas test l'équipe Belleville Un coup de fil, on débarque on t'baise, on t'liquide Zooogatagaaa J'fais mon entrée dans la cabine Un peu comme un boxeur J'volais déjà tout à la cantine On m'a pas élevé chez les bonnes surs Y'a ceux qui volent, ceux qui dealent, ceux qui braquent et les bosseurs Y'a ceux qui sautent, ceux qui tirent, ceux qui parlent et les crosseurs pour protester Tandis que nous on s'amuse Tout ceux qui viendront pour tester Repartiront avec le S.A.M.U T'as le flow de l'abbé Pierre, avec un tout ptit duvet T'as rien à faire dans le RAP comme un black dans un salon d'UV Arrêtes de m'parler de coke On t'a fait sniffer de la craie mec On a cramé ta loc', nous fait pas croire que t'es un mec de grec Aaaah hoooougataga Nous on bicrave sous la grêle Les boloss se grattent les veines quand au quartier on fait la grève Le 34 des rappeurs sucent des bites à crédit Ils veulent pas me faire d'la place par peur de pointer aux ASSEDICS J'sais pas pour qui ils se prennent, mais ils sont pas si terribles Si mon flow avait des mains, il aurait déjà baffé tes rimes You might also likeBelleville viens surtout pas test l'équipe Un coup de fil, on débarque on t'baise, on t'liquide Belleville viens surtout pas test l'équipe Un coup de fil, on débarque on t'baise, on t'liquide Belleville viens surtout pas test l'équipe Un coup de fil, on débarque on t'baise, on t'liquide Belleville viens surtout pas test l'équipe Un coup de fil, on débarque on t'baise, on t'liquide ...</t>
+          <t>J'suis déconseillé aux mines-ga Aux michtonneuses et de manière générale A toutes les meufs zine-ga J'ai pas de temps et encore moins de tunes à perdre Donc si t'es bonne et que tu frimes pas, faut que tu m'appelles John Steed Espèce de vieille meuf, t'as senti l'odeur des tunes et des véhicules Ca y est, t'es prête à échanger ton cul Mister You Espèce de vieille meuf, j'voulais t'laisser mon numéro Tu m'as dit OK mais si de côté t'a mis au moins 100 000 euros Dry Espèce de vieille meuf, ici nos sacs sont remplis de billets Tu veux ton Louis Vuitton? Viens taffer, on va te rhabiller Wira Espèce de vieille meuf, si y'a que les biftons qui t'attirent Arrête de faire des manières et viens nous faire une petite gâterie J'suis pas un plouc arrache toi Je chante pas la Cucaracha Moi j'suis un loup, j'tire mon coup et j'natchave C'est aussi simple que d'dire bonjour Tu t'es fais belle coquine, là c'est sur ton boule qu'on zoome Dis-le moi si ça te déplait, arrête de faire ta mijaurée steuplait J'te manque pas d'respect, tu fais exprès, j'ai cramé ton vice Je sais bien où tu veux en venir mais oublie c'est pas méthodique C'est bon, on les connait les meufs comme toi Qui font leurs coups en douce et ont des airs de psychopathe Tu trompes ton gars avec le premier venu Tu seras bien près de mes burnes, attends que je m'occupe de ton cas là Et puis merde, j'm'en tape, t'as 2 ans d'âge mental Les ta-tass comme toi ça court les rues J'préfère les filles sérieuses qui se respectent Pas celles qui se laissent faire et qui se comportent comme des chiennes J'balance des 16 en vrac pour les gros comiques qui m'font gol-ri Lorsqu'ils me parlent d'hydroponic C'est Wira Zaka, enchanté mesdames et mesdames J'me fous de leurs médailles, venez juste embrasser mes burnes You might also like John Steed Espèce de vieille meuf, t'as senti l'odeur des tunes et des véhicules Ca y est, t'es prête à échanger ton cul Dry Espèce de vieille meuf, ici nos sacs sont remplis de billets Tu veux ton Louis Vuitton? Viens taffer, on va te rhabiller Wira Espèce de vieille meuf, si y'a que les biftons qui t'attirent Arrête de faire des manières et viens nous faire une petite gâterie Mister You Espèce de vieille meuf, j'voulais t'laisser mon numéro Tu m'as dit OK mais si de côté t'a mis au moins 100 000 euros Madame n'est pas une michtonneuse mais elle n'sort pas avec les pauvres Il en faut plein pour être heureuse, elle ouvre son cur devant une clé de coffre Elle est pas là pour ton argent car c'est clair, elle préfère l'or A la recherche de l'espoir, rallume tes phares, il pourrait faire noir Woogataga, j'ai vu et là j'vous raconte ce qu'elles m'ont fait voir Elles m'ont montré que l'avenir rime avec gent-ar donc désespoir Si timide puis si vulgaire, si si, j'vous pousse à l'croire C'est le nerf de la guerre, wallah les meufs c'est que des histoires La vérité c'est peu plaisant, c'est blessant tels des rasoirs La liberté s'cache en prison, si j'guide mon peuple ça s'ra dérisoire On dirait le soir dans ma tête même quand il est 14 heures Une folle m'a dit faut faire la fête, c'est à bronzer que l'équateur sert Dieu est grand, le monde est petit, tu connais tous les coins tah sah Yes, sah el sbah, sans mascara t'as l'air bizarre Une fois à l'hotel bah tu ressort plus avant 13 heures C'est plus Lancôme ton trésor vu que t'as l'cul dans le compresseur Et c'est le désordre dans ta tête et encore t'as que 20 piges T'as une reput' de vraie pute mais bon toi tu t'en fiches Tu veux être riche, shab tu sniffes, tu veux faire partie d'la jet-set Tu mérites qu'un tour d'YZ, espèce de vieille khenzete John Steed Espèce de vieille meuf, t'as senti l'odeur des tunes et des véhicules Ca y est, t'es prête à échanger ton cul Mister You Espèce de vieille meuf, j'voulais t'laisser mon numéro Tu m'as dit OK mais si de côté t'a mis au moins 100 000 euros Wira Espèce de vieille meuf, si y'a que les biftons qui t'attirent Arrête de faire des manières et viens nous faire une petite gâterie Dry Espèce de vieille meuf, ici nos sacs sont remplis de billets Tu veux ton Louis Vuitton? Viens taffer, on va te rhabiller Moi j'kiffe pas les fouffes qui ont une bite dans le veau-cer Une liasse à la place du cur, qui s'frottent devant les gangsters Les Holster de ma garde les font mouiller En soirée, sous vodka, ma clique elles aimeraient souiller Espèce de vieille meuf, tu m'as rodave avec une poupée genre Halle Berry Comme Vanessa, t'as choqué J'ai pare-choqué la rue avec mes rimes et mes crochets Les crasseuses s'accrochent à mon zgeg comme un trophée Elles en ont trop fait, cramées comme les vil-ci Hassoul, par tié-pi, cassez-vous loin d'ici Laissez donc la place à ses dames qui ont la classe Qui déclassent la number one des michtos en place J'vous fracasse a coup de hanches Veux tu ton x dans le merco benz, dans ton benz La puissance du beau negro, après mon passage tu crieras Woogataga Nous ce qu'on aime c'est les boules qui s'font pas hagra, mon gars John Steed Espèce de vieille meuf, t'as senti l'odeur des tunes et des véhicules Ca y est, t'es prête à échanger ton cul Mister You Espèce de vieille meuf, j'voulais t'laisser mon numéro Tu m'as dit OK mais si de côté t'a mis au moins 100 000 euros Wira Espèce de vieille meuf, si y'a que les biftons qui t'attirent Arrête de faire des manières et viens nous faire une petite gâterie Dry Espèce de vieille meuf, ici nos sacs sont remplis de billets Tu veux ton Louis Vuitton? Viens taffer, on va te rhabiller</t>
         </is>
       </c>
     </row>
@@ -4878,12 +4878,12 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Vieux mec</t>
+          <t>Viens pas test</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>COUPLET 1 - MISTER YOU Espèce de vieux mec et jdirai même espèce de vieille merde Tes tombé love dune vieille meuf qui insulte sa belle-mère Qui nest autre que la femme qui ta mis au monde Et vu que tu nes quun bouffon tu laisses passer cette chose immonde Arrête de m3iyane tes fatigué questu connait espèce de 3ayane Ah rkhiss va, sale vieux ceu-mé Tes pas mon pote, tu ma boycott pour mettre un ouk Tes quun pd, tu tfera péter comme un boloss au métro Ourcq WOOGATAGA dahwa tes sérieux ou quoi Tu crois qutu vas mtrahir et ten sortir avec tous tes doigts Chut tait-toi ya les peu-stu sur tous les toits Tu fais ni pipi ni caca mais tu squatte trop les lettes-toi WOOGATABRAAAH Jai du cran moi Si jdemande la main de Carla sa serai juste pour lui mettre une peu-cran Certes, tes ptetre intrigant Mais ta pas le style dun briguant Essé reste quille-tran Le monde est petit car Dieu est grand REFRAIN GOR SAFARA Sa joue les hommes dans la zone De vrais gosses devant les civils .................................. Jamais la pour la daronne A croire qu'il n'a plus de famille Devenue l'esclave d'une vraie bouffonne Répond plus au téléphone Constamment sur messagerie Tous ses potes l'appel Fantôme Tous ces man sans paroles remplis de False story Leurs daronnes sont des vrai cochonne You might also likeCOUPLET 2 - GORSAFARA ..... franchement vasi tiens ta langue Trop de vieux mec trop de vieux type transforme le WOOGATAGANG Boussoul bâtiment tous amateur de gang-bang Real man a Gangsta a osé Paname .... Ta tout dit ta tout fait on font tu n'fais que sucer Le comble des vrais ke-mé il est difficile d'imiter T'es toujours bien sapé le petit reuf a les Shoes trouée Tu balade ta chienne en bolide pendant que la Mif prend le tro-mé On ta vu t'esquivé quand ton pote c'est fait cafouillé T'étonne pas si aujourd'hui les petits de la Tess veulent te dépouillé Des des des Barres A la Baraque c'est toujours la Hess T'explose le moindre billets dans les clubs Ou une paire de fesse Connard c'est tout juste si ta Gadji te tiens pas en laisse Et celle qui ta enfanté n'a pas le droit A la moindre pièce REFRAIN GOR SAFARA Sa joue les hommes dans la zone De vrais gosses devant les civils .................................. Jamais la pour la daronne A croire qu'il n'a plus de famille Devenue l'esclave d'une vraie bouffonne Répond plus au téléphone Constamment sur messagerie Tous ses potes l'appel Fantôme Tous ces man sans paroles remplis de False story Leurs daronnes sont des vrai cochonne COUPLET 3 - MISTER YOU Cest toi qui a le pushka mais cest toi qui ble-trem Tous tes crimes sont passionnelles tes un peu comme Cantat Bertrand Etant petit on sest fait hagar donc cest normal quon tape les grands Nous dehwa cest de lahwa et toi cest dla lette-bran A cause des mecs comme wat les gens boycott ma coupe fashion Chez moi les ptits bicrave du crack ils jouent pas trop à la Playstation Ta rien dcharmant, ta pas dargent en plus tes cheum Moi cque jkifferai voir cest que tous les jeunes de cité jeûnent Car j'me sens comme ses de-mer quand je rompt le carême pour un kamas J'me répète que ses tards-ba ils boycottent leurs mère pour une conasse Hamdoullah j'suis pas comme a-s j'sais que les rents-pa c'est comme la prière Pour eux lève-toi frère même quand t'es trop naze INSTRU All that she wants is another baby All that she wants is another baby WOOGATABRAAAAAH REFRAIN GOR SAFARA Sa joue les hommes dans la zone De vrais gosses devant les civils .................................. Jamais la pour la daronne A croire qu'il n'a plus de famille Devenue l'esclave d'une vraie bouffonne Répond plus au téléphone Constamment sur messagerie Tous ses potes l'appel Fantôme Tous ces man sans paroles remplis de False story Leurs daronnes sont des vrais cochonnes -Salut ma chérie comment tu va ? ta passer une bonne journée -Oh vasi la j'ai pas trop le temps -mais euh euh mais sinon mais mais mais -rend toi utile la va me chercher ma tenue s'il te plait Elle est chez ma copine j'lai oublier j'vais sortir en boite -mais attend 2 petites minutes -Quel 2 minutes la vasi vasi prend le métro la -Nan c'est vraiment parce que c'est toi ma chérie -Ouais Stylie -D'accord j'y vais en courant -Ouais mais ta intérêt</t>
+          <t>AAAAAh attention B.I.L.E.L Mr Yougataga John Steed petrodollar AAAAAAAH, bbrrrrrraaaa Belleville viens surtout pas test l'équipe Le ptit yas Un coup de fil, on débarque on t'baise, on t'liquide Dédicace Belleville viens surtout pas test l'équipe Belleville Un coup de fil, on débarque on t'baise, on t'liquide Zooogatagaaa J'fais mon entrée dans la cabine Un peu comme un boxeur J'volais déjà tout à la cantine On m'a pas élevé chez les bonnes surs Y'a ceux qui volent, ceux qui dealent, ceux qui braquent et les bosseurs Y'a ceux qui sautent, ceux qui tirent, ceux qui parlent et les crosseurs pour protester Tandis que nous on s'amuse Tout ceux qui viendront pour tester Repartiront avec le S.A.M.U T'as le flow de l'abbé Pierre, avec un tout ptit duvet T'as rien à faire dans le RAP comme un black dans un salon d'UV Arrêtes de m'parler de coke On t'a fait sniffer de la craie mec On a cramé ta loc', nous fait pas croire que t'es un mec de grec Aaaah hoooougataga Nous on bicrave sous la grêle Les boloss se grattent les veines quand au quartier on fait la grève Le 34 des rappeurs sucent des bites à crédit Ils veulent pas me faire d'la place par peur de pointer aux ASSEDICS J'sais pas pour qui ils se prennent, mais ils sont pas si terribles Si mon flow avait des mains, il aurait déjà baffé tes rimes You might also likeBelleville viens surtout pas test l'équipe Un coup de fil, on débarque on t'baise, on t'liquide Belleville viens surtout pas test l'équipe Un coup de fil, on débarque on t'baise, on t'liquide Belleville viens surtout pas test l'équipe Un coup de fil, on débarque on t'baise, on t'liquide Belleville viens surtout pas test l'équipe Un coup de fil, on débarque on t'baise, on t'liquide ...</t>
         </is>
       </c>
     </row>
@@ -4895,12 +4895,12 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Vote ou Raï, Part 1</t>
+          <t>Vieux mec</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Jarrive en force men le bléd kima kima Hannibal Rap mta3 les cannibales wléd blédi on est al ! Maghrébin comme Massinissa 7ar kima el harissa Jay men tounés la3ziza souti youssel men ghir viza J'ai la dale n7eb nakel la tour Eiffel Nelbis el gilet par balle trop de cadavre a l'appel Tounés bled chahid yé franca ménech 3abid Rana 7did tounsi dziri maghribi sendid Tnafassna el crimogéne fi 3oudh el oxygéne 3arbi dans les veines 3arbi moslém ménech indigénes Cliqui Cliqui j'aime C'est balti yougataga Tunis gataga ghanni w achta7 nakata nakata Men Tounes el Wahran w men Wahran li Ribat Rap mta3 lebléd débarque Rainb Fever 4 Met le son dans ta gova 5ouya chméta fel kléb Jarrête le rap quand Carla Bruni porte le hijab You might also like2</t>
+          <t>COUPLET 1 - MISTER YOU Espèce de vieux mec et jdirai même espèce de vieille merde Tes tombé love dune vieille meuf qui insulte sa belle-mère Qui nest autre que la femme qui ta mis au monde Et vu que tu nes quun bouffon tu laisses passer cette chose immonde Arrête de m3iyane tes fatigué questu connait espèce de 3ayane Ah rkhiss va, sale vieux ceu-mé Tes pas mon pote, tu ma boycott pour mettre un ouk Tes quun pd, tu tfera péter comme un boloss au métro Ourcq WOOGATAGA dahwa tes sérieux ou quoi Tu crois qutu vas mtrahir et ten sortir avec tous tes doigts Chut tait-toi ya les peu-stu sur tous les toits Tu fais ni pipi ni caca mais tu squatte trop les lettes-toi WOOGATABRAAAH Jai du cran moi Si jdemande la main de Carla sa serai juste pour lui mettre une peu-cran Certes, tes ptetre intrigant Mais ta pas le style dun briguant Essé reste quille-tran Le monde est petit car Dieu est grand REFRAIN GOR SAFARA Sa joue les hommes dans la zone De vrais gosses devant les civils .................................. Jamais la pour la daronne A croire qu'il n'a plus de famille Devenue l'esclave d'une vraie bouffonne Répond plus au téléphone Constamment sur messagerie Tous ses potes l'appel Fantôme Tous ces man sans paroles remplis de False story Leurs daronnes sont des vrai cochonne You might also likeCOUPLET 2 - GORSAFARA ..... franchement vasi tiens ta langue Trop de vieux mec trop de vieux type transforme le WOOGATAGANG Boussoul bâtiment tous amateur de gang-bang Real man a Gangsta a osé Paname .... Ta tout dit ta tout fait on font tu n'fais que sucer Le comble des vrais ke-mé il est difficile d'imiter T'es toujours bien sapé le petit reuf a les Shoes trouée Tu balade ta chienne en bolide pendant que la Mif prend le tro-mé On ta vu t'esquivé quand ton pote c'est fait cafouillé T'étonne pas si aujourd'hui les petits de la Tess veulent te dépouillé Des des des Barres A la Baraque c'est toujours la Hess T'explose le moindre billets dans les clubs Ou une paire de fesse Connard c'est tout juste si ta Gadji te tiens pas en laisse Et celle qui ta enfanté n'a pas le droit A la moindre pièce REFRAIN GOR SAFARA Sa joue les hommes dans la zone De vrais gosses devant les civils .................................. Jamais la pour la daronne A croire qu'il n'a plus de famille Devenue l'esclave d'une vraie bouffonne Répond plus au téléphone Constamment sur messagerie Tous ses potes l'appel Fantôme Tous ces man sans paroles remplis de False story Leurs daronnes sont des vrai cochonne COUPLET 3 - MISTER YOU Cest toi qui a le pushka mais cest toi qui ble-trem Tous tes crimes sont passionnelles tes un peu comme Cantat Bertrand Etant petit on sest fait hagar donc cest normal quon tape les grands Nous dehwa cest de lahwa et toi cest dla lette-bran A cause des mecs comme wat les gens boycott ma coupe fashion Chez moi les ptits bicrave du crack ils jouent pas trop à la Playstation Ta rien dcharmant, ta pas dargent en plus tes cheum Moi cque jkifferai voir cest que tous les jeunes de cité jeûnent Car j'me sens comme ses de-mer quand je rompt le carême pour un kamas J'me répète que ses tards-ba ils boycottent leurs mère pour une conasse Hamdoullah j'suis pas comme a-s j'sais que les rents-pa c'est comme la prière Pour eux lève-toi frère même quand t'es trop naze INSTRU All that she wants is another baby All that she wants is another baby WOOGATABRAAAAAH REFRAIN GOR SAFARA Sa joue les hommes dans la zone De vrais gosses devant les civils .................................. Jamais la pour la daronne A croire qu'il n'a plus de famille Devenue l'esclave d'une vraie bouffonne Répond plus au téléphone Constamment sur messagerie Tous ses potes l'appel Fantôme Tous ces man sans paroles remplis de False story Leurs daronnes sont des vrais cochonnes -Salut ma chérie comment tu va ? ta passer une bonne journée -Oh vasi la j'ai pas trop le temps -mais euh euh mais sinon mais mais mais -rend toi utile la va me chercher ma tenue s'il te plait Elle est chez ma copine j'lai oublier j'vais sortir en boite -mais attend 2 petites minutes -Quel 2 minutes la vasi vasi prend le métro la -Nan c'est vraiment parce que c'est toi ma chérie -Ouais Stylie -D'accord j'y vais en courant -Ouais mais ta intérêt</t>
         </is>
       </c>
     </row>
@@ -4912,12 +4912,12 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Ya ceux</t>
+          <t>Vote ou Raï, Part 1</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Franco c'est plus d'la patience, crois moi qu'j'en perds mon latin Si tu ne veux pas tout baiser quand j'pète mon joint dès l'matin Catin, boloss, j'ai creusé l'écart Minuit sur la terre j'suis vers la lune à minuit et quart Bon bref, RS4, attitude Rolex Big up, cités chaudes, grosse banlieue lyonnaise Younes prend leur la couronne et même le brassard Moi j'aime trop le saint frérot dans ce rap j'pars en croisade Rien que j'coupe des têtes, cheval, GP800 Déter, ouais j'ai trop la dalle j'suis trop puissant J'envoie un chargeur complet sur ton barreau Un costard à Palerme tu m'as vu dans Chaos K-O, pelo, Carlo, Brigante Placard en pleine été car ils t'ont briganté Non faut pas fréquenter, si t'a pas de grosses couilles Bois du sec de Tennessee nan je n'veux pas de Moscou x2 Y'a ceux qui braquent, y'a ceux qui delaent y'a ceux qui braquent ceux qui dealent Y'a ceux qui parlent, y'a ceux qui tirent, y'a ceux qui restent, y'a ceux qui s'tirent Y'a ceux qui crèveraient l'un pour l'autre, y'a ceux qu'on plus rien à s'dire Y'a Christian Dior, y'a Hello Kitty Y'a les graves hauts y'a les petits L'atmosphère est machiavélique, les p'tits charbonnent des vélibs Poto, là, faut que tu t'équipes, c'est plus les bagares en équipe On t'liquide, on est quittes pour nous t'es qu'un faux caïd hein Ils rappent en mode les States, nous en mode Al Quaida Vends d'la cocaïna Dès que tu peux tu va tomber, dès que tu l'veux tu vas mourir Sans qu'tu l'veuilles tu va périr C'étaient les meilleurs maintenant c'est les pires Combien me suceront la bite quand j'aurais bâti mon empire ? J'ai plus rien à leur dire, envers eux rien n'm'attire Poto t'es pas mature, tu va rentrer dans la matrix Ça lâche des rafales de balles, les Zoulous s'coucher tout bas On est pas fiers de faire les mafieux pendant qu'nos mères sont tout pâles C'est pour mes arbi tous-bab, c'est pas des traîtres en tout cas On fais du sale sur tout-terrain, chez nous y'as pas de trucages Ne t'accroches pas si tu lâches, pour moi t'es un fils de lâche Le boule à Nicki Minaj, on lui rentre le pot du T-Max You might also likex2 Qu'est ce qui vous arrive ? J'viens resserrer votre câble Plus rien ne m'effraie je soigne mes plaies avec d'la Vodka Plus rien ne m'adoucit, une balle malgré mon jeu d'jambe Quand j'vois l'état de l'espèce humaine j'ai du respect pour peu d'gens L'rap c'est un bar à timp, moi j'choisis mes victimes Tu va sucer toute la nuit finit les emplois fictifs Nike sa mère le 50, tout ça pour moi c'est pareil Personne ne remplit mon frigo XXX de tonnes et d'barettes C'est pas de l'impro, pour faire du sale j'suis un pro J'fais faire du bruit comme un pot, venu faire des sous comme un gros Oh, j'élimine les faux c'est la voix d'la relève mon ami Ok, Tirgo au micro venu faire du sale j'en suis ravi J'ai égaré mon navire, j'suis un naufragé du 94 J'vais me propager comme d'la frappe Je suis le putain de joker dans le jeu de carte J'arive en mode à la one again Gros joint d'beuh en mode hollande et du shit a la marocaine x21</t>
+          <t>Jarrive en force men le bléd kima kima Hannibal Rap mta3 les cannibales wléd blédi on est al ! Maghrébin comme Massinissa 7ar kima el harissa Jay men tounés la3ziza souti youssel men ghir viza J'ai la dale n7eb nakel la tour Eiffel Nelbis el gilet par balle trop de cadavre a l'appel Tounés bled chahid yé franca ménech 3abid Rana 7did tounsi dziri maghribi sendid Tnafassna el crimogéne fi 3oudh el oxygéne 3arbi dans les veines 3arbi moslém ménech indigénes Cliqui Cliqui j'aime C'est balti yougataga Tunis gataga ghanni w achta7 nakata nakata Men Tounes el Wahran w men Wahran li Ribat Rap mta3 lebléd débarque Rainb Fever 4 Met le son dans ta gova 5ouya chméta fel kléb Jarrête le rap quand Carla Bruni porte le hijab You might also like2</t>
         </is>
       </c>
     </row>
@@ -4929,12 +4929,12 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Youcenzo</t>
+          <t>Ya ceux</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Mister Youcenzo Hmm J'ai fais l'dawa je sais plus, j'crois qu'on a laissé des plumes J'me rappelle juste qu'on a posé en gros J'ai mis d'côté les études, j'ai préféré faire des thunes Pendant qu'ces haineux font qu'jacter dans l'dos, yeah Mamacita, à ton vice on est habitués Oh yeah mamacita, des meufs belles y'en a partout tu sais On est bien, on est plein en bas du bloc à faire du blé, dans mon tieks on est trop Depuis le départ on se bat, on s'emballe pour une étoile sur l'maillot comme Christiano Ronaldo Minuit dans la ville, j'ai pas l'moral à zéro Regarde d'où tu viens, tu ne seras pas déçu gros Fais ça pour la thune, à la base y a pas d'études Prêt à sortir l'projet, j'ai les che-po pleines d'euros J'ai fais l'dawa je sais plus, j'crois qu'on a laissé des plumes J'me rappelle juste qu'on a posé en gros J'ai mis d'côté les études, j'ai préféré faire des thunes Pendant qu'ces haineux font qu'jacter dans l'dos, yeah Mamacita, à ton vice on est habitués Oh yeah mamacita, des meufs belles y'en a partout tu sais You might also like J'ai fais l'dawa je sais plus, j'crois qu'on a laissé des plumes J'me rappelle juste qu'on a posé en gros J'ai mis d'côté les études, j'ai préféré faire des thunes Pendant qu'ces haineux font qu'jacter dans l'dos, yeah Mamacita, à ton vice on est habitués Oh yeah mamacita, des meufs belles y'en a partout tu sais J'ai fais l'dawa je sais plus, j'crois qu'on a laissé des plumes J'me rappelle juste qu'on a posé en gros J'ai mis d'côté les études, j'ai préféré faire des thunes Pendant qu'ces haineux font qu'jacter dans l'dos, yeah Mamacita, à ton vice on est habitués Oh yeah mamacita, des meufs belles y'en a partout tu sais Ouais Erise Yougataga, Lucenzo</t>
+          <t>Franco c'est plus d'la patience, crois moi qu'j'en perds mon latin Si tu ne veux pas tout baiser quand j'pète mon joint dès l'matin Catin, boloss, j'ai creusé l'écart Minuit sur la terre j'suis vers la lune à minuit et quart Bon bref, RS4, attitude Rolex Big up, cités chaudes, grosse banlieue lyonnaise Younes prend leur la couronne et même le brassard Moi j'aime trop le saint frérot dans ce rap j'pars en croisade Rien que j'coupe des têtes, cheval, GP800 Déter, ouais j'ai trop la dalle j'suis trop puissant J'envoie un chargeur complet sur ton barreau Un costard à Palerme tu m'as vu dans Chaos K-O, pelo, Carlo, Brigante Placard en pleine été car ils t'ont briganté Non faut pas fréquenter, si t'a pas de grosses couilles Bois du sec de Tennessee nan je n'veux pas de Moscou x2 Y'a ceux qui braquent, y'a ceux qui delaent y'a ceux qui braquent ceux qui dealent Y'a ceux qui parlent, y'a ceux qui tirent, y'a ceux qui restent, y'a ceux qui s'tirent Y'a ceux qui crèveraient l'un pour l'autre, y'a ceux qu'on plus rien à s'dire Y'a Christian Dior, y'a Hello Kitty Y'a les graves hauts y'a les petits L'atmosphère est machiavélique, les p'tits charbonnent des vélibs Poto, là, faut que tu t'équipes, c'est plus les bagares en équipe On t'liquide, on est quittes pour nous t'es qu'un faux caïd hein Ils rappent en mode les States, nous en mode Al Quaida Vends d'la cocaïna Dès que tu peux tu va tomber, dès que tu l'veux tu vas mourir Sans qu'tu l'veuilles tu va périr C'étaient les meilleurs maintenant c'est les pires Combien me suceront la bite quand j'aurais bâti mon empire ? J'ai plus rien à leur dire, envers eux rien n'm'attire Poto t'es pas mature, tu va rentrer dans la matrix Ça lâche des rafales de balles, les Zoulous s'coucher tout bas On est pas fiers de faire les mafieux pendant qu'nos mères sont tout pâles C'est pour mes arbi tous-bab, c'est pas des traîtres en tout cas On fais du sale sur tout-terrain, chez nous y'as pas de trucages Ne t'accroches pas si tu lâches, pour moi t'es un fils de lâche Le boule à Nicki Minaj, on lui rentre le pot du T-Max You might also likex2 Qu'est ce qui vous arrive ? J'viens resserrer votre câble Plus rien ne m'effraie je soigne mes plaies avec d'la Vodka Plus rien ne m'adoucit, une balle malgré mon jeu d'jambe Quand j'vois l'état de l'espèce humaine j'ai du respect pour peu d'gens L'rap c'est un bar à timp, moi j'choisis mes victimes Tu va sucer toute la nuit finit les emplois fictifs Nike sa mère le 50, tout ça pour moi c'est pareil Personne ne remplit mon frigo XXX de tonnes et d'barettes C'est pas de l'impro, pour faire du sale j'suis un pro J'fais faire du bruit comme un pot, venu faire des sous comme un gros Oh, j'élimine les faux c'est la voix d'la relève mon ami Ok, Tirgo au micro venu faire du sale j'en suis ravi J'ai égaré mon navire, j'suis un naufragé du 94 J'vais me propager comme d'la frappe Je suis le putain de joker dans le jeu de carte J'arive en mode à la one again Gros joint d'beuh en mode hollande et du shit a la marocaine x21</t>
         </is>
       </c>
     </row>
@@ -4946,12 +4946,12 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Yougataflow</t>
+          <t>Youcenzo</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Ouais Ouais Ouais Mister Yougataga sur une instru téh Jay'Z Aie Aie Aie J'veux voir toutes les mains en l'air Tous les Majeurs en l'air Tous les verres en l'air Tous les zdéh en l'air C'est Yougataga l'Commissaire nique sa grand-mère Français j'y comprend rien ni vocabulaire ni grammaire 2010 c'est au cachot que j'ai passé l'été Nique sa mère les raccourcis, et nique sa mère la facilité À quoi bon faire simple quand on peut faire compliqué C'est ou la santé ou l'D5 quand le tier-quar est trop fliqué 2011 quelques millions d'euros à péter, quelques fils de putes à plomber Quitte à engager quelques clandés J'suis venu pour doigté les condés les bâtards qui m'ont boycotté Zoogata, woogataa hein bandes de PD Attendez 2,3 minutes j'me ressers un verre de champagne Suivi d'une coupe et ensuite d'une flûte Ahahah les concurrents téh Paris msèkine Ils sont morts dans le film moi j'suis un gamin là j'suis entrain de gole-ri Vas-y jette ton lacet, quand y'a plus de shit, j'peux plus ricaner J'suis comme Chef Dahmani j'suis dans l'assault et là j'suis prêt à caner Moi, c'est Yougataga zoogataga gangst to gangst Prêt à manger plus de riz qu'un thaï même plus que l'Oncle Ben's J'veux voir toutes les mains en l'air Tous les Majeurs en l'air Tous les verres en l'air Tous les zdéh en l'air C'est Yougataga l'Commissaire nique sa grand-mère Français j'y comprend rien ni vocabulaire ni grammaire ... Que des mathématiques ma gueule ahh Woogataga vous faites quoi dans la vie ? Moi j'fais attention Zoogataga à coups de calibre dans leurs gueules ma gueule Zoogataga Yougataga Woogataga Zoogataga Yougataga Woogataga Zoogataga Yougatagaaaaaaaa 'tention Bébébébébéh quoi aaah woogatagaYou might also like</t>
+          <t>Mister Youcenzo Hmm J'ai fais l'dawa je sais plus, j'crois qu'on a laissé des plumes J'me rappelle juste qu'on a posé en gros J'ai mis d'côté les études, j'ai préféré faire des thunes Pendant qu'ces haineux font qu'jacter dans l'dos, yeah Mamacita, à ton vice on est habitués Oh yeah mamacita, des meufs belles y'en a partout tu sais On est bien, on est plein en bas du bloc à faire du blé, dans mon tieks on est trop Depuis le départ on se bat, on s'emballe pour une étoile sur l'maillot comme Christiano Ronaldo Minuit dans la ville, j'ai pas l'moral à zéro Regarde d'où tu viens, tu ne seras pas déçu gros Fais ça pour la thune, à la base y a pas d'études Prêt à sortir l'projet, j'ai les che-po pleines d'euros J'ai fais l'dawa je sais plus, j'crois qu'on a laissé des plumes J'me rappelle juste qu'on a posé en gros J'ai mis d'côté les études, j'ai préféré faire des thunes Pendant qu'ces haineux font qu'jacter dans l'dos, yeah Mamacita, à ton vice on est habitués Oh yeah mamacita, des meufs belles y'en a partout tu sais You might also like J'ai fais l'dawa je sais plus, j'crois qu'on a laissé des plumes J'me rappelle juste qu'on a posé en gros J'ai mis d'côté les études, j'ai préféré faire des thunes Pendant qu'ces haineux font qu'jacter dans l'dos, yeah Mamacita, à ton vice on est habitués Oh yeah mamacita, des meufs belles y'en a partout tu sais J'ai fais l'dawa je sais plus, j'crois qu'on a laissé des plumes J'me rappelle juste qu'on a posé en gros J'ai mis d'côté les études, j'ai préféré faire des thunes Pendant qu'ces haineux font qu'jacter dans l'dos, yeah Mamacita, à ton vice on est habitués Oh yeah mamacita, des meufs belles y'en a partout tu sais Ouais Erise Yougataga, Lucenzo</t>
         </is>
       </c>
     </row>
@@ -4963,12 +4963,12 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Yougatakayz</t>
+          <t>Yougataflow</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Ouai Ouai Ouai Salut ça va? Comment ça va? Ça va très bien Quoi comment ça se passe? Ça s'passe t'il? Ça s'passe t'il pas? Ougataga, lever les bras Tirgoooo! Ok, c'est ta i-ve poto, fait que-cro les potos Les michtonneuses en vrai mériteraient même pas une photo 94 coco, c'est pas les chiffres du loto Un concert à Bercy sur la scène j'ramène des motos On est au top VIP ramène l'auto, la beuh, le shit, l'alcool Les vips dans nos locaux Mais l'étau se resserre t'es disparu comme Etoo' T'as des gros métaux mais t'es pas un mec du ghetto On est tous en place et t'as pas d'amigos Nous sommes Ancelloti laissez leur José Anigo C'est vrai que j'en rigole poto c'est pas l'même niveau VIP 4 Sose, family Baise les rivaux Baise les rivaux Toute l'année khey j'veux en découdre Pour l'instant on est sur écoute j'avance j'vois plus rien sur ma route You You You Yougatakayz x4 You might also like J'suis en part d'collac, Bouteille d'colaté Hier j'suis au max pour bandit comme Al Grosse dédicace pour DJ Kayz 5 6 Llions-Mi et après j'me casse Ça bicrave la poudre tah Frank 1 2 3 4 putes et après j'me casse Matte mes corones sert à rien qu'tu m'les casse Sahb le Rosay la bicrave et les gazelles 53 94 ça pisse les XXX Investit dans la bière, le crack et l'canabis J'veux voir toutes les mains en l'air, tout le monde sur la piste Les a3ineurs niquez vos mères me faites pas la bise Chez moi c'est la guerre on peux pas faire autrement Fuck ceux qui boycott la Putain d'leur Maman J'vais tous les allumer click click Brah WOOGATABrahh, Levez les bras J'en ai absolument rien a battre de ta i-ve Criminel comme XXX même si Vodka mennivre Jean Pepe, T-Shirt Tah Yves, La serveuse a du mal a calculer l'tarif J'ai la peau dorée, Armand de Brignac, Grosse fête en bois ou dans une grosse baraque Paris Oran New-York, Soir-ce c'est Kech-Marra Pour mes 3arbis, Sonikés, banbarras Big-Up la Street en Vodka comme Jawouara Bête de heflits, Pas d'baveux trois bous-mara J'revide la baraque comme khel, Karim et Barra Comme Oussama j'ai c'qui faut pour débarras Ils sont dans l'embarras, on force les routes barrées Trop d'joints, Hagras, Pour décoller on est parés Big up a Pepe à tous mes XXX</t>
+          <t>Ouais Ouais Ouais Mister Yougataga sur une instru téh Jay'Z Aie Aie Aie J'veux voir toutes les mains en l'air Tous les Majeurs en l'air Tous les verres en l'air Tous les zdéh en l'air C'est Yougataga l'Commissaire nique sa grand-mère Français j'y comprend rien ni vocabulaire ni grammaire 2010 c'est au cachot que j'ai passé l'été Nique sa mère les raccourcis, et nique sa mère la facilité À quoi bon faire simple quand on peut faire compliqué C'est ou la santé ou l'D5 quand le tier-quar est trop fliqué 2011 quelques millions d'euros à péter, quelques fils de putes à plomber Quitte à engager quelques clandés J'suis venu pour doigté les condés les bâtards qui m'ont boycotté Zoogata, woogataa hein bandes de PD Attendez 2,3 minutes j'me ressers un verre de champagne Suivi d'une coupe et ensuite d'une flûte Ahahah les concurrents téh Paris msèkine Ils sont morts dans le film moi j'suis un gamin là j'suis entrain de gole-ri Vas-y jette ton lacet, quand y'a plus de shit, j'peux plus ricaner J'suis comme Chef Dahmani j'suis dans l'assault et là j'suis prêt à caner Moi, c'est Yougataga zoogataga gangst to gangst Prêt à manger plus de riz qu'un thaï même plus que l'Oncle Ben's J'veux voir toutes les mains en l'air Tous les Majeurs en l'air Tous les verres en l'air Tous les zdéh en l'air C'est Yougataga l'Commissaire nique sa grand-mère Français j'y comprend rien ni vocabulaire ni grammaire ... Que des mathématiques ma gueule ahh Woogataga vous faites quoi dans la vie ? Moi j'fais attention Zoogataga à coups de calibre dans leurs gueules ma gueule Zoogataga Yougataga Woogataga Zoogataga Yougataga Woogataga Zoogataga Yougatagaaaaaaaa 'tention Bébébébébéh quoi aaah woogatagaYou might also like</t>
         </is>
       </c>
     </row>
@@ -4980,10 +4980,27 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
+          <t>Yougatakayz</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Ouai Ouai Ouai Salut ça va? Comment ça va? Ça va très bien Quoi comment ça se passe? Ça s'passe t'il? Ça s'passe t'il pas? Ougataga, lever les bras Tirgoooo! Ok, c'est ta i-ve poto, fait que-cro les potos Les michtonneuses en vrai mériteraient même pas une photo 94 coco, c'est pas les chiffres du loto Un concert à Bercy sur la scène j'ramène des motos On est au top VIP ramène l'auto, la beuh, le shit, l'alcool Les vips dans nos locaux Mais l'étau se resserre t'es disparu comme Etoo' T'as des gros métaux mais t'es pas un mec du ghetto On est tous en place et t'as pas d'amigos Nous sommes Ancelloti laissez leur José Anigo C'est vrai que j'en rigole poto c'est pas l'même niveau VIP 4 Sose, family Baise les rivaux Baise les rivaux Toute l'année khey j'veux en découdre Pour l'instant on est sur écoute j'avance j'vois plus rien sur ma route You You You Yougatakayz x4 You might also like J'suis en part d'collac, Bouteille d'colaté Hier j'suis au max pour bandit comme Al Grosse dédicace pour DJ Kayz 5 6 Llions-Mi et après j'me casse Ça bicrave la poudre tah Frank 1 2 3 4 putes et après j'me casse Matte mes corones sert à rien qu'tu m'les casse Sahb le Rosay la bicrave et les gazelles 53 94 ça pisse les XXX Investit dans la bière, le crack et l'canabis J'veux voir toutes les mains en l'air, tout le monde sur la piste Les a3ineurs niquez vos mères me faites pas la bise Chez moi c'est la guerre on peux pas faire autrement Fuck ceux qui boycott la Putain d'leur Maman J'vais tous les allumer click click Brah WOOGATABrahh, Levez les bras J'en ai absolument rien a battre de ta i-ve Criminel comme XXX même si Vodka mennivre Jean Pepe, T-Shirt Tah Yves, La serveuse a du mal a calculer l'tarif J'ai la peau dorée, Armand de Brignac, Grosse fête en bois ou dans une grosse baraque Paris Oran New-York, Soir-ce c'est Kech-Marra Pour mes 3arbis, Sonikés, banbarras Big-Up la Street en Vodka comme Jawouara Bête de heflits, Pas d'baveux trois bous-mara J'revide la baraque comme khel, Karim et Barra Comme Oussama j'ai c'qui faut pour débarras Ils sont dans l'embarras, on force les routes barrées Trop d'joints, Hagras, Pour décoller on est parés Big up a Pepe à tous mes XXX</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Mister You</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
           <t>Zoogatazblex</t>
         </is>
       </c>
-      <c r="C268" t="inlineStr">
+      <c r="C269" t="inlineStr">
         <is>
           <t>J'veux un putain d'ventilo, mais j'ai pas d'lovés sur mon pécule Attends j'te récapitule Ça fait huit jours que j'tourne en rond dans une putain d'cellule Jamais vu d'aussi près l'bitume J'souhaite à personne le placard pendant la canicule Ce putain de soleil, ces putains de grilles aux fenêtres Sur mon lit j'fais bronzette, j'ressemble à une gaufrette J'écris des lettres pour le coiffeur, pour la muscul' La juge sait plus quoi faire pour que j'me sente minuscule Mais bats les yeuks, on s'fait la causette de fenêtre à fenêtre T'es pas content, on t'fait ta fête La recette ? Deux, trois boîtes de thon dans une chaussette Bracos, peu-stu, faux chèques on est tous là pour chose-quelque Même un chien voudrait pas d'la gamelle qu'on mange Mon co' veut rouler son pét' et aussi démouler son cake Donc j'tire le rideau et j'crame une peau d'orange Gros on est bien loin des chiottes de Prison Break Un pigeon m'guette, là derrière les barreaux J'ai des chtars sur l'dos, et ni l'baveux, ni l'dermato' pourront sauver ma peau Wesh surveillant ! La douche, là ! Ça fait une heure que j'ai mis l'drapeau ! Alors je cogne à la porte comme un rat mort Qu'on m'colle un rapport, j'm'en bats les noix d'cajou J'irai au mitard avec le phone à Bazou Prévenez les majeurs, dites au cas où Qué pasa ?, j'entends comme des booms de grenades C'est les colis qui tombent dans la cour de promenade Narvalo, on s'lave au lavabo comme au camping J'ai écrit c'texte sur un bon d'cantine You might also like Mercredi 30 Juin 2010, 21 heures 27 Ça fait près d'une semaine qui font lère-ga aux arrivants Seth Tu demanderas même quand c'est la merde bah moi je m'en bas les coucougnettes Il me reste qu'un zdah alors je le roule sans faire tomber aucune boulette J'appelle Foued pas au phone-télé, nan par la fenêtre, j'ai eu la fouille ministériel J'ai du le planquer, dahwa t'inquiète pas Dans la maine-se je reprends une ce-pu et je me rebranche, nan Il m'en faut 2 ouais, il me faut une puce Bouygues et une puce Orange À cette heure-ci, je me verrais bien en train de me habat dans un ranch Woogataga, un petit verre de Vodka, avec un zeste d'orange J'ai envie de faire du rodéo, une petite lehsa et que des coups de hanches Mais trop souvent on m'a boycotté, je suis rancunier envers beaucoup de ens-g Qu'ils aillent se faire enculer, la roue elle fait pas du sur-place On m'a dit, aides-toi et le ciel t'aidera, dahwa c'est pour ça que je me surpasse Je sais pas ce qui ce passe dans ma tête, je sais ce qui ce passe dans ma cité Les petits, ils ont repris rrain-té donc les grands sont sur-excités Quand la tension devient trop forte, les plombs ils sont obligés de sauter Armé de mes cordes vocales, l'instru' j'étais en train de la ligoter Si t'as pas de parloir soit débrouillard, obliger de traficoter Quand t'es en plein cur de la chose faut juste voir le bon côté Quand on me pose la question, wesh You alors comment vont les zamours ? Je réponds, ils vont bien, ils sont sur la 2, ils s'marrent presque tous les jours Dites à Zemmour qu'il s'étonne pas que je contienne autant de haine en moi J'observe que plus les années passent, plus elles se font rares les peines en moi J'ai envie de faire beaucoup de hébètes, investir dans mon bled Je kifferais rendre à bel Mohamed ce que jadis était à Mohamed La charité faut que je l'ordonne bien donc je la commence par moi même Les faux je leur donne rien si ce n'est un savon quand je suis au hammam J'ai un fusil, je fais pas de K-1, je suis le genre de mec qui vend de la one Dahwa moi je viens pas de l'usine crois moi, là-bas profite à oi-m Bon bah je vais me faire un petit kawa vu que là il est déjà 7 heures du mat' Ensuite faut que je dorme et Inch'Allah dès que je sors, je pète l'audimat2</t>
         </is>

</xml_diff>